<commit_message>
Changed ISA for unsigned branches
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\git\RISCV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklas/riscv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B9A8BB-4BC3-4CB6-85B1-1C36BEF43C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680D165C-88EE-C340-A498-72FDB9A5AA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="194">
   <si>
     <t>R-Type</t>
   </si>
@@ -611,6 +611,15 @@
   </si>
   <si>
     <t>1xx11xx</t>
+  </si>
+  <si>
+    <t>1010 (subu)</t>
+  </si>
+  <si>
+    <t>B-Type (unsigned)</t>
+  </si>
+  <si>
+    <t>subu</t>
   </si>
 </sst>
 </file>
@@ -706,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -731,24 +740,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -13019,7 +13025,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -13335,25 +13341,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC93BE0-3612-4B4B-91A6-E5F017AEE7A8}">
-  <dimension ref="A1:Q126"/>
+  <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.90625" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.36328125" customWidth="1"/>
-    <col min="7" max="7" width="22.90625" customWidth="1"/>
-    <col min="8" max="8" width="1.453125" customWidth="1"/>
-    <col min="16" max="16" width="14.26953125" customWidth="1"/>
-    <col min="17" max="17" width="13.26953125" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" customWidth="1"/>
+    <col min="8" max="8" width="1.5" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -13362,7 +13368,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -13413,7 +13419,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -13458,7 +13464,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -13503,7 +13509,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -13548,7 +13554,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -13593,7 +13599,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -13638,7 +13644,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -13683,7 +13689,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -13728,7 +13734,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -13773,7 +13779,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -13818,7 +13824,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -13863,7 +13869,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H13" s="11"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -13875,11 +13881,11 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -13896,11 +13902,11 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="14"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="6" t="s">
         <v>4</v>
       </c>
@@ -13927,7 +13933,7 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="1"/>
@@ -13970,7 +13976,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="1"/>
@@ -14013,7 +14019,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="1"/>
@@ -14056,7 +14062,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="1"/>
@@ -14099,7 +14105,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="1"/>
@@ -14142,7 +14148,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="1"/>
@@ -14185,7 +14191,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="1"/>
@@ -14228,7 +14234,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="1"/>
@@ -14271,7 +14277,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="1"/>
@@ -14314,7 +14320,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="1"/>
@@ -14357,7 +14363,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="1"/>
@@ -14400,7 +14406,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="1"/>
@@ -14443,7 +14449,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="1"/>
@@ -14486,7 +14492,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="1"/>
@@ -14529,7 +14535,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="1"/>
@@ -14572,7 +14578,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H31" s="11"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -14584,7 +14590,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>50</v>
       </c>
@@ -14599,13 +14605,13 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
       <c r="E33" s="7" t="s">
         <v>6</v>
       </c>
@@ -14626,7 +14632,7 @@
       <c r="P33" s="6"/>
       <c r="Q33" s="6"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -14667,7 +14673,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -14708,7 +14714,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H36" s="11"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -14720,7 +14726,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>53</v>
       </c>
@@ -14741,7 +14747,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>54</v>
       </c>
@@ -14774,7 +14780,7 @@
       <c r="P38" s="6"/>
       <c r="Q38" s="6"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -14817,7 +14823,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -14860,7 +14866,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D41" s="1" t="s">
         <v>23</v>
       </c>
@@ -14899,7 +14905,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H42" s="11"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -14911,7 +14917,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>62</v>
       </c>
@@ -14932,7 +14938,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>63</v>
       </c>
@@ -14965,7 +14971,7 @@
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -15008,7 +15014,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -15051,7 +15057,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -15094,7 +15100,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -15137,7 +15143,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -15171,7 +15177,7 @@
         <v>87</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="P49" s="1" t="s">
         <v>97</v>
@@ -15180,7 +15186,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -15214,7 +15220,7 @@
         <v>87</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="P50" s="1" t="s">
         <v>97</v>
@@ -15223,7 +15229,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="H51" s="11"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
@@ -15235,7 +15241,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>74</v>
       </c>
@@ -15256,13 +15262,13 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A53" s="14" t="s">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
       <c r="E53" s="6" t="s">
         <v>6</v>
       </c>
@@ -15283,7 +15289,7 @@
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -15324,7 +15330,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -15335,7 +15341,7 @@
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>98</v>
       </c>
@@ -15346,24 +15352,24 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
       <c r="E58" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="G58" s="14"/>
+      <c r="G58" s="12"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>22</v>
       </c>
@@ -15380,7 +15386,7 @@
       </c>
       <c r="G59" s="13"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
@@ -15397,7 +15403,7 @@
       </c>
       <c r="G60" s="13"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>23</v>
       </c>
@@ -15414,7 +15420,7 @@
       </c>
       <c r="G61" s="13"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
@@ -15431,7 +15437,7 @@
       </c>
       <c r="G62" s="13"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>26</v>
       </c>
@@ -15448,7 +15454,7 @@
       </c>
       <c r="G63" s="13"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -15457,7 +15463,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -15466,7 +15472,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
         <v>117</v>
       </c>
@@ -15477,22 +15483,22 @@
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
       <c r="E67" s="8" t="s">
         <v>101</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>22</v>
       </c>
@@ -15507,7 +15513,7 @@
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
@@ -15520,7 +15526,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>23</v>
       </c>
@@ -15533,7 +15539,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>27</v>
       </c>
@@ -15546,7 +15552,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>28</v>
       </c>
@@ -15559,21 +15565,21 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>129</v>
       </c>
@@ -15582,7 +15588,7 @@
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>83</v>
       </c>
@@ -15599,7 +15605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>85</v>
       </c>
@@ -15616,7 +15622,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>87</v>
       </c>
@@ -15633,490 +15639,493 @@
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>133</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>135</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E89" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="4" t="s">
-        <v>152</v>
-      </c>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="1" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B98" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" s="1" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A99" s="1" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B100" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A100" s="1" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A101" s="1" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B102" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A103" s="1" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B104" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B104" s="1"/>
+      <c r="B105" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A105" s="1" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A106" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="B106" s="1"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B107" s="1"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B108" s="1"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B109" s="1"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A110" s="1"/>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>168</v>
+      </c>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A112" s="4" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A113" s="6" t="s">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="B113" s="6" t="s">
+      <c r="B114" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C113" s="6" t="s">
+      <c r="C114" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="D113" s="6" t="s">
+      <c r="D114" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E113" s="16" t="s">
+      <c r="E114" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A114" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>87</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>87</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>87</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>87</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>87</v>
       </c>
       <c r="E119" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A120" s="1" t="s">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B121" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A121" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>185</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>97</v>
@@ -16125,49 +16134,77 @@
         <v>185</v>
       </c>
       <c r="D122" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E122" s="1" t="s">
+      <c r="E123" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
     </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
@@ -16182,24 +16219,13 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -16215,7 +16241,7 @@
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16226,11 +16252,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA4E5D8-8AD0-4CFD-9333-C4E2BFF55E5C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added sheet for verification
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklas/riscv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DCDE2E-12AD-A04A-9475-202C8367656E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E7D6B4-A449-1148-B6BB-799AA8D40EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
-    <sheet name="Architecture" sheetId="2" r:id="rId2"/>
-    <sheet name="Control Unit" sheetId="3" r:id="rId3"/>
+    <sheet name="Verification" sheetId="5" r:id="rId2"/>
+    <sheet name="Architecture" sheetId="2" r:id="rId3"/>
+    <sheet name="Control Unit" sheetId="3" r:id="rId4"/>
+    <sheet name="Bitnumbers" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="218">
   <si>
     <t>R-Type</t>
   </si>
@@ -626,13 +628,79 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>wii</t>
+  </si>
+  <si>
+    <t>Checked instructions</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>lh</t>
+  </si>
+  <si>
+    <t>lw</t>
+  </si>
+  <si>
+    <t>lbu</t>
+  </si>
+  <si>
+    <t>lhu</t>
+  </si>
+  <si>
+    <t>addi</t>
+  </si>
+  <si>
+    <t>slli</t>
+  </si>
+  <si>
+    <t>slti</t>
+  </si>
+  <si>
+    <t>sltiu</t>
+  </si>
+  <si>
+    <t>xori</t>
+  </si>
+  <si>
+    <t>srli</t>
+  </si>
+  <si>
+    <t>srai</t>
+  </si>
+  <si>
+    <t>ori</t>
+  </si>
+  <si>
+    <t>andi</t>
+  </si>
+  <si>
+    <t>auipc</t>
+  </si>
+  <si>
+    <t>sb</t>
+  </si>
+  <si>
+    <t>sh</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>lui</t>
+  </si>
+  <si>
+    <t>checked</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -657,6 +725,19 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
@@ -728,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -771,11 +852,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -838,6 +932,55 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>719720</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>81362</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3532BE40-B97A-0745-9B38-DC776E22A9D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3708400" y="609600"/>
+          <a:ext cx="9393820" cy="10406462"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10550,7 +10693,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -13504,8 +13647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC93BE0-3612-4B4B-91A6-E5F017AEE7A8}">
   <dimension ref="A1:Q127"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="G83" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16405,21 +16548,568 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F45CEA-DDAA-4F86-A633-29B993BC7DE7}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F6BEDF-58A8-7846-8BA3-49A7BA2DADCE}">
+  <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="94" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="21" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="21"/>
+    </row>
+    <row r="40" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="21"/>
+    </row>
+    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="21"/>
+    </row>
+    <row r="42" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="21"/>
+    </row>
+    <row r="43" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="21"/>
+    </row>
+    <row r="44" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="21"/>
+    </row>
+    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="21"/>
+    </row>
+    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="21"/>
+    </row>
+    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="21"/>
+    </row>
+    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="21"/>
+    </row>
+    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="21"/>
+    </row>
+    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="21"/>
+    </row>
+    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="21"/>
+    </row>
+    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="21"/>
+    </row>
+    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="21"/>
+    </row>
+    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="21"/>
+    </row>
+    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="21"/>
+    </row>
+    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="21"/>
+    </row>
+    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="21"/>
+    </row>
+    <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="21"/>
+    </row>
+    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="21"/>
+    </row>
+    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="21"/>
+    </row>
+    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="21"/>
+    </row>
+    <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="21"/>
+    </row>
+    <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="21"/>
+    </row>
+    <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="21"/>
+    </row>
+    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="21"/>
+    </row>
+    <row r="66" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="21"/>
+    </row>
+    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="21"/>
+    </row>
+    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="21"/>
+    </row>
+    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="21"/>
+    </row>
+    <row r="70" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="21"/>
+    </row>
+    <row r="71" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="21"/>
+    </row>
+    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="21"/>
+    </row>
+    <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="21"/>
+    </row>
+    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="21"/>
+    </row>
+    <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="21"/>
+    </row>
+    <row r="76" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="21"/>
+    </row>
+    <row r="77" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="21"/>
+    </row>
+    <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A78" s="21"/>
+    </row>
+    <row r="79" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A79" s="21"/>
+    </row>
+    <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A80" s="21"/>
+    </row>
+    <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="21"/>
+    </row>
+    <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="21"/>
+    </row>
+    <row r="83" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="21"/>
+    </row>
+    <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A84" s="21"/>
+    </row>
+    <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A85" s="21"/>
+    </row>
+    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A86" s="21"/>
+    </row>
+    <row r="87" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="21"/>
+    </row>
+    <row r="88" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="21"/>
+    </row>
+    <row r="89" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="21"/>
+    </row>
+    <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="21"/>
+    </row>
+    <row r="91" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A91" s="21"/>
+    </row>
+    <row r="92" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="21"/>
+    </row>
+    <row r="93" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A93" s="21"/>
+    </row>
+    <row r="94" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="21"/>
+    </row>
+    <row r="95" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="21"/>
+    </row>
+    <row r="96" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="21"/>
+    </row>
+    <row r="97" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="21"/>
+    </row>
+    <row r="98" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A98" s="21"/>
+    </row>
+    <row r="99" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="21"/>
+    </row>
+    <row r="100" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="21"/>
+    </row>
+    <row r="101" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="21"/>
+    </row>
+    <row r="102" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A102" s="21"/>
+    </row>
+    <row r="103" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="21"/>
+    </row>
+    <row r="104" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A104" s="21"/>
+    </row>
+    <row r="105" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="21"/>
+    </row>
+    <row r="106" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="21"/>
+    </row>
+    <row r="107" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A107" s="21"/>
+    </row>
+    <row r="108" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A108" s="21"/>
+    </row>
+    <row r="109" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="21"/>
+    </row>
+    <row r="110" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="21"/>
+    </row>
+    <row r="111" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A111" s="21"/>
+    </row>
+    <row r="112" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A112" s="21"/>
+    </row>
+    <row r="113" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A113" s="21"/>
+    </row>
+    <row r="114" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="21"/>
+    </row>
+    <row r="115" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="21"/>
+    </row>
+    <row r="116" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="21"/>
+    </row>
+    <row r="117" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="21"/>
+    </row>
+    <row r="118" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A118" s="21"/>
+    </row>
+    <row r="119" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="21"/>
+    </row>
+    <row r="120" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A120" s="21"/>
+    </row>
+    <row r="121" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="21"/>
+    </row>
+    <row r="122" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="21"/>
+    </row>
+    <row r="123" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="21"/>
+    </row>
+    <row r="124" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" s="21"/>
+    </row>
+    <row r="125" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" s="21"/>
+    </row>
+    <row r="126" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="21"/>
+    </row>
+    <row r="127" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="21"/>
+    </row>
+    <row r="128" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A128" s="21"/>
+    </row>
+    <row r="129" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A129" s="21"/>
+    </row>
+    <row r="130" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A130" s="21"/>
+    </row>
+    <row r="131" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A131" s="21"/>
+    </row>
+    <row r="132" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A132" s="21"/>
+    </row>
+    <row r="133" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A133" s="21"/>
+    </row>
+    <row r="134" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A134" s="21"/>
+    </row>
+    <row r="135" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A135" s="21"/>
+    </row>
+    <row r="136" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A136" s="21"/>
+    </row>
+    <row r="137" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A137" s="21"/>
+    </row>
+    <row r="138" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A138" s="21"/>
+    </row>
+    <row r="139" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A139" s="21"/>
+    </row>
+    <row r="140" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A140" s="21"/>
+    </row>
+    <row r="141" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A141" s="21"/>
+    </row>
+    <row r="142" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A142" s="21"/>
+    </row>
+    <row r="143" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A143" s="21"/>
+    </row>
+    <row r="144" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A144" s="21"/>
+    </row>
+    <row r="145" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A145" s="21"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:B38">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"checked"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F45CEA-DDAA-4F86-A633-29B993BC7DE7}">
+  <dimension ref="S39"/>
+  <sheetViews>
+    <sheetView zoomScale="63" workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="39" spans="19:19" x14ac:dyDescent="0.2">
+      <c r="S39" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA4E5D8-8AD0-4CFD-9333-C4E2BFF55E5C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -16432,4 +17122,359 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC27F950-0B8E-6F4A-BC17-1410D0AF1938}">
+  <dimension ref="A1:AF5"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="32" width="3.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <v>30</v>
+      </c>
+      <c r="C1">
+        <v>29</v>
+      </c>
+      <c r="D1">
+        <v>28</v>
+      </c>
+      <c r="E1">
+        <v>27</v>
+      </c>
+      <c r="F1">
+        <v>26</v>
+      </c>
+      <c r="G1">
+        <v>25</v>
+      </c>
+      <c r="H1">
+        <v>24</v>
+      </c>
+      <c r="I1">
+        <v>23</v>
+      </c>
+      <c r="J1">
+        <v>22</v>
+      </c>
+      <c r="K1">
+        <v>21</v>
+      </c>
+      <c r="L1">
+        <v>20</v>
+      </c>
+      <c r="M1">
+        <v>19</v>
+      </c>
+      <c r="N1">
+        <v>18</v>
+      </c>
+      <c r="O1">
+        <v>17</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>15</v>
+      </c>
+      <c r="R1">
+        <v>14</v>
+      </c>
+      <c r="S1">
+        <v>13</v>
+      </c>
+      <c r="T1">
+        <v>12</v>
+      </c>
+      <c r="U1">
+        <v>11</v>
+      </c>
+      <c r="V1">
+        <v>10</v>
+      </c>
+      <c r="W1">
+        <v>9</v>
+      </c>
+      <c r="X1">
+        <v>8</v>
+      </c>
+      <c r="Y1">
+        <v>7</v>
+      </c>
+      <c r="Z1">
+        <v>6</v>
+      </c>
+      <c r="AA1">
+        <v>5</v>
+      </c>
+      <c r="AB1">
+        <v>4</v>
+      </c>
+      <c r="AC1">
+        <v>3</v>
+      </c>
+      <c r="AD1">
+        <v>2</v>
+      </c>
+      <c r="AE1">
+        <v>1</v>
+      </c>
+      <c r="AF1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>11</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>13</v>
+      </c>
+      <c r="O2">
+        <v>14</v>
+      </c>
+      <c r="P2">
+        <v>15</v>
+      </c>
+      <c r="Q2">
+        <v>16</v>
+      </c>
+      <c r="R2">
+        <v>17</v>
+      </c>
+      <c r="S2">
+        <v>18</v>
+      </c>
+      <c r="T2">
+        <v>19</v>
+      </c>
+      <c r="U2">
+        <v>20</v>
+      </c>
+      <c r="V2">
+        <v>21</v>
+      </c>
+      <c r="W2">
+        <v>22</v>
+      </c>
+      <c r="X2">
+        <v>23</v>
+      </c>
+      <c r="Y2">
+        <v>24</v>
+      </c>
+      <c r="Z2">
+        <v>25</v>
+      </c>
+      <c r="AA2">
+        <v>26</v>
+      </c>
+      <c r="AB2">
+        <v>27</v>
+      </c>
+      <c r="AC2">
+        <v>28</v>
+      </c>
+      <c r="AD2">
+        <v>29</v>
+      </c>
+      <c r="AE2">
+        <v>30</v>
+      </c>
+      <c r="AF2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>3</v>
+      </c>
+      <c r="Y3">
+        <v>4</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <v>6</v>
+      </c>
+      <c r="AB3">
+        <v>7</v>
+      </c>
+      <c r="AC3">
+        <v>8</v>
+      </c>
+      <c r="AD3">
+        <v>9</v>
+      </c>
+      <c r="AE3">
+        <v>10</v>
+      </c>
+      <c r="AF3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4">
+        <v>3</v>
+      </c>
+      <c r="X4">
+        <v>4</v>
+      </c>
+      <c r="Y4">
+        <v>5</v>
+      </c>
+      <c r="Z4">
+        <v>6</v>
+      </c>
+      <c r="AA4">
+        <v>7</v>
+      </c>
+      <c r="AB4">
+        <v>8</v>
+      </c>
+      <c r="AC4">
+        <v>9</v>
+      </c>
+      <c r="AD4">
+        <v>10</v>
+      </c>
+      <c r="AE4">
+        <v>11</v>
+      </c>
+      <c r="AF4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
+      </c>
+      <c r="S5">
+        <v>7</v>
+      </c>
+      <c r="T5">
+        <v>8</v>
+      </c>
+      <c r="U5">
+        <v>9</v>
+      </c>
+      <c r="V5">
+        <v>10</v>
+      </c>
+      <c r="W5">
+        <v>11</v>
+      </c>
+      <c r="X5">
+        <v>12</v>
+      </c>
+      <c r="Y5">
+        <v>13</v>
+      </c>
+      <c r="Z5">
+        <v>14</v>
+      </c>
+      <c r="AA5">
+        <v>15</v>
+      </c>
+      <c r="AB5">
+        <v>16</v>
+      </c>
+      <c r="AC5">
+        <v>17</v>
+      </c>
+      <c r="AD5">
+        <v>18</v>
+      </c>
+      <c r="AE5">
+        <v>19</v>
+      </c>
+      <c r="AF5">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed architecture to enable to write only byte or half to data memory
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklas/riscv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E7D6B4-A449-1148-B6BB-799AA8D40EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD59C56-69B6-E74B-93AC-2E03EA7C018A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="220">
   <si>
     <t>R-Type</t>
   </si>
@@ -694,6 +694,12 @@
   </si>
   <si>
     <t>checked</t>
+  </si>
+  <si>
+    <t>Mem Write</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -809,7 +815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -854,6 +860,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13645,10 +13657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC93BE0-3612-4B4B-91A6-E5F017AEE7A8}">
-  <dimension ref="A1:Q127"/>
+  <dimension ref="A1:Q132"/>
   <sheetViews>
-    <sheetView topLeftCell="G83" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16493,11 +16505,53 @@
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" s="1"/>
+      <c r="A127" s="16" t="s">
+        <v>218</v>
+      </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A128" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B128" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B129" s="23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B130" s="23" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B131" s="23" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B132" s="23" t="s">
+        <v>215</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -16551,7 +16605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F6BEDF-58A8-7846-8BA3-49A7BA2DADCE}">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="125" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -17092,8 +17146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F45CEA-DDAA-4F86-A633-29B993BC7DE7}">
   <dimension ref="S39"/>
   <sheetViews>
-    <sheetView zoomScale="63" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView topLeftCell="E1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update for binary input
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklas/riscv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AC2B4C-06C5-E141-8D98-B68BA52555DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA25984-D3E0-104F-ACE0-27E81A0CB4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="223">
   <si>
     <t>R-Type</t>
   </si>
@@ -706,6 +706,9 @@
   </si>
   <si>
     <t>x1</t>
+  </si>
+  <si>
+    <t>r</t>
   </si>
 </sst>
 </file>
@@ -846,18 +849,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -871,6 +862,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13665,7 +13668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC93BE0-3612-4B4B-91A6-E5F017AEE7A8}">
   <dimension ref="A1:Q132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G87" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A83" zoomScale="139" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
@@ -14204,10 +14207,10 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="14"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -14225,10 +14228,10 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="12"/>
+      <c r="B15" s="22"/>
       <c r="C15" s="6" t="s">
         <v>4</v>
       </c>
@@ -14256,8 +14259,8 @@
       <c r="Q15" s="6"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>22</v>
@@ -14299,8 +14302,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>24</v>
@@ -14342,8 +14345,8 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>23</v>
@@ -14385,8 +14388,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>26</v>
@@ -14428,8 +14431,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
         <v>27</v>
@@ -14471,8 +14474,8 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
@@ -14516,8 +14519,8 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>24</v>
@@ -14559,8 +14562,8 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
         <v>23</v>
@@ -14602,8 +14605,8 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
         <v>25</v>
@@ -14645,8 +14648,8 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
         <v>26</v>
@@ -14688,8 +14691,8 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
         <v>27</v>
@@ -14731,8 +14734,8 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
         <v>27</v>
@@ -14774,8 +14777,8 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
         <v>28</v>
@@ -14817,8 +14820,8 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
         <v>28</v>
@@ -14860,8 +14863,8 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
         <v>22</v>
@@ -14930,12 +14933,12 @@
       <c r="Q32" s="1"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
       <c r="E33" s="7" t="s">
         <v>6</v>
       </c>
@@ -14957,10 +14960,10 @@
       <c r="Q33" s="6"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
         <v>52</v>
@@ -14998,10 +15001,10 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
         <v>31</v>
@@ -15295,177 +15298,177 @@
       <c r="P44" s="6"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16" t="s">
+    <row r="45" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16" t="s">
+      <c r="C45" s="12"/>
+      <c r="D45" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16" t="s">
+      <c r="E45" s="12"/>
+      <c r="F45" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G45" s="16" t="s">
+      <c r="G45" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="17"/>
-      <c r="I45" s="16" t="s">
+      <c r="H45" s="13"/>
+      <c r="I45" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J45" s="16" t="s">
+      <c r="J45" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K45" s="16" t="s">
+      <c r="K45" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="L45" s="16" t="s">
+      <c r="L45" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="M45" s="16" t="s">
+      <c r="M45" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="N45" s="16" t="s">
+      <c r="N45" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="O45" s="16" t="s">
+      <c r="O45" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="P45" s="16" t="s">
+      <c r="P45" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="Q45" s="16" t="s">
+      <c r="Q45" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16" t="s">
+    <row r="46" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16" t="s">
+      <c r="E46" s="12"/>
+      <c r="F46" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G46" s="16" t="s">
+      <c r="G46" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="H46" s="17"/>
-      <c r="I46" s="16" t="s">
+      <c r="H46" s="13"/>
+      <c r="I46" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J46" s="16" t="s">
+      <c r="J46" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K46" s="16" t="s">
+      <c r="K46" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="L46" s="16" t="s">
+      <c r="L46" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="M46" s="16" t="s">
+      <c r="M46" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="N46" s="16" t="s">
+      <c r="N46" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="O46" s="16" t="s">
+      <c r="O46" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="P46" s="16" t="s">
+      <c r="P46" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="Q46" s="16" t="s">
+      <c r="Q46" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16" t="s">
+    <row r="47" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16" t="s">
+      <c r="E47" s="12"/>
+      <c r="F47" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G47" s="16" t="s">
+      <c r="G47" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H47" s="17"/>
-      <c r="I47" s="16" t="s">
+      <c r="H47" s="13"/>
+      <c r="I47" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J47" s="16" t="s">
+      <c r="J47" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K47" s="16" t="s">
+      <c r="K47" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="L47" s="16" t="s">
+      <c r="L47" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="M47" s="16" t="s">
+      <c r="M47" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="N47" s="16" t="s">
+      <c r="N47" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="O47" s="16" t="s">
+      <c r="O47" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="P47" s="16" t="s">
+      <c r="P47" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="Q47" s="16" t="s">
+      <c r="Q47" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="16"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16" t="s">
+    <row r="48" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16" t="s">
+      <c r="E48" s="12"/>
+      <c r="F48" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G48" s="16" t="s">
+      <c r="G48" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="H48" s="17"/>
-      <c r="I48" s="16" t="s">
+      <c r="H48" s="13"/>
+      <c r="I48" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="J48" s="16" t="s">
+      <c r="J48" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K48" s="16" t="s">
+      <c r="K48" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="L48" s="16" t="s">
+      <c r="L48" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="M48" s="16" t="s">
+      <c r="M48" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="N48" s="16" t="s">
+      <c r="N48" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="O48" s="16" t="s">
+      <c r="O48" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="P48" s="16" t="s">
+      <c r="P48" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="Q48" s="16" t="s">
+      <c r="Q48" s="12" t="s">
         <v>91</v>
       </c>
     </row>
@@ -15589,12 +15592,12 @@
       <c r="Q52" s="1"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
       <c r="E53" s="6" t="s">
         <v>6</v>
       </c>
@@ -15615,44 +15618,44 @@
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
     </row>
-    <row r="54" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="16"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16" t="s">
+    <row r="54" spans="1:17" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G54" s="16" t="s">
+      <c r="G54" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="H54" s="19"/>
-      <c r="I54" s="16" t="s">
+      <c r="H54" s="15"/>
+      <c r="I54" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="J54" s="16" t="s">
+      <c r="J54" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K54" s="16" t="s">
+      <c r="K54" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="L54" s="16" t="s">
+      <c r="L54" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="M54" s="16" t="s">
+      <c r="M54" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="N54" s="16" t="s">
+      <c r="N54" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="O54" s="16" t="s">
+      <c r="O54" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="P54" s="16" t="s">
+      <c r="P54" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="Q54" s="16" t="s">
+      <c r="Q54" s="12" t="s">
         <v>92</v>
       </c>
     </row>
@@ -15682,103 +15685,103 @@
       <c r="A58" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
       <c r="E58" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="G58" s="12"/>
+      <c r="G58" s="22"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
       <c r="E59" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F59" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="G59" s="13"/>
+      <c r="G59" s="20"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
       <c r="E60" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F60" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G60" s="13"/>
+      <c r="G60" s="20"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
       <c r="E61" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F61" s="13" t="s">
+      <c r="F61" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="G61" s="13"/>
+      <c r="G61" s="20"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
       <c r="E62" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F62" s="13" t="s">
+      <c r="F62" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="13"/>
+      <c r="G62" s="20"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
       <c r="E63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F63" s="13" t="s">
+      <c r="F63" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="13"/>
+      <c r="G63" s="20"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -15813,11 +15816,11 @@
       <c r="A67" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
       <c r="E67" s="8" t="s">
         <v>101</v>
       </c>
@@ -15828,11 +15831,11 @@
       <c r="A68" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
       <c r="E68" s="1" t="s">
         <v>120</v>
       </c>
@@ -15843,11 +15846,11 @@
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
       <c r="E69" s="1" t="s">
         <v>121</v>
       </c>
@@ -15856,11 +15859,11 @@
       <c r="A70" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B70" s="13" t="s">
+      <c r="B70" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
       <c r="E70" s="1" t="s">
         <v>122</v>
       </c>
@@ -15869,11 +15872,11 @@
       <c r="A71" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
       <c r="E71" s="1" t="s">
         <v>123</v>
       </c>
@@ -15882,11 +15885,11 @@
       <c r="A72" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
       <c r="E72" s="1" t="s">
         <v>128</v>
       </c>
@@ -16138,7 +16141,9 @@
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
+      <c r="C90" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
     </row>
@@ -16511,7 +16516,7 @@
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" s="16" t="s">
+      <c r="A127" s="12" t="s">
         <v>218</v>
       </c>
       <c r="B127" s="1"/>
@@ -16520,65 +16525,54 @@
       <c r="E127" s="1"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A128" s="22" t="s">
+      <c r="A128" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B128" s="22" t="s">
+      <c r="B128" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="23" t="s">
+      <c r="A129" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B129" s="23" t="s">
+      <c r="B129" s="19" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="23" t="s">
+      <c r="A130" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B130" s="23" t="s">
+      <c r="B130" s="19" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="23" t="s">
+      <c r="A131" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B131" s="23" t="s">
+      <c r="B131" s="19" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A132" s="23" t="s">
+      <c r="A132" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B132" s="23" t="s">
+      <c r="B132" s="19" t="s">
         <v>215</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
@@ -16593,13 +16587,24 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B71:D71"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -16611,19 +16616,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F6BEDF-58A8-7846-8BA3-49A7BA2DADCE}">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="17" t="s">
         <v>198</v>
       </c>
       <c r="B2" t="s">
@@ -16631,7 +16636,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="17" t="s">
         <v>199</v>
       </c>
       <c r="B3" t="s">
@@ -16639,7 +16644,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="17" t="s">
         <v>200</v>
       </c>
       <c r="B4" t="s">
@@ -16647,7 +16652,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="17" t="s">
         <v>201</v>
       </c>
       <c r="B5" t="s">
@@ -16655,7 +16660,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="17" t="s">
         <v>202</v>
       </c>
       <c r="B6" t="s">
@@ -16663,7 +16668,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="17" t="s">
         <v>203</v>
       </c>
       <c r="B7" t="s">
@@ -16671,7 +16676,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="17" t="s">
         <v>204</v>
       </c>
       <c r="B8" t="s">
@@ -16679,7 +16684,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="17" t="s">
         <v>205</v>
       </c>
       <c r="B9" t="s">
@@ -16687,7 +16692,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="17" t="s">
         <v>206</v>
       </c>
       <c r="B10" t="s">
@@ -16695,7 +16700,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="17" t="s">
         <v>207</v>
       </c>
       <c r="B11" t="s">
@@ -16703,7 +16708,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="17" t="s">
         <v>208</v>
       </c>
       <c r="B12" t="s">
@@ -16711,7 +16716,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="17" t="s">
         <v>209</v>
       </c>
       <c r="B13" t="s">
@@ -16719,7 +16724,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="17" t="s">
         <v>210</v>
       </c>
       <c r="B14" t="s">
@@ -16727,7 +16732,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="17" t="s">
         <v>211</v>
       </c>
       <c r="B15" t="s">
@@ -16735,7 +16740,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="17" t="s">
         <v>212</v>
       </c>
       <c r="B16" t="s">
@@ -16743,7 +16748,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="17" t="s">
         <v>213</v>
       </c>
       <c r="B17" t="s">
@@ -16751,7 +16756,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="17" t="s">
         <v>214</v>
       </c>
       <c r="B18" t="s">
@@ -16759,7 +16764,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="17" t="s">
         <v>215</v>
       </c>
       <c r="B19" t="s">
@@ -16767,7 +16772,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B20" t="s">
@@ -16775,7 +16780,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="17" t="s">
         <v>133</v>
       </c>
       <c r="B21" t="s">
@@ -16783,7 +16788,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="17" t="s">
         <v>137</v>
       </c>
       <c r="B22" t="s">
@@ -16791,7 +16796,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B23" t="s">
@@ -16799,7 +16804,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="17" t="s">
         <v>138</v>
       </c>
       <c r="B24" t="s">
@@ -16807,7 +16812,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="17" t="s">
         <v>139</v>
       </c>
       <c r="B25" t="s">
@@ -16815,7 +16820,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="17" t="s">
         <v>149</v>
       </c>
       <c r="B26" t="s">
@@ -16823,7 +16828,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="17" t="s">
         <v>151</v>
       </c>
       <c r="B27" t="s">
@@ -16831,7 +16836,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="17" t="s">
         <v>135</v>
       </c>
       <c r="B28" t="s">
@@ -16839,7 +16844,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="17" t="s">
         <v>136</v>
       </c>
       <c r="B29" t="s">
@@ -16847,7 +16852,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="17" t="s">
         <v>216</v>
       </c>
       <c r="B30" t="s">
@@ -16855,7 +16860,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="17" t="s">
         <v>173</v>
       </c>
       <c r="B31" t="s">
@@ -16863,7 +16868,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="17" t="s">
         <v>174</v>
       </c>
       <c r="B32" t="s">
@@ -16871,7 +16876,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="17" t="s">
         <v>175</v>
       </c>
       <c r="B33" t="s">
@@ -16879,7 +16884,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="17" t="s">
         <v>176</v>
       </c>
       <c r="B34" t="s">
@@ -16887,7 +16892,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="17" t="s">
         <v>177</v>
       </c>
       <c r="B35" t="s">
@@ -16895,7 +16900,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="17" t="s">
         <v>178</v>
       </c>
       <c r="B36" t="s">
@@ -16903,335 +16908,341 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="17" t="s">
         <v>179</v>
       </c>
+      <c r="B37" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="17" t="s">
         <v>180</v>
       </c>
+      <c r="B38" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
+      <c r="A39" s="17"/>
     </row>
     <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="21"/>
+      <c r="A40" s="17"/>
     </row>
     <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="21"/>
+      <c r="A41" s="17"/>
     </row>
     <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
+      <c r="A42" s="17"/>
     </row>
     <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A43" s="21"/>
+      <c r="A43" s="17"/>
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
+      <c r="A44" s="17"/>
     </row>
     <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
+      <c r="A45" s="17"/>
     </row>
     <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
+      <c r="A46" s="17"/>
     </row>
     <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A47" s="21"/>
+      <c r="A47" s="17"/>
     </row>
     <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A48" s="21"/>
+      <c r="A48" s="17"/>
     </row>
     <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="21"/>
+      <c r="A49" s="17"/>
     </row>
     <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="21"/>
+      <c r="A50" s="17"/>
     </row>
     <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="21"/>
+      <c r="A51" s="17"/>
     </row>
     <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
+      <c r="A52" s="17"/>
     </row>
     <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
+      <c r="A53" s="17"/>
     </row>
     <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="21"/>
+      <c r="A54" s="17"/>
     </row>
     <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="21"/>
+      <c r="A55" s="17"/>
     </row>
     <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="21"/>
+      <c r="A56" s="17"/>
     </row>
     <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="21"/>
+      <c r="A57" s="17"/>
     </row>
     <row r="58" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="21"/>
+      <c r="A58" s="17"/>
     </row>
     <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="21"/>
+      <c r="A59" s="17"/>
     </row>
     <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="21"/>
+      <c r="A60" s="17"/>
     </row>
     <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="21"/>
+      <c r="A61" s="17"/>
     </row>
     <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="21"/>
+      <c r="A62" s="17"/>
     </row>
     <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="21"/>
+      <c r="A63" s="17"/>
     </row>
     <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="21"/>
+      <c r="A64" s="17"/>
     </row>
     <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="21"/>
+      <c r="A65" s="17"/>
     </row>
     <row r="66" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="21"/>
+      <c r="A66" s="17"/>
     </row>
     <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="21"/>
+      <c r="A67" s="17"/>
     </row>
     <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="21"/>
+      <c r="A68" s="17"/>
     </row>
     <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="21"/>
+      <c r="A69" s="17"/>
     </row>
     <row r="70" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="21"/>
+      <c r="A70" s="17"/>
     </row>
     <row r="71" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="21"/>
+      <c r="A71" s="17"/>
     </row>
     <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="21"/>
+      <c r="A72" s="17"/>
     </row>
     <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="21"/>
+      <c r="A73" s="17"/>
     </row>
     <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="21"/>
+      <c r="A74" s="17"/>
     </row>
     <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="21"/>
+      <c r="A75" s="17"/>
     </row>
     <row r="76" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="21"/>
+      <c r="A76" s="17"/>
     </row>
     <row r="77" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="21"/>
+      <c r="A77" s="17"/>
     </row>
     <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="21"/>
+      <c r="A78" s="17"/>
     </row>
     <row r="79" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="21"/>
+      <c r="A79" s="17"/>
     </row>
     <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="21"/>
+      <c r="A80" s="17"/>
     </row>
     <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A81" s="21"/>
+      <c r="A81" s="17"/>
     </row>
     <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A82" s="21"/>
+      <c r="A82" s="17"/>
     </row>
     <row r="83" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A83" s="21"/>
+      <c r="A83" s="17"/>
     </row>
     <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A84" s="21"/>
+      <c r="A84" s="17"/>
     </row>
     <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A85" s="21"/>
+      <c r="A85" s="17"/>
     </row>
     <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="21"/>
+      <c r="A86" s="17"/>
     </row>
     <row r="87" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87" s="21"/>
+      <c r="A87" s="17"/>
     </row>
     <row r="88" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88" s="21"/>
+      <c r="A88" s="17"/>
     </row>
     <row r="89" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89" s="21"/>
+      <c r="A89" s="17"/>
     </row>
     <row r="90" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A90" s="21"/>
+      <c r="A90" s="17"/>
     </row>
     <row r="91" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91" s="21"/>
+      <c r="A91" s="17"/>
     </row>
     <row r="92" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A92" s="21"/>
+      <c r="A92" s="17"/>
     </row>
     <row r="93" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93" s="21"/>
+      <c r="A93" s="17"/>
     </row>
     <row r="94" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94" s="21"/>
+      <c r="A94" s="17"/>
     </row>
     <row r="95" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95" s="21"/>
+      <c r="A95" s="17"/>
     </row>
     <row r="96" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A96" s="21"/>
+      <c r="A96" s="17"/>
     </row>
     <row r="97" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A97" s="21"/>
+      <c r="A97" s="17"/>
     </row>
     <row r="98" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="21"/>
+      <c r="A98" s="17"/>
     </row>
     <row r="99" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A99" s="21"/>
+      <c r="A99" s="17"/>
     </row>
     <row r="100" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100" s="21"/>
+      <c r="A100" s="17"/>
     </row>
     <row r="101" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A101" s="21"/>
+      <c r="A101" s="17"/>
     </row>
     <row r="102" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A102" s="21"/>
+      <c r="A102" s="17"/>
     </row>
     <row r="103" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A103" s="21"/>
+      <c r="A103" s="17"/>
     </row>
     <row r="104" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A104" s="21"/>
+      <c r="A104" s="17"/>
     </row>
     <row r="105" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" s="21"/>
+      <c r="A105" s="17"/>
     </row>
     <row r="106" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="21"/>
+      <c r="A106" s="17"/>
     </row>
     <row r="107" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A107" s="21"/>
+      <c r="A107" s="17"/>
     </row>
     <row r="108" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A108" s="21"/>
+      <c r="A108" s="17"/>
     </row>
     <row r="109" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A109" s="21"/>
+      <c r="A109" s="17"/>
     </row>
     <row r="110" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A110" s="21"/>
+      <c r="A110" s="17"/>
     </row>
     <row r="111" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A111" s="21"/>
+      <c r="A111" s="17"/>
     </row>
     <row r="112" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A112" s="21"/>
+      <c r="A112" s="17"/>
     </row>
     <row r="113" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A113" s="21"/>
+      <c r="A113" s="17"/>
     </row>
     <row r="114" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A114" s="21"/>
+      <c r="A114" s="17"/>
     </row>
     <row r="115" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="21"/>
+      <c r="A115" s="17"/>
     </row>
     <row r="116" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="21"/>
+      <c r="A116" s="17"/>
     </row>
     <row r="117" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="21"/>
+      <c r="A117" s="17"/>
     </row>
     <row r="118" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="21"/>
+      <c r="A118" s="17"/>
     </row>
     <row r="119" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="21"/>
+      <c r="A119" s="17"/>
     </row>
     <row r="120" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="21"/>
+      <c r="A120" s="17"/>
     </row>
     <row r="121" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="21"/>
+      <c r="A121" s="17"/>
     </row>
     <row r="122" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="21"/>
+      <c r="A122" s="17"/>
     </row>
     <row r="123" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="21"/>
+      <c r="A123" s="17"/>
     </row>
     <row r="124" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="21"/>
+      <c r="A124" s="17"/>
     </row>
     <row r="125" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="21"/>
+      <c r="A125" s="17"/>
     </row>
     <row r="126" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A126" s="21"/>
+      <c r="A126" s="17"/>
     </row>
     <row r="127" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A127" s="21"/>
+      <c r="A127" s="17"/>
     </row>
     <row r="128" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A128" s="21"/>
+      <c r="A128" s="17"/>
     </row>
     <row r="129" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A129" s="21"/>
+      <c r="A129" s="17"/>
     </row>
     <row r="130" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A130" s="21"/>
+      <c r="A130" s="17"/>
     </row>
     <row r="131" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A131" s="21"/>
+      <c r="A131" s="17"/>
     </row>
     <row r="132" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A132" s="21"/>
+      <c r="A132" s="17"/>
     </row>
     <row r="133" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A133" s="21"/>
+      <c r="A133" s="17"/>
     </row>
     <row r="134" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A134" s="21"/>
+      <c r="A134" s="17"/>
     </row>
     <row r="135" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A135" s="21"/>
+      <c r="A135" s="17"/>
     </row>
     <row r="136" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A136" s="21"/>
+      <c r="A136" s="17"/>
     </row>
     <row r="137" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A137" s="21"/>
+      <c r="A137" s="17"/>
     </row>
     <row r="138" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A138" s="21"/>
+      <c r="A138" s="17"/>
     </row>
     <row r="139" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A139" s="21"/>
+      <c r="A139" s="17"/>
     </row>
     <row r="140" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A140" s="21"/>
+      <c r="A140" s="17"/>
     </row>
     <row r="141" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A141" s="21"/>
+      <c r="A141" s="17"/>
     </row>
     <row r="142" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A142" s="21"/>
+      <c r="A142" s="17"/>
     </row>
     <row r="143" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" s="21"/>
+      <c r="A143" s="17"/>
     </row>
     <row r="144" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A144" s="21"/>
+      <c r="A144" s="17"/>
     </row>
     <row r="145" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A145" s="21"/>
+      <c r="A145" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:B38">
@@ -17248,7 +17259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F45CEA-DDAA-4F86-A633-29B993BC7DE7}">
   <dimension ref="S39"/>
   <sheetViews>
-    <sheetView topLeftCell="G18" zoomScale="82" workbookViewId="0">
+    <sheetView zoomScale="56" workbookViewId="0">
       <selection activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Started to add C extension
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklas/riscv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA25984-D3E0-104F-ACE0-27E81A0CB4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA009BC-0F8A-C747-A3FC-9DA3D6AF3BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="740" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
   </bookViews>
   <sheets>
     <sheet name="ISA" sheetId="1" r:id="rId1"/>
     <sheet name="Verification" sheetId="5" r:id="rId2"/>
     <sheet name="Architecture" sheetId="2" r:id="rId3"/>
-    <sheet name="Control Unit" sheetId="3" r:id="rId4"/>
-    <sheet name="Bitnumbers" sheetId="4" r:id="rId5"/>
+    <sheet name="Compressed ISA" sheetId="6" r:id="rId4"/>
+    <sheet name="Control Unit" sheetId="3" r:id="rId5"/>
+    <sheet name="Bitnumbers" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="280">
   <si>
     <t>R-Type</t>
   </si>
@@ -709,6 +710,177 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compressed </t>
+  </si>
+  <si>
+    <t>Expanded</t>
+  </si>
+  <si>
+    <t>C.LWSP</t>
+  </si>
+  <si>
+    <t>C.SWSP</t>
+  </si>
+  <si>
+    <t>lw rd, offset(x2)</t>
+  </si>
+  <si>
+    <t>sw rs2, offset(x2)</t>
+  </si>
+  <si>
+    <t>C.LW</t>
+  </si>
+  <si>
+    <t>lw rd, offset(rs1)</t>
+  </si>
+  <si>
+    <t>C.SW</t>
+  </si>
+  <si>
+    <t>sw rs2, offset(rs1)</t>
+  </si>
+  <si>
+    <t>C.J</t>
+  </si>
+  <si>
+    <t>jal x0, offset</t>
+  </si>
+  <si>
+    <t>C.JAL</t>
+  </si>
+  <si>
+    <t>jal x1, offset</t>
+  </si>
+  <si>
+    <t>C.JR</t>
+  </si>
+  <si>
+    <t>jalr x0, 0(rs1)</t>
+  </si>
+  <si>
+    <t>C.JALR</t>
+  </si>
+  <si>
+    <t>jalr x1, 0(rs1)</t>
+  </si>
+  <si>
+    <t>Notice</t>
+  </si>
+  <si>
+    <t>(pc+2)</t>
+  </si>
+  <si>
+    <t>C.BEQZ</t>
+  </si>
+  <si>
+    <t>beq rs1, x0, offset</t>
+  </si>
+  <si>
+    <t>C.BNEZ</t>
+  </si>
+  <si>
+    <t>bne rs1, x0, offset</t>
+  </si>
+  <si>
+    <t>C.LI</t>
+  </si>
+  <si>
+    <t>addi rd, x0, imm</t>
+  </si>
+  <si>
+    <t>C.LUI</t>
+  </si>
+  <si>
+    <t>lui rd, imm</t>
+  </si>
+  <si>
+    <t>C.ADDI</t>
+  </si>
+  <si>
+    <t>addi rd, rd, imm</t>
+  </si>
+  <si>
+    <t>C.ADDI16SP</t>
+  </si>
+  <si>
+    <t>addi x2, x2, nzimm[9:4]</t>
+  </si>
+  <si>
+    <t>C.ADDI4SPN</t>
+  </si>
+  <si>
+    <t>addi rd, x2, nzuimm[9:2]</t>
+  </si>
+  <si>
+    <t>C.SLLI</t>
+  </si>
+  <si>
+    <t>slli rd, rd, shamt[5:0]</t>
+  </si>
+  <si>
+    <t>shamt[5] must be zero</t>
+  </si>
+  <si>
+    <t>C.SRLI</t>
+  </si>
+  <si>
+    <t>srli rd, rd, shamt</t>
+  </si>
+  <si>
+    <t>C.SRAI</t>
+  </si>
+  <si>
+    <t>srai rd, rd, shamt</t>
+  </si>
+  <si>
+    <t>C.ANDI</t>
+  </si>
+  <si>
+    <t>andi rd, rd, imm</t>
+  </si>
+  <si>
+    <t>C.MV</t>
+  </si>
+  <si>
+    <t>add rd, x0, rs2</t>
+  </si>
+  <si>
+    <t>C.ADD</t>
+  </si>
+  <si>
+    <t>add rd, rd, rs2</t>
+  </si>
+  <si>
+    <t>C.AND</t>
+  </si>
+  <si>
+    <t>and rd, rd, rs2</t>
+  </si>
+  <si>
+    <t>C.OR</t>
+  </si>
+  <si>
+    <t>or rd, rd, rs2</t>
+  </si>
+  <si>
+    <t>C.XOR</t>
+  </si>
+  <si>
+    <t>xor rd, rd, rs2</t>
+  </si>
+  <si>
+    <t>C.SUB</t>
+  </si>
+  <si>
+    <t>sub rd, rd, rs2</t>
+  </si>
+  <si>
+    <t>C.NOP</t>
+  </si>
+  <si>
+    <t>add x0, x0, x0</t>
   </si>
 </sst>
 </file>
@@ -863,16 +1035,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -10716,6 +10888,1471 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152039</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD4058CC-F0CC-1D1B-545A-79A4EDE34BB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9017000" y="800100"/>
+          <a:ext cx="7772400" cy="3542939"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7702555-E762-985F-CC76-4DD7EB375B4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9131300" y="4483100"/>
+          <a:ext cx="7277100" cy="1778000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DB34207-5A29-FAEC-D467-DF562C5B62A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1752600" y="7010400"/>
+          <a:ext cx="7848600" cy="4385733"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>804333</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>67734</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>270933</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>106033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A6F3D7C-C4A2-FACD-A2C6-0CBBBDE074F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10837333" y="7179734"/>
+          <a:ext cx="7848600" cy="6947099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>414866</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A29A6E92-D9D9-1736-1B0A-FF50E4F9501F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19668066" y="7366000"/>
+          <a:ext cx="7395634" cy="4775200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152751</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>188043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>528231</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>13455</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DB0130F-E109-02A7-A806-BBE50DBCA543}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7636680" y="7853400"/>
+            <a:ext cx="375480" cy="21960"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DB0130F-E109-02A7-A806-BBE50DBCA543}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7619040" y="7835400"/>
+              <a:ext cx="411120" cy="57600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>158151</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>28252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>782391</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>81532</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CDB1A54-9906-5282-C631-03B74739C1D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7642080" y="8479800"/>
+            <a:ext cx="624240" cy="53280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CDB1A54-9906-5282-C631-03B74739C1D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7624080" y="8462160"/>
+              <a:ext cx="659880" cy="88920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>139791</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>16037</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>752511</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>47357</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53873DC1-2145-FD1B-E9ED-B049846D9D5C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7623720" y="8860680"/>
+            <a:ext cx="612720" cy="31320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53873DC1-2145-FD1B-E9ED-B049846D9D5C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7606080" y="8843040"/>
+              <a:ext cx="648360" cy="66960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>145551</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>72594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>718311</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>106434</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{909D4868-9E60-5073-43BB-0B33F1498638}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7629480" y="9506880"/>
+            <a:ext cx="572760" cy="33840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{909D4868-9E60-5073-43BB-0B33F1498638}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7611480" y="9489069"/>
+              <a:ext cx="608400" cy="69105"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>602024</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>156499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>675831</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>179216</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="18" name="Ink 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A154B8EA-5E1C-E10B-42E6-CD4FD7EB2776}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2250000" y="9983880"/>
+            <a:ext cx="5909760" cy="612360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="18" name="Ink 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A154B8EA-5E1C-E10B-42E6-CD4FD7EB2776}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2231838" y="9965784"/>
+              <a:ext cx="5945720" cy="648190"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>796784</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>15714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>653459</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>125514</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="19" name="Ink 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F639315B-A5F8-7F98-3355-0D791F6D9814}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2444760" y="9450000"/>
+            <a:ext cx="4861080" cy="109800"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="19" name="Ink 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F639315B-A5F8-7F98-3355-0D791F6D9814}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2426968" y="9432360"/>
+              <a:ext cx="4897026" cy="145440"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590504</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>130480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>42231</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>131237</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="22" name="Ink 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4809950E-9751-DFB1-5ADC-3AE096ABAB6E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2238480" y="8385480"/>
+            <a:ext cx="5287680" cy="590400"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="22" name="Ink 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4809950E-9751-DFB1-5ADC-3AE096ABAB6E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2220663" y="8367743"/>
+              <a:ext cx="5323678" cy="626237"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>663224</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>86163</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>281631</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>28935</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="23" name="Ink 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6E4D68C-7CBD-FED3-6E1B-082DB74364B1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2311200" y="7751520"/>
+            <a:ext cx="5454360" cy="139320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="23" name="Ink 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6E4D68C-7CBD-FED3-6E1B-082DB74364B1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2293388" y="7733742"/>
+              <a:ext cx="5490347" cy="175238"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>322047</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>70454</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>265192</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>130934</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8E768F4-98E7-1BBA-6C69-AF92543425D0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11105640" y="10907280"/>
+            <a:ext cx="5745600" cy="60480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8E768F4-98E7-1BBA-6C69-AF92543425D0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11087820" y="10889640"/>
+              <a:ext cx="5781603" cy="96120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520767</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>28614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>403950</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>132294</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="25" name="Ink 24">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5E502B1-0D41-5194-5D74-F2A36191A68A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11304360" y="11245680"/>
+            <a:ext cx="6514560" cy="103680"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="25" name="Ink 24">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5E502B1-0D41-5194-5D74-F2A36191A68A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11286175" y="11228040"/>
+              <a:ext cx="6550566" cy="139320"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>243592</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>67574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>614190</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>160454</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="26" name="Ink 25">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA6F674-B18B-865E-740A-A9AD218CC497}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="16829640" y="10904400"/>
+            <a:ext cx="1199520" cy="92880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="26" name="Ink 25">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CA6F674-B18B-865E-740A-A9AD218CC497}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16812000" y="10886400"/>
+              <a:ext cx="1235160" cy="128520"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>657706</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>100009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>590051</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>92769</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="27" name="Ink 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DDC6350-DA1D-949F-1D37-AD26FFC262EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="19730520" y="7324560"/>
+            <a:ext cx="5734800" cy="182880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="27" name="Ink 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DDC6350-DA1D-949F-1D37-AD26FFC262EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19712700" y="7307076"/>
+              <a:ext cx="5770804" cy="217498"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>10583</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>79730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>501648</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>33970</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="28" name="Ink 27">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D16FF56-F2F9-0ED4-CAED-CB325DE59E8F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="19912320" y="7874640"/>
+            <a:ext cx="6293520" cy="144360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="28" name="Ink 27">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D16FF56-F2F9-0ED4-CAED-CB325DE59E8F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19894153" y="7857289"/>
+              <a:ext cx="6329491" cy="178715"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>795251</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171289</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>454488</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>14289</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="29" name="Ink 28">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97EB6ED1-78E5-BB98-C60A-B5A0CC597F84}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="25670520" y="7395840"/>
+            <a:ext cx="488160" cy="33120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="29" name="Ink 28">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97EB6ED1-78E5-BB98-C60A-B5A0CC597F84}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="25652520" y="7377840"/>
+              <a:ext cx="523800" cy="68760"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>161063</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>180130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>416688</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>104130</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="30" name="Ink 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFC027CB-C0C7-AC3F-1F6C-8B13A0470FAC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="20062800" y="8165160"/>
+            <a:ext cx="6058080" cy="114120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="30" name="Ink 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFC027CB-C0C7-AC3F-1F6C-8B13A0470FAC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="20044990" y="8148317"/>
+              <a:ext cx="6094064" cy="148150"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>200663</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>2811</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>527208</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>30851</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="31" name="Ink 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24532649-36CF-D97A-9D7A-8463F1C3FED5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="20102400" y="8938440"/>
+            <a:ext cx="6129000" cy="218160"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="31" name="Ink 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24532649-36CF-D97A-9D7A-8463F1C3FED5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="20084228" y="8921226"/>
+              <a:ext cx="6164980" cy="252939"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>202463</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>136572</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>379608</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>59132</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId38">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="32" name="Ink 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0C598DB-55E9-E8E2-5A4A-411F41DDEA49}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="20104200" y="9832680"/>
+            <a:ext cx="5979600" cy="112680"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="32" name="Ink 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0C598DB-55E9-E8E2-5A4A-411F41DDEA49}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="20086387" y="9815503"/>
+              <a:ext cx="6015589" cy="146690"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>113543</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>97933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>658968</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>21213</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId40">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="33" name="Ink 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E92CBB0F-739B-F36E-6347-C879606C392E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="20015280" y="10364400"/>
+            <a:ext cx="6347880" cy="113400"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="33" name="Ink 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E92CBB0F-739B-F36E-6347-C879606C392E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19997477" y="10347562"/>
+              <a:ext cx="6383848" cy="147420"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>9503</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>91773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>428208</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>116174</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId42">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="34" name="Ink 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3B4B2D5-5EF8-1D21-F80C-EBB583AFB454}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="19911240" y="10548360"/>
+            <a:ext cx="6221160" cy="404640"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="34" name="Ink 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3B4B2D5-5EF8-1D21-F80C-EBB583AFB454}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19893071" y="10530828"/>
+              <a:ext cx="6257135" cy="439353"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
@@ -13347,6 +14984,524 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:17:25.376"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24575,'1'7'0,"3"-1"0,13-6 0,7 0 0,4 0 0,0 0 0,-1 0 0,-1 0 0,-2 0 0,4 0 0,-4 0 0,-3 0 0,-1 0 0,-2 0 0,-1 0 0,4 3 0,1 2 0,0-1 0,2 1 0,-3-1 0,-1 0 0,-3 0 0,-4-2 0,-1-2 0,-2 3 0,5 1 0,4 1 0,3-2 0,0-2 0,0-1 0,-1 0 0,1 0 0,1 0 0,-2 0 0,2 0 0,-5 0 0,3 0 0,-1 0 0,-1 0 0,-2 0 0,-3 0 0,2 0 0,-1 0 0,0 0 0,-1 0 0,-3 0 0,1 0 0,1 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,-2 0 0,2 0 0,-2 0 0,1 0 0,0 0 0,0 0 0,-5 0 0,-2 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink10.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:18:44.825"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 24575,'27'0'0,"37"0"0,-9 0 0,7 0 0,22 0 0,6 0 0,-24 0 0,0 0 0,1 0 0,1 0 0,-1 0 0,0 0 0,30 0 0,-1 0 0,-7 0 0,0 0 0,2 0 0,0 0 0,4 0 0,1 0-400,-23 0 1,1 0 0,1 0 399,6 0 0,2 0 0,3 0 0,-14 0 0,2 0 0,2 0 0,1 0-445,5 0 1,1 0-1,2 0 1,1 0 444,9 1 0,2 1 0,1-1 0,4 2-672,-10-1 0,2 1 0,2 0 0,2 1 0,2-1 672,-7 0 0,1 0 0,3 0 0,0 0 0,2-1 0,1 1-523,-6-1 1,1 1 0,2-1 0,1 1 0,0-1 0,1 0 0,1 0 522,-8-1 0,1 0 0,0 0 0,1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,2-1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-2 0 0,-1 0 0,7 0 0,-2 0 0,0 0 0,-1 0 0,0 0 0,-1 0 0,0 0-234,-3 0 1,-1 0-1,0 0 1,0 0-1,-2 0 1,0 0-1,-1 0 234,6 0 0,-1 0 0,-1 0 0,-2 0 0,0 0 0,-1 0-33,9 0 0,-2 0 0,-1 0 0,-1 0 0,-2 0 33,-7 0 0,-1-1 0,-2 1 0,-2 0 0,-3 1 598,25-1 0,-5 2 0,-5 0-598,-18 0 0,-4 0 0,-5 2 1826,2 1 0,-6 1-1826,32 11 3384,-22-1-3384,6 2 1222,-29-7 1,5 1-1223,14 0 0,6-1 0,17 2 0,5-1-92,-25-5 1,3 0 0,0-1 91,6 0 0,0-1 0,0 0 0,-1 0 0,-1-1 0,-1-1 0,-3 0 0,-1 0 0,-2 0-40,-4 0 0,-2 1 1,-1-1 39,26 0 0,-3-1 0,-8 1 0,-1-1 0,-8 0 0,-2-1 0,-3-1 0,0 0 0,-1 0 0,1 0 392,5 0 1,3 0-393,7 0 0,2 0 0,3 0 0,-1 0 62,-1 0 0,-2 0-62,-5-3 0,-1-1 0,-4-1 0,1-2 0,8-2 0,4-2 0,7-1 0,4 0-284,-23 4 1,2 0 0,1 1 283,5-1 0,2 0 0,-1 1 0,-3-1 0,-1 1 0,-1 1-16,-5 0 1,-2 1 0,-2 1 15,19-3 0,-6 1 0,-17 2 0,-4 1 0,30-2 0,-23 2 0,-18 3 847,5 0-847,6 0 49,16 0-49,17 0 0,-37 2 0,3 0 0,7 0 0,3 1 0,4-1 0,2 0 0,1 0 0,0 0 0,-5-2 0,-2 0 0,-1 0 0,0 0 0,-2 0 0,-1 0 0,-2 0 0,-1 0 0,-3 0 0,-2 0 0,40 0 0,-14 0 0,-9 0 0,7 0 0,3 0 0,-4 0 0,-2 0 0,-9 0 0,3 0 0,9 0 0,8 0 0,-4 0 0,-13 0 0,-14 0 0,-12 0 0,-5 0 0,-3 0 0,-7 0 0,-4 0 0,-1-2 0,2-2 0,-1 1 0,-3 1 0,-5 1 0,-4 1 0,-4 0 0,-5 0 0,-2 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:18:47.739"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 18 24575,'89'0'0,"-35"-2"0,3 0 0,9 0 0,3-1 0,9 1 0,2-1 0,8 1 0,-1 0 0,-7 2 0,-2 0 0,-8 0 0,-4 0 0,-11 0 0,-4 0 0,25 0 0,-17 0 0,-13 0 0,-9 0 0,-4 1 0,-5 1 0,-2 0 0,-1 2 0,-1 0 0,0-2 0,-1 0 0,1 0 0,5 2 0,2 2 0,4 2 0,0 0 0,1 1 0,2 0 0,-1 0 0,7 2 0,4 1 0,1-1 0,-2 1 0,-3-4 0,-3-1 0,-2-2 0,-2-3 0,1 0 0,3 0 0,8 1 0,1 0 0,5 1 0,0 0 0,-5-1 0,4 2 0,6 1 0,11 1 0,1 2 0,-7 0 0,-15-3 0,-9-1 0,1-2 0,4-3 0,4 3 0,-4 2 0,-8 1 0,-11 1 0,1-1 0,8-1 0,14 1 0,1-3 0,-9 0 0,-16-2 0,-15-1 0,-7 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink12.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:18:56.190"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 281 24575,'22'0'0,"12"0"0,16 0 0,24 0 0,21 0 0,-40 0 0,1 0 0,5 0 0,1 0 0,2 0 0,2 0 0,5 0 0,2 0 0,3 0 0,0 0 0,1 0 0,1 0 0,3 0 0,-1 0 0,-2 0 0,-2 0 0,-2 0 0,-1 0 0,0 0 0,-2 0 0,-5 1 0,-1 2 0,-2 1 0,-1 1 0,-3 1 0,0 1 0,-3 0 0,0-1 0,2-2 0,0 0 0,1 0 0,1-1 0,1 1 0,2 0 0,2 0 0,1 0 0,1 0 0,1 0 0,5-2 0,0 0 0,0-2 0,0 1 0,-1 1 0,-1 0 0,-4 2 0,-1 1 0,-5 1 0,0 1 0,-2 1 0,-1 1 0,-1-1 0,0-1 0,3 0 0,1 0 0,0-1 0,1 0 0,4 0 0,0 0 0,3 0 0,1-1 0,3 0 0,1-1 0,4-1 0,2-2 0,2 1 0,3-2 0,5 0 0,3 0 0,-28 0 0,1 0 0,1 0-186,5 0 1,0 0 0,1 0 185,1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-2 0 0,-3 0 0,-1 0 0,-1 0 0,24 0 0,-2 0 0,-7 0 0,-4 0 0,-7 0 0,-3 0 0,-8 0 0,-2 0 0,-4 0 0,0 0 0,-2 0 0,-1 0 0,0 0 0,2 0 278,4 0 0,1 0-278,-3 0 0,0 0 0,-5 1 0,-1 1 0,31 1 0,-26 2 0,-13 1 0,-6-3 0,7 3 0,15-2 0,11 0 0,12-1 0,13-3 0,-38 0 0,4 0 0,10 0 0,3 0 0,7 0 0,2-1 0,7-4 0,2-2 0,1-3 0,1-3 0,0-3 0,1-2 0,-27 5 0,0-1 0,1-1-215,2 0 0,1-1 0,1-1 215,3 1 0,1-1 0,1-1 0,3 0 0,1-2 0,-1 1 0,-4 0 0,-1 0 0,-1 1 0,-5 1 0,-2 1 0,-2 1 0,23-6 0,-3 1 0,-12 5 0,-2 1 0,-6 2 0,-2 1 0,-6 3 0,-1 1 0,-5 1 0,-2 0 0,42-1 645,-4 0-645,-2-1 0,-3 3 0,-7 2 0,-12 3 0,-12 0 0,-9 0 0,0 0 0,8 0 0,11 0 0,13 0 0,2 0 0,-2 0 0,1 0 0,6 0 0,13 0 0,-42 0 0,1 0 0,-1 0 0,0 0 0,46 0 0,-2 0 0,-2 0 0,-42 0 0,2 0 0,6 0 0,2 0 0,6 0 0,2 0 0,7 0 0,3 0 0,5 0 0,2 2 0,4 3 0,0 2 0,1 1 0,0 1 0,-4 3 0,-2 1 0,-10 0 0,-4 0 0,-12-3 0,-5-1 0,28 8 0,-25-7 0,-4-3 0,19 3 0,24-2 0,-37-3 0,2-2 0,3 0 0,1-1 0,-3-2 0,0 1 0,-6-1 0,-1 0 0,39 0 0,-13 0 0,-16 0 0,-11 0 0,-2 0 0,-3 0 0,5 0 0,4 0 0,-4 0 0,0 0 0,-7 0 0,-3 0 0,4 0 0,1-1 0,-3-1 0,-10-2 0,-11 1 0,-8-1 0,-2 1 0,0 1 0,-8 0 0,-2 2 0,-7-2 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink13.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:19:05.756"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 181 24575,'60'0'0,"9"0"0,27 0 0,-40-1 0,2 2 0,10 1 0,2 2 0,8 2 0,2 2 0,5 2 0,2 2 0,6 1 0,2-1 0,2-2 0,0-1 0,-30-4 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,3 0 0,0 0 0,1 1-235,1-1 0,0 0 0,1 0 235,1-1 0,0-1 0,0 0 0,-1 1 0,-1-2 0,0 1 0,-4-1 0,-2-1 0,-1 0 87,24-1 0,-3 0-87,-11 1 0,-3 0 0,-8 1 0,-1 0 0,-6 0 0,-1 0 0,1 2 0,1 0 0,5-1 0,1 0 265,5 1 1,0 0-266,6 0 0,2 0 0,3-1 0,0-1 0,-1 1 0,-1-2 0,0 0 0,-1-1 0,-5 1 0,0-2 0,-2 1 0,-1 0 0,0 0 0,0 0 0,3 0 0,1 0 0,6 0 0,3 0 0,7 0 0,1 0 0,4 0 0,-1 0 0,1 0 0,-3 0 0,-8 0 0,-3 0 0,-12 0 0,-3 0 0,-8 0 0,-3 0 0,38 0 0,5 0 0,-41 0 0,1 0 0,7 0 0,1 0 0,4 0 0,1 0 0,0 0 0,-2 0 0,-2 1 0,0-2 0,-4 1 0,0-1 0,-3-3 0,0-1 0,3-2 0,2-1 0,5-4 0,3-1 0,6 0 0,3-1 0,6 1 0,1 1 0,-1-1 0,0 1 0,1 0 0,1 0 0,0 0 0,0-2 0,2-2 0,1 0 0,-1 1 0,0-1 0,-2 0 0,-1-1 0,-1 2 0,-1 1 0,-3 2 0,-3 0 0,-4 1 0,-2 0 0,-4 1 0,-2 2 0,-7 1 0,-2 0 0,-4 1 0,-3 2 0,45-1 0,-15 4 0,-6 1 0,-2 0 0,1 0 0,10 0 0,-34 0 0,1 0 0,6 0 0,2 0 0,11 0 0,4 0 0,6 0 0,1 0 0,1 0 0,0 0 0,1 0 0,0 0 0,-6 0 0,0 0 0,-2 0 0,1 0 0,3 0 0,1 0 0,0 0 0,1-1 0,2-1 0,0 0 0,-2-1 0,-1 1 0,-5 0 0,0-1 0,-6 1 0,-2 1 0,-6 1 0,-1 0 0,-3 0 0,-1 0 0,-5 0 0,-1 0 0,45 0 0,0 2 0,-46 1 0,0 3 0,6 1 0,2 1 0,8 2 0,2 2 0,8 2 0,2 0 0,7-1 0,1 0 0,0 0 0,-1 1 0,-5-1 0,-2 0 0,-8-2 0,-3 2 0,-10-1 0,-4 0 0,35 7 0,-18-4 0,-11-5 0,6-6 0,18-1 0,-32-3 0,3 0 0,7-1 0,2 2 0,2 0 0,0 1 0,1 0 0,-1 1 0,-4 0 0,-2 1 0,-5 1 0,-1-1 0,36 0 0,-26-1 0,-16-2 0,-14-1 0,1 0 0,3 0 0,5 0 0,8 0 0,9 0 0,11 0 0,6 0 0,3 0 0,-4 0 0,-5 0 0,-7 0 0,-10 0 0,-6 0 0,-6 0 0,-1 0 0,1 0 0,2 0 0,4 0 0,-1 0 0,0 0 0,-3 0 0,-4 0 0,4 0 0,3 0 0,4 0 0,-3 0 0,-5 0 0,-2 0 0,2 0 0,2 0 0,1 0 0,3 0 0,2 2 0,-3 2 0,-2-1 0,-10-1 0,-4-2 0,-5 0 0,-6 0 0,0 0 0,-4 0 0,-4-19 0,-5 14 0,-4-13 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink14.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:19:07.473"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 91 24575,'39'-4'0,"12"1"0,21 3 0,10 0 0,2-3 0,-4-4 0,-11-3 0,-11-1 0,-8 2 0,-5 2 0,0 2 0,6 0 0,6 0 0,9 0 0,4 2 0,-2 0 0,0 2 0,-3-2 0,-5 0 0,-8 0 0,-12 2 0,-12 1 0,-7 0 0,-4 0 0,-8 0 0,-1 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:19:15.924"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 280 24575,'38'-4'0,"14"0"0,29 4 0,-32 0 0,2 0 0,5 0 0,0 0 0,0 0 0,-2 0 0,-1 0 0,-2 0 0,46 0 0,1 0 0,-47 0 0,1 0 0,1 1 0,2-1 0,7 2 0,4 1 0,9 1 0,4 0 0,16 1 0,5 1-325,-24-2 0,2 0 0,1-1 325,6-1 0,2 0 0,-1 0 0,-2 0 0,-1-1 0,-2 0-36,-6-1 1,-2 0-1,-3 0 36,22 0 0,-3 0 0,-8 0 0,0 0 0,14 0 0,3 0-284,-26 0 1,2 0 0,2 0 283,7 0 0,3 0 0,1 0 0,1 0 0,1 0 0,0 0 0,-6 0 0,-1 0 0,0 0 0,4 0 0,0 0 0,0 0 0,4 0 0,0 0 0,2 0-410,4 0 1,1 0 0,1 0 409,-23 0 0,0 0 0,1 0 0,-2 0 0,23 0 0,-1 0 0,-3 0 134,-8 0 0,-2 0 0,-3 0-134,-8 0 0,-2 0 0,-3 0 49,22 0 0,-3 0-49,-2 0 0,0 0 0,1 0 0,3 0 0,8-2 0,4 0 35,-26-1 0,3-1 0,0 0-35,-1-1 0,1-1 0,-1 0 0,2-1 0,-1 0 0,1-1 0,-2-1 0,1-1 0,-2 1 0,-3-1 0,-1 1 0,0-1 0,0 2 0,0 1 0,0-1 376,-2 1 0,-1-1 0,-1 2-376,24 0 0,-2 1 249,-10 0 0,-3 0-249,-8-1 0,-3-1 0,-6 1 0,0-1 0,3 1 0,1 0 388,6 0 1,3 0-389,2 0 0,1 0 76,4 1 0,1 0-76,-3-1 0,0 0 0,-4 0 0,0 1 0,0 1 0,0-1 0,1 0 0,0-1 0,6 1 0,1 1 0,1-1 0,-1 1 0,0 1 0,-2 1 0,-7 0 0,-3 1 0,-8 1 0,-1 0 0,-2 0 0,0 0 0,4 0 0,1 0 0,6 0 0,2 0 0,2 0 0,0 0 0,-4 0 0,-4 0 0,-10 0 0,-3 0 0,31 0 0,-11 0 0,1 0 0,15 0 0,-37 1 0,0 1 0,7 1 0,1 2 0,5 1 0,0 1 0,2 1 0,1 1 0,2 0 0,0 1 0,0-1 0,-1 0 0,-4 0 0,-1 0 0,-7-1 0,-1 0 0,38 8 0,-22-1 0,-11-2 0,-11-3 0,0-1 0,16 1 0,19 1 0,-34-3 0,1 2 0,2-1 0,-1 1 0,-2 0 0,-2-1 0,38 6 0,-12-5 0,-7 0 0,-8-3 0,-6 0 0,-4-1 0,-5-3 0,1 0 0,7 3 0,11-2 0,18 0 0,17-1 0,-44-2 0,1-2 0,2 1 0,0 0 0,-1 0 0,-1 0 0,-2 0 0,-1 0 0,45 0 0,-8 0 0,-8 0 0,-12 0 0,-5 0 0,0 0 0,6 0 0,9 0 0,5 0 0,12 0 0,-41 0 0,2 0 0,5 1 0,2-2 0,0 0 0,-1-1 0,-9-1 0,-4 0 0,24-5 0,-26-1 0,-11 0 0,0 0 0,9-2 0,4 1 0,0 2 0,3-1 0,-2 1 0,3 2 0,1 3 0,-9 3 0,-6-2 0,-11-1 0,-9 1 0,-6-1 0,-4 1 0,-3-1 0,1 0 0,-1 1 0,0-1 0,-2-1 0,-2-3 0,-1-7 0,-3-6 0,-10-11-1696,-10-8 0,6 16 0,-2 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink16.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:19:18.971"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 482 24575,'83'-4'0,"-20"2"0,8 1 0,24 0 0,8 2 0,-26-1 0,4 0 0,1 0 0,13 0 0,4 0 0,2 0-1141,-15 0 0,3 0 0,1 0 0,1 0 1141,-13 0 0,2 0 0,0 0 0,2 0 0,-1 0 0,5 0 0,2 0 0,0 0 0,-1 0 0,-1 0 0,15 0 0,-2 0 0,-1 0 0,-3 0 95,-12 0 1,-2-1-1,-2 1 1,-4 1-96,10-1 0,-3 2 0,-5 0 478,12 3 1,-4 2-479,-5 2 0,0 2 0,8 4 0,3 0-347,-18-4 1,3 0 0,3-2 346,15 1 0,5-2 0,3-1-70,-17-2 1,2-1 0,3 0 0,2-1 69,-7-1 0,2 0 0,2-1 0,1-1 0,3 1-487,-6 0 0,2-1 0,2 1 0,1-1 0,1-1 1,2 0 486,-5-1 0,1 0 0,1 0 0,1-1 0,2-1 0,0 0 0,1-1-452,-5 0 0,2-1 0,1-1 0,0 0 0,1 0 0,1-2 0,-1 1 0,1-2 452,-9 1 0,1-1 0,0-1 0,1 0 0,0 0 0,-1-1 0,0 0 0,-1 0 0,0 0 0,5-1 0,1-1 0,-2-1 0,1 1 0,-2-1 0,0 0 0,-1 1 0,-2 0-141,4-1 0,-2 0 0,0 0 0,-1 1 0,-2-1 0,-1 2 1,-2-1 140,16-1 0,-1-1 0,-3 2 0,-3 0 0,-1 1 100,6 1 0,-3 1 0,-2 1 0,0 0-100,-5 0 0,0 1 0,-2 0 0,1 0 0,-2 1 0,-1 1 0,-1 0 0,1 0 0,-3 1 0,0 1 0,-1-1 0,0 2 442,0 0 1,0 0 0,0 1-1,-2 0-442,21 1 0,-2 0 0,-3 0 0,-6 2 0,-3 0 0,-1 0 1252,-3 0 0,-2 0 0,-2 0-1252,-8 0 0,-3 0 0,1 0 0,31 0 0,0 0 0,-1 0 0,0 0 0,-1 0 0,-2 0 0,-1 3 0,-3 2 1354,-9 1 1,-4 1-1355,-11 1 0,-3 1 867,-11-1 0,-2 0-867,42 2 627,-36-4 1,4 0-628,20 2 0,7-1 0,-18 0 0,4 0 0,1 0-49,4 0 1,2-1 0,-1-1 48,-1 1 0,1 0 0,-4 0 0,23 2 0,-5-1 0,-16-2 0,-4 0 0,-12 0 0,-4-1 0,39-1 0,-46-3 0,1 0 0,3 0 0,0 0 0,2 0 0,-1 0 585,44 0-585,-19 3 0,-16 0 0,-12 2 0,0 3 0,8 0 0,0 2 0,-7 0 0,-13-2 0,-12 0 0,-3-1 0,3 1 0,3 3 0,2 0 0,-1 2 0,-1-3 0,2 1 0,5 0 0,7-2 0,14 0 0,22 2 0,-31-6 0,2-1 0,4 1 0,2-1 0,-1-2 0,-1-1 0,39-1 0,-13 0 0,-19 0 0,-15 0 0,-13 0 0,-14 0 0,-10 0 0,-13-4-1696,-12-7 0,5 4 0,-3-3 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink17.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:19:23.172"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 203 24575,'63'-4'0,"-17"2"0,7 1 0,28 0 0,9 2 0,-16-1 0,4 0 0,2 0 0,5 0 0,3 0 0,2 0-541,-15 0 1,2 0 0,2 0 0,-1 0 540,0 0 0,1 0 0,0 0 0,1 0 0,4 0 0,0 0 0,1 0 0,1 0 0,4 0 0,1 0 0,0 0 0,-2 0 0,-8 0 0,-1 0 0,-2 0 0,1 0 0,-3-1 0,1 1 0,-1 0 0,-2 1-98,18 0 0,-2 1 1,-2 0 97,-5 2 0,-2 0 0,0 0 0,-3 0 0,0 1 0,-1 0-78,-8 0 1,-1 1 0,0 0 77,29 0 0,-1 0 0,-5-1 0,-2 0 0,1 1 0,0-2 0,0 0 0,-2-2 0,-2 1 0,-1-1 0,0 1 0,0-1 0,3 1 0,-1 0 0,-1 0 0,0 1 0,-3 0 0,1 1 0,-2-2 0,1-1 0,-1 1 0,0 0 0,6-1 0,2-1 0,4-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-2 0 0,0 0 0,0 0 0,1 0 0,-25 0 0,3 0 0,0 0-256,8 0 1,1 0 0,1 0 255,2 0 0,1 0 0,0 0 0,4 0 0,0 0 0,0 0 0,-3 0 0,0 0 0,0 0 0,3 0 0,0 0 0,2 0 36,6 0 1,1 0 0,1 0-37,-21 0 0,0 0 0,1 0 0,0 0 0,2 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,-1 0 0,1 0 0,-1 0 0,-3 0 0,1 0 0,-1 0 0,-2 0 0,20-1 0,-2-1 0,-2-1-38,-3 0 0,-2-1 0,1-1 38,0 0 0,-1-2 0,1 0 0,0 1 0,0-1 0,1 1 0,2 1 0,0 1 0,1 0 0,2 0 0,0 0 0,0 0 0,-4 0 0,-1 0 0,0 0 0,-3-2 0,-1 1 0,-1-2 38,-9 2 1,-2-1 0,-2 0-39,19-2 0,-5 1 386,-10 0 0,-2 0-386,-7 2 0,1-1 718,3 0 0,1-2-718,10 0 0,3 1 0,3-2 0,1 0 0,2-2 0,0 0 503,-7 2 0,-3-1-503,-13 1 0,-3 0 63,-11 2 0,-3 1-63,28-4 0,-7 3 0,6 0 0,8 0 0,3 2 0,-2 1 0,-12 4 0,-11 0 0,-4 0 0,-3 0 0,5 0 0,7 0 0,3 0 0,1 0 0,-8 0 0,-10 0 0,-5 0 0,2 0 0,17 0 0,18 0 0,10 0 0,-1 0 0,-11 0 0,-17 0 0,-11 0 0,-6 0 0,0 0 0,5 0 0,2 0 0,0 0 0,-6 0 0,-4 0 0,0 0 0,2 0 0,8 0 0,8 0 0,6 1 0,-5 1 0,-11 2 0,-13 2 0,-12 1 0,-7-1 0,-4-1 0,-4-1 0,-2-1 0,-3 0 0,-2-2 0,0 1 0,0 0 0,1-2 0,4 0 0,2 0 0,2 0 0,0 2 0,-1 0 0,-4-1 0,-9-10 0,-1 5 0,-5-7 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink18.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:19:27.172"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 289 24575,'46'-4'0,"33"1"0,-18 3 0,7 0 0,-1 0 0,5 0 0,3 0 0,6 0 0,2 0 0,1 0 0,5 0 0,1 0 0,2 0-708,-15 0 0,2 0 0,0 0 1,-2 0 707,18 0 0,-2 0 0,1 0 0,-19 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,-2 0 0,15 0 0,-2 0 0,-1 0 147,-2 1 0,-1-1 0,-3 1-147,23 1 0,-7 1 285,-17 1 0,-5 1-285,-11 1 0,-2 0 0,2 0 0,1-2 0,8 0 0,4-2 0,13 0 0,4 0 0,-25-2 0,1 0 0,-1 0 0,33 0 0,-2 0 0,-5 0 0,-1 0 0,-7 0 0,-1 0 0,-3 0 0,1 0 0,8 0 0,2 0 0,-26 0 0,1 0 0,1 0 294,3 0 0,2 0 0,0 0-294,4 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,0 0 0,-1 0 0,-1-2 0,0 1 0,-1-1 0,-2 0 0,-1 0 0,-1 0 0,31-1 0,-3 0 176,-6 0 0,-2 1-176,-7 2 0,-2 0 0,-6 0 0,-1 0 0,-4 0 0,0 0 0,0 0 0,0 0 0,-3 0 0,-1 0 284,0 0 1,0 0-285,0 0 0,1 0 8,0 0 1,2 0-9,14 0 0,3 0 0,-21 0 0,3 0 0,1 0-289,8 0 1,3 0-1,1 0 289,5 0 0,0 0 0,0 0 0,-3 0 0,-2 0 0,-1 0 0,-7 0 0,-1 0 0,-3-1 0,25-1 0,-4 0 0,-5-1 0,-1 1 0,-2-1 0,0 1 0,4 0 0,0 0 0,1 0 0,1-1 0,2 1 0,0-1 0,2 1 0,0 0 0,1 0 0,-1 1 0,-1 1 0,-1 0 0,-1 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-3 0 0,-2 0 0,-7 0 0,-2 0 0,-4 0 0,0 0 0,-4 0 0,0 0 0,-2 0 0,0 0 433,-2 0 0,-2 0-433,-5 0 0,-1 0 0,35 0 0,-10 0 0,0 0 0,4 0 0,12 0 0,-43-1 0,1-2 0,1 1 0,-1-1 0,4 0 0,-1-2 0,3-1 0,0 0 0,6-1 0,3 0 0,18 0 0,4 0 0,7-1 0,3 2-267,-25 2 0,3 1 0,0 0 267,3 0 0,1 0 0,0-1 0,-5-1 0,0 0 0,-1 0 0,-2 1 0,-1 0 0,-3 0 0,22-3 0,-4-1 0,-10 1 0,-2-1 0,-5 1 0,2-1 0,12-2 0,4-1 0,9 1 0,3 1-247,-25 2 1,1 2 0,1 0 246,3-1 0,0 1 0,-1 1 0,-5 0 0,-1 1 0,-1 1 383,29-1 0,-4 0-383,-13 0 0,-2-1 0,-2 1 0,-1 1 0,-1-1 0,2 1 0,6 0 0,1 0 0,3 2 0,-2 0 0,-4 0 0,-3 0 0,-10 0 0,-4 0 0,32 0 769,-34 0-769,-27 0 5,-14 0-5,-9 0 0,-3 0 0,-4 0 0,-4 0 0,-2 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink19.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:19:31.955"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 503 24575,'14'-3'0,"13"0"0,41 3 0,24 0 0,-21 0 0,6 0 0,5 0 0,3 0 0,4 0 0,3 0 0,-24 0 0,2 0 0,1 0-342,4 0 1,2 0 0,0 0 341,4 0 0,1 0 0,2 0 0,8 0 0,1 0 0,1 0 0,-2-1 0,0 1 0,0 1 0,-4 0 0,0 0 0,1 2 0,4 0 0,1 1 0,0 1-381,-1 2 1,-1 2-1,3 0 381,-20-2 0,1 2 0,1-1 0,1 0 0,4 1 0,1-1 0,0 0 0,1 0 0,0 1 0,1-1 0,0 0 0,-1 0 0,-1-1 0,0 0 0,-1-1 0,0 1 0,-2 0 0,-1-1 0,0 1 0,-1 0 0,20 3 0,-2 0 0,1 1 0,-22-2 0,1 0 0,-1 1 0,2 0 0,2 1 0,2 0 0,-1 1 0,2 0 0,2 1 0,0 0 0,1 0 0,0 0 0,3 0 0,1 0 0,0 0 0,-1-1 0,-4 0 0,0 0 0,-2-1 0,-1 0 0,17 2 0,-3-1 0,-1 0-201,-8-2 0,-2 0 1,-2-1 200,-8 1 0,-1-1 0,-1 1 0,-3-1 0,0 0 0,1 1 0,2-2 0,0 1 0,1-1 0,-1 0 0,-1 0 0,0 0 0,28-1 0,-2-1 0,-11-1 0,-3-2 0,-13 0 0,-3-1 347,-5-2 1,-1 0-348,9 0 0,2 0 0,10 0 0,4 0 0,-21 0 0,3 0 0,0 0 243,8 0 0,1 0 1,1 0-244,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-6 0 0,-1 0 0,1 0 0,3-1 0,0 0 0,2-2 0,9-1 0,1-2 0,2-1-278,7-2 0,2-2 0,2-1 278,-20 2 0,2-2 0,0 1 0,-1-1 0,-4 1 0,0 0 0,0-1 0,-3 2 0,17-3 0,-2 1 0,-1 1-155,-6 1 1,-2 1-1,-2 0 155,-8 0 0,-3 1 0,1 0 0,29-5 0,1-1 0,-30 4 0,0 0 0,1-1 0,3-2 0,1-2 0,0 0 0,3 0 0,0 0 0,-1-1 0,-2 0 0,-1 0 0,-3-1 0,23-6 0,-5 2 0,-12 4 0,-5 2 0,-11 2 0,-3 1 312,-6 2 1,-1 0-313,0 1 0,2 1 749,3-3 0,2 0-749,11-1 0,4 0 0,10-2 0,4-1 0,7-1 0,0-2 0,3 1 0,-1-2 0,-4 0 0,-2-1 0,-6 1 0,-3 0 259,-3 1 0,-2 1-259,-6 2 0,-1 1 0,-1 3 0,-2 1 0,0 2 0,-1 1 0,-3 2 0,-1 2 0,-1 0 0,-2 2 0,-3-1 0,0 2 0,1 0 0,0 0 0,5 0 0,1 0 0,2 0 0,-1 0 0,-1 0 0,-1 0 0,38 0 0,-23 0 0,-20 0 0,-12 0 0,-2 0 0,6 5 0,3 7 0,1 4 0,-1 4 0,0-2 0,6 0 0,5 3 0,0 1 0,-10 2 0,-11-5 0,-13-4 0,-7-4 0,-3-2 0,1-1 0,0 1 0,6 3 0,8 3 0,4-1 0,-3-4 0,-16-6 0,-25-4 0,-38 0 0,-35 0 0,32 0 0,-3-1 0,0-1 0,1-1 0,-36-7 0,13-3 0,-11-4 0,30 7 0,-4 0 0,-14-2 0,-3 1 0,-8-1 0,0 1 0,6 1 0,4 1 0,12 3 0,4 1 0,-23-2 0,25 0 0,6-2 0,-7-1 0,-12 0 0,-5 2 0,-11 4 0,-7-3 0,36 3 0,-3-1 0,-14-3 0,-3 0 0,-3-2 0,-1 0 0,1 0 0,2 0 0,7 1 0,1 0 0,-3 2 0,-4 1 0,-14 1 0,-4 2-245,22 0 0,-2 0 1,-1 0 244,-4 0 0,0 1 0,1-1 0,9 0 0,1-1 0,3-1 0,-21-2 0,3-2 0,-1 0 0,-2-1 0,18 3 0,-2 0 0,-5 1-549,-19 0 1,-5 2-1,-2-1 549,19 1 0,-3 1 0,0-1 0,1 1 0,1 0 0,1 0 0,0 0 0,3-1-100,-14-1 0,3 0 0,6-2 100,-12-2 0,9-2 331,24 3 0,6 0-331,-22-5 0,17 1 0,-10 3 1679,-24 2-1679,38 5 0,-3 1 169,-8 0 1,-3 0-170,-6 1 0,-1 0 0,-2 0 0,-2 0 0,-1 0 0,0 0 0,2 0 0,0 0 0,6 1 0,0 2 0,4 2 0,1 2 0,3 3 0,0 2 0,0 1 0,-1 2 0,2 0 0,2 0 0,6-2 0,3 0 0,-39 7 0,24-3 0,15-3 0,6-1 0,0-1 0,-4-1 0,-9 2 0,-7-1 0,-4 2 0,-11 2 0,36-8 0,-2 1 0,-5 2 0,-2 0 0,-5 0 0,-1 1 0,-5 0 0,0 0 0,0 1 0,0-1 0,1 0 0,2-1 0,4-2 0,3-1 0,5 0 0,2-1 0,-43 1 0,3-4 0,-3-1 0,45-3 0,-1 0 0,-10 0 0,-2 0 0,-1 0 0,-1 0 0,0 0 0,1 0 0,2 0 0,1 0 0,8 0 0,1 0 0,2 0 0,1 0 0,-38 0 0,11 0 0,11-2 0,9-1 0,2 0 0,-4-3 0,-6 1 0,-8-2 0,-1 0 0,3 3 0,-3 0 0,-6 4 0,-8 0 0,-3 0 0,0-3 0,10-1 0,2 0 0,0 1 0,-8 3 0,36 0 0,-2 0 0,-6 0 0,-1 0 0,-3 0 0,-1 0 0,-1 0 0,-1 0 0,-3 0 0,-2 1 0,-11 3 0,-5 4 0,16 0 0,-4 3 0,-3 3-52,6 1 0,-4 2 1,1 1-1,7-2 1,-20 5-1,6 0 1,0 2-1,-1 1 1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:17:48.374"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 148 24575,'52'0'0,"9"0"0,14 0 0,1 0 0,-3 0 0,-15 0 0,-5 0 0,-5 0 0,-1 0 0,6 0 0,3 0 0,6 0 0,6 0 0,-4 0 0,-7 0 0,-8 0 0,-11 0 0,-10 0 0,-8 0 0,-5 0 0,-3 0 0,2 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,3 0 0,5-4 0,4 0 0,1-1 0,1 2 0,1-1 0,15-6 0,12-6 0,13-4 0,0 2 0,-15 4 0,-8 1 0,-13 3 0,1-1 0,-2 3 0,-13 4 0,-4 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:17:54.908"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'64'0'0,"25"0"0,-27 0 0,4 0 0,10 0 0,2 0 0,0 0 0,0 0 0,-7 0 0,-3 0 0,-10 0 0,-3 0 0,35 5 0,-17 5 0,2 0 0,-3 3 0,-3-5 0,-6-4 0,-14 0 0,-8-1 0,-7 2 0,-1-1 0,-1 0 0,0-4 0,1 0 0,-1 0 0,1 0 0,-1 3 0,0 1 0,-14 1 0,-3-2 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:18:02.441"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 94 24575,'79'0'0,"14"0"0,-36 0 0,3 0 0,1 0 0,-2 0 0,-5 0 0,-2 0 0,35 0 0,-19 0 0,0 0 0,7 0 0,1 0 0,-2 0 0,-14 0 0,-13 0 0,5 0 0,10 0 0,17 0 0,14 0 0,-8 0 0,-16 0 0,-21 0 0,-26 0 0,-12 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1550">189 12 24575,'39'-6'0,"38"0"0,-17 6 0,7 0 0,19 0 0,4 0 0,-22 0 0,2 0 0,1 0 0,-2 0 0,1 0 0,-1 0 0,28 0 0,-3 0 0,-18 0 0,-5 0 0,24 0 0,-31 0 0,-37 0 0,-12 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:18:05.707"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">14746 504 24575,'13'0'0,"1"0"0,13 0 0,22 0 0,32 0 0,-31 0 0,3 0 0,6 0 0,0 0 0,1 0 0,-1 0 0,-3 0 0,-3 0 0,42 0 0,-14 0 0,-7 0 0,1 0 0,5 0 0,-5 0 0,5 0 0,-7-4 0,-11 0 0,-10-1 0,-14-1 0,-10 2 0,-1-4 0,-2 0 0,-12 3 0,-1 1 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1517">14946 1387 24575,'20'0'0,"0"0"0,1 0 0,4 0 0,1 0 0,-2-4 0,-3-4 0,-4-1 0,2-1 0,13-1 0,21-1 0,30-4 0,-31 6 0,3 1 0,8-2 0,2 0 0,3 1 0,-1 1 0,-5 3 0,-3 0 0,37-4 0,-31 6 0,-38-1 0,-10 2 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7551">0 1238 24575,'58'0'0,"28"0"0,-30 0 0,4 0 0,8 0 0,2 0 0,2 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 0 0,-2 0 0,-1 0 0,-5 0 0,-1 0 0,-3 0 0,-1 0 0,-4 0 0,-1 0 0,42 0 0,-1 0 0,-13 0 0,-13 0 0,-7 0 0,-7 0 0,1 0 0,4 0 0,-5 0 0,4 0 0,3 0 0,7 0 0,12-5 0,4-1 0,2 0 0,8-4 0,1 4 0,1-5 0,-44 5 0,2 1 0,0-1 0,0-1 0,2 0 0,0 0 0,2 0 0,-1-1 0,-2 1 0,-2-1 0,1 1 0,0 1 0,-1 1 0,0-1 0,-3 1 0,-1 0 0,48-5 0,-9 2 0,9-2 0,-43 6 0,1-1 0,6-2 0,1 0 0,7-1 0,1 0 0,-1-1 0,1-1 0,1-1 0,1 1 0,-2 1 0,-1 0 0,3-2 0,0 1 0,5 1 0,0 0 0,3-2 0,0 0 0,2 0 0,-1 0 0,-5 1 0,0 0 0,-6 1 0,0 1 0,-2 3 0,1 1 0,8 0 0,3 2 0,14 1 0,5 2-293,-24-1 0,2 0 0,1 0 293,5 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,-2-1 0,-1 1 0,1 1 0,-1 0 0,1 2 0,-2 0 0,-2 0 0,-2 0 0,0 1-26,25 3 1,-2 2 25,-9 1 0,-4 0 0,-11-3 0,-4-1 0,-4 1 0,-1-1 0,-5-3 0,1-2 0,1-1 0,1 0 438,7 0 1,2 0-439,4 0 0,2 0 0,9 0 0,3 0 0,9 0 0,4 0-296,-28 0 0,2 0 1,2 0 295,6 0 0,2 0 0,3 0 0,-16 0 0,2 0 0,2 0 0,2 0-597,13 0 1,2 0-1,3 0 1,0 0 596,-15 1 0,2-1 0,0 1 0,1 0 0,1 0 0,3 1 0,0 0 0,2 1 0,-1 1 0,-1 0 0,-3 1 0,1 1 0,-1 0 0,-1 2 0,-3 0-251,8 3 1,-2 1 0,-2 1 0,-3 1 250,13 5 0,-2 0 0,-7 2 0,-18-2 0,-4 0 0,-5 1 0,7 4 0,-6 1 388,-13-1 1,-3 0-389,27 23 2355,-11 5-2355,-11-3 1195,-12-5-1195,-8-8 0,3-7 0,23 4 0,-11-13 0,5 0 0,14 2 0,3-1 0,5 0 0,-1-2 0,-7-4 0,-3-2 0,29 1 0,-33-8 0,-19-6 0,-10 0 0,-8-8 0,-5-8 0,2-9 0,7-14 0,20-14 0,19-5 0,2 0 0,-6 12 0,-22 17 0,-21 9 0,-9 6 0,-8 2 0,-14 1 0,-26 1 0,-43-1 0,26 6 0,-4 0 0,-7-1 0,-1-1 0,2 1 0,3 0 0,8-1 0,2 1 0,3-1 0,0 2 0,1 1 0,0 1 0,-5 1 0,0 0 0,-3 1 0,1 2 0,5-3 0,-1 1 0,1-2 0,0 0 0,1 0 0,-2 0 0,-14 0 0,-5 0 0,-19 2 0,-6 0-363,18 1 1,-3 0 0,-2 0 362,-3 0 0,-1 0 0,2 0 0,6 0 0,3 1 0,3-2 0,-18 0 0,8-1 0,28 0 0,5 0 0,-31-2 0,2 0 0,-10 3 0,-6 1 1087,6 0-1087,10 0 0,-8 0 0,40 0 0,-2 0 0,-12 0 0,-1 0 0,-5 0 0,0 0 0,0 0 0,1 0 0,4 0 0,2 0 0,11 0 0,1-1 0,-47-5 0,4-2 0,43 3 0,0 1 0,-3-1 0,0-1 0,4 3 0,-1 0 0,-2 0 0,-1 1 0,-5-1 0,-2 2 0,-5 1 0,-1 0 0,-7 0 0,0 0 0,-1 0 0,2 0 0,5 0 0,1 0 0,0 0 0,2 0 0,5 0 0,2 0 0,-1 0 0,-1 0 0,-5 0 0,-1 0 0,-5 0 0,-3 0 0,-5 2 0,-2 2 0,-3 1 0,-1 1 0,5 3 0,0 1 0,3 0 0,2 1 0,5-1 0,2-1 0,3-1 0,1-1 0,-1 0 0,1 0 0,4-1 0,1-1 0,-2-2 0,0 0 0,5-1 0,0 1 0,2-3 0,-1 0 0,-3 0 0,0 0 0,-4 0 0,-3 0 0,-8 0 0,-1 0 0,-2 0 0,0 0 0,0 0 0,1 0 0,1 0 0,1 0 0,3-3 0,-1-1 0,-8 1 0,-1-1 0,-6-3 0,-1-1 0,-5 1 0,-2 0 0,26 2 0,-2 0 0,2-1 0,-31-5 0,1 0 0,1 3 0,1-1 0,5-2 0,2 1 0,4 2 0,1 2 0,-1 2 0,1 0 0,-1 0 0,2 0 0,3 2 0,3-2 0,7-2 0,3-1 0,11 0 0,4 0 0,-33-10 0,12 2 0,-1 0 0,-16 1 0,-5 4 0,-1-1 0,5 3 0,11-3 0,-1 2 0,-4 3 0,-3 3 0,6 3 0,11 0 0,15 0 0,16 0 0,12 0 0,8-1 0,-3-7 0,14 5 0,-5-4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10452">214 372 24575,'53'0'0,"20"0"0,22 0 0,-35 0 0,2 0 0,11 0 0,3 0 0,7 0 0,2 0 0,12 1 0,2 1 0,-1 3 0,0 1 0,-3 0 0,-1 2 0,-3 1 0,-2 1 0,-4 0 0,-1 0 0,1-1 0,-1 0 0,1 1 0,0-1 0,0-1 0,-1 0 0,-2 0 0,-3-1 0,-7 2 0,-2 0 0,-5-2 0,-2 1 0,-7 1 0,-1-1 0,0-2 0,0 0 0,3 1 0,2 0 0,4 2 0,1 0 0,3 2 0,2 0 0,-1 0 0,0-1 0,0 1 0,-1-1 0,-3-2 0,-1-2 0,-3-1 0,-1-2 0,-1 1 0,0-1 0,-1-3 0,1 0 0,-4 0 0,2 0 0,5 0 0,2 0 0,0 0 0,1 0 0,1 0 0,0 0 0,8 0 0,1 0 0,5 0 0,2 0 0,9 0 0,3 0 0,4 0 0,1 0 0,-2 0 0,-1 0 0,-5 0 0,-1 0 0,-3 0 0,-1 0 0,5 0 0,0 0 0,6 0 0,0 0 0,1 0 0,0 0 0,-31 0 0,1 0 0,-1 0 0,31 0 0,-1 0 0,-6 0 0,1 0 0,3 0 0,1 0-198,-29 0 0,0 0 1,1 0 197,4 0 0,0 0 0,2 0 0,5 0 0,2 0 0,0 0 0,4 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-2 0 0,0 0 0,-1 0 0,-5 0 0,0 0 0,-1 0 0,-1-2 0,-1-1 0,0 0 0,-2-1 0,-2-1 0,-1 0 0,22-4 0,-2 1 0,-6 0 0,-2 0 0,-6 1 0,-1 1 0,1 2 0,1-1 0,4-4 0,2-1 0,7-3 0,3-2 0,5-2 0,2-3-215,-29 4 0,0-2 0,1 1 215,3 1 0,1 1 0,-1-1 0,-3-1 0,0 0 0,-1-1 0,-4 1 0,0 1 0,-1-1 204,27-5 0,0 0-204,-1-3 0,1 0 0,0 2 0,0 1 0,-3 1 0,-2 0 0,-5 1 0,-4 1 0,-13 3 0,-2 2 0,-8 1 0,-1 2 0,41-5 659,-15 5-659,-7 0 171,-14 1-171,-6 4 0,1 1 0,0 5 0,7 0 0,-6 0 0,-8 0 0,-8 0 0,-6 0 0,-4 0 0,-6 0 0,-7 2 0,-8 2 0,-3 3 0,1 2 0,0 1 0,0 1 0,0-2 0,-2-1 0,4-2 0,1 3 0,4 6 0,3 1 0,3 3 0,13 2 0,11 6 0,12 6 0,0 0 0,-8-2 0,-11-6 0,-12-5 0,-10-4 0,-6-8 0,-6-5 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:18:19.057"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">13388 270 24575,'-21'0'0,"-14"0"0,-34 0 0,20 0 0,-5 0 0,-8 0 0,-2 0 0,-1 0 0,1 0 0,2 0 0,0 0 0,-5 0 0,-3 0 0,-8 0 0,-3 0 0,-6 0 0,-1 0 0,0 0 0,2 0 0,9 0 0,2 0 0,7 0 0,-2 0 0,-7 0 0,-4 0 0,-11 0 0,-2 0-182,24 2 1,-2 1 0,0 0 181,-2 0 0,-1 0 0,3 0 0,-28 2 0,4 0 0,8-1 0,3-1 0,9-2 0,2-2 0,5 1 0,0 0 0,0 1 0,0-2 0,-1-1 0,0-2 0,-4 0 0,0-1 272,-1 0 0,1-3-272,-1 0 0,0-2 0,-4 0 0,0 0 0,-1-3 0,1 0 0,-2 1 0,2 2 0,4 0 0,1 1 0,4 2 0,1 1 0,4 1 0,2-1 0,0 0 0,1-1 0,2 1 0,0 0 0,1-2 0,0 0 0,-4 2 0,0 0 0,-4-1 0,0-1 0,-2 1 0,-2 1 0,2 1 0,-1-1 0,6-1 0,0 1 0,2 2 0,1 0 0,1-2 0,1 0 0,2 1 0,0 0 0,-1 2 0,-1 0 0,2 0 0,-1 1 0,-2 2 0,0 0 0,-2 0 0,-2 0 0,-7 0 0,-3 0 0,-6 0 0,-3 0 0,-3 5 0,-2 2 0,-3 2 0,2 2 0,6 1 0,3-1 0,4 0 0,2-1 0,4-3 0,1-1 0,5-1 0,1-1 0,3 0 0,1-1 0,1 1 0,1-1 0,-2-3 0,1 0 0,2 0 0,1 0 0,1 0 0,0 0 0,1 0 0,1 0 0,2 0 0,0 0 0,0 0 0,1 0 0,-43 0 0,12 0 0,-1 0 0,-1 0 0,-6 0 0,-9 0 0,47 0 0,0 0 0,-4 0 0,0 0 0,-1 0 0,1 0 0,4 0 0,1 0 0,-1 0 0,0 0 0,-48 0 0,43 0 0,-1 0 0,-8 0 0,-1 0 0,-4 0 0,-1 0 0,-2 0 0,1 0 0,3 0 0,1 0 0,3 0 0,1 0 0,3 0 0,1 0 0,2 0 0,0 0 0,3 0 0,0 0 0,0 0 0,1 0 0,2 0 0,2 0 0,-44 0 0,7 0 0,12 0 0,-4 0 0,-10 0 0,37 0 0,-2 0 0,-5 0 0,-1 0 0,-4 0 0,-1 0 0,3 0 0,0 0 0,5 0 0,1 0 0,1 0 0,0 0 0,4 0 0,-1 0 0,-2 0 0,-2 0 0,0 0 0,2 0 0,-42 0 0,5 0 0,16 0 0,6 0 0,-5 0 0,-2 0 0,-7 0 0,0-1 0,7-5 0,9-9 0,17-5 0,9-3 0,11 4 0,16 10 0,3 3 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:18:23.607"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">263 1184 24575,'24'0'0,"39"0"0,5 0 0,9 0 0,-10 0 0,3 0 0,2 0 0,9 0 0,2 0 0,0 0-583,4 0 1,1 0-1,-1 0 583,-4 0 0,0 0 0,1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-2 0 0,-7 0 0,0 0 0,-3 0 89,-5 2 0,-2 0 1,-1 0-90,31 2 0,-2 0 0,-1 3 0,1 0 0,2 0 0,2 0 0,-31-3 0,1-1 0,-1 1 0,28 3 0,-2 0 0,-7-1 0,-2 2 180,-5-1 0,-2 0-180,-4 1 0,0-1 0,4-1 0,2 0 0,13 0 0,4 0-228,-29 0 0,2 1 0,1 0 228,6 1 0,2 0 0,0 0 0,6 3 0,1 0 0,-1 0 0,2 1 0,0 0 0,1-1-113,7-1 1,0-1-1,1 0 113,-3 0 0,0 0 0,0-1 0,0-2 0,-1 0 0,0 0 0,-4 0 0,0-1 0,-2 1-92,-9 0 0,-2 0 0,0-1 92,-2-1 0,0-1 0,-1 0 0,27 2 0,-2-2 0,0-2 0,2-2 0,-28 1 0,2 0 0,1 0 0,0 0 0,1 0 0,1 0 0,5 0 0,2 0 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-4 0 0,0 0 0,0 0 0,-1 0 0,-1 0 0,0 0 0,-5 0 0,-1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,3 0 0,0 0 0,2 0 0,8 0 0,1 0 0,2 0-339,6 0 0,1 0 0,1 0 339,-1 1 0,1-1 0,-2 2 0,-3 0 0,-2 1 0,-1 0 84,-9 0 0,-1 0 0,-2 0-84,-6 1 0,-1 0 0,-2-1 0,26 2 0,-3 0 560,-11-2 1,-3 0-561,-11 2 0,-2 0 250,-6 0 1,-3-1-251,41 2 1129,-5-1-1129,0-5 432,1 0-432,-39 0 0,3 0 0,12 0 0,3 0 0,19 0 0,7 0 0,-17-1 0,5-1 0,0-1-299,6-1 0,0-1 0,0-1 299,-2 0 0,0-2 0,-3-1 0,-8 0 0,-3-1 0,-3-1 0,15-4 0,-5-1 0,-7 2 0,-3 0 0,-8 1 0,0-1 0,-2 1 0,0 0 0,-4 1 0,-1 0 0,-3 2 0,-2 2 897,42-5-897,-17 3 0,-1 4 0,3-10 0,15-7 0,-42 10 0,0-2 0,37-17 0,-20 3 0,-27-2 0,-13-8 0,3-23 0,-1-13 0,0-3 0,-8 13 0,-11 20 0,-8 15 0,-11 7 0,-7 4 0,-15-1 0,-13-5 0,-9 0 0,-3-1 0,4 2 0,7-1 0,11 6 0,5 2 0,-3 5 0,-9 1 0,-12-7 0,1-3 0,0-11 0,-4-14 0,20 11 0,-1-4 0,-10-11 0,-1-2 0,-3-3 0,0 2 0,2 5 0,2 5 0,-26-11 0,20 31 0,15 18 0,6 5 0,-6 0 0,-1 3 0,0 5 0,-11 1 0,-20 5 0,14-6 0,-5 1 0,-15 1 0,-4 1 0,-12 3 0,-2 0 0,-3-2 0,1-2 0,4 1 0,1-1 0,-2-1 0,-2 2 0,31-4 0,0 1 0,-2 2-275,-6 2 0,-2 2 1,-1 1 274,-5 2 0,-2 0 0,-1 2 0,-4 1 0,-2 1 0,-1 1-448,-4 1 0,-1 0 0,0 1 448,23-7 0,0 1 0,1-1 0,0 1 0,-20 5 0,1 0 0,2-1-107,8-3 0,1 0 0,4-2 107,-20 2 0,5-3 0,19-5 0,4-4 0,10-4 0,4 0 754,-35 2-754,8 1 1376,6 0-1376,1-4 359,-13-2-359,38 0 0,-4 0 0,-13 0 0,-5 0 0,-7 0 0,-3 0 0,-4 0 0,-1 0 0,-4 0 0,2 0 0,7 0 0,2 0 0,4 0 0,0 0 0,5-2 0,1-2 0,4-2 0,0-2 0,1-2 0,0-1 0,3 0 0,3 0 0,6 2 0,1-1 0,-39-7 0,8-1 0,0-4 0,-6 0 0,0 4 0,0 2 0,-1 1 0,7-1 0,-1-4 0,-6 3 0,-4 1 0,44 8 0,-1-1 0,-2 0 0,0 0 0,-2-2 0,0 1 0,-2-1 0,-1 1 0,-2 2 0,0 1 0,5 1 0,0 0 0,-44-4 0,0 1 0,0-3 0,47 6 0,-1 1 0,-3 1 0,-1 1 0,-1 1 0,0 1 0,-1 0 0,0 2 0,1-1 0,1 0 0,0 0 0,-1 0 0,-1 0 0,-1 0 0,0-2 0,-1 1 0,-6-2 0,-1 0 0,-5 0 0,0 0 0,-5 0 0,-2 1 0,-2 0 0,-3 2 0,-4 0 0,-1 0 0,-1 0 0,-2 0 0,-5 0 0,-1 0 0,-1 0 0,2 0 0,7 0 0,2 0 0,9 0 0,5 0 0,12 0 0,4 0 0,7-1 0,2 2 0,-41 4 0,2 1 0,0 4 0,5 1 0,2-5 0,7-1 0,6-1 0,1 0 0,13 1 0,1 3 0,-6 3 0,-4 5 0,-11 3 0,-6 3 0,-2 4 0,-1 4 0,5 2 0,6 1 0,6-7 0,8-2 0,13-6 0,11-5 0,18-6 0,6-2 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2283">1 789 24575,'50'-21'0,"36"-16"0,-22 11 0,4-3 0,7-4 0,0 0 0,-7 2 0,-3 2 0,-11 7 0,-3 4 0,19-1 0,-20 12 0,-16 4 0,-11 3 0,-5 0 0,0 0 0,4 0 0,6 0 0,4 0 0,0 3 0,0 1 0,0 0 0,12 0 0,21-3 0,20-1 0,-33 0 0,1 0 0,1 0 0,1 0 0,-2-1 0,2-4 0,7-5 0,1-5 0,2-7 0,0-4 0,2-4 0,-3-1 0,-9 3 0,-4 3 0,19-6 0,-39 21 0,-17 10 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:18:29.040"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 383 24575,'48'0'0,"13"0"0,18 0 0,10 0 0,8 0 0,-46 0 0,1 0 0,6 0 0,1 0 0,4 0 0,2 0 0,-1 0 0,1 0 0,6 0 0,0 0 0,-1 0 0,0 0 0,4 0 0,0 0 0,0 0 0,0 0 0,-4 0 0,0 0 0,-5 0 0,-1 0 0,-5 0 0,-1 0 0,-3 1 0,-2-2 0,-2-3 0,-1-1 0,3-1 0,1-1 0,0 1 0,0 0 0,5 0 0,1 1 0,-2 2 0,0 1 0,0-1 0,-1 0 0,3 0 0,0 0 0,1 1 0,2 0 0,6 2 0,3 0 0,4 0 0,0 0 0,0 0 0,-1 0 0,-2 0 0,-1 0 0,-5 0 0,-2 0 0,-7 0 0,-2 0 0,1 0 0,-1 0 0,-1 0 0,-2 0 0,40 0 0,-7 0 0,-17 0 0,-1 0 0,5 0 0,7 0 0,6 0 0,2 0 0,8 0 0,-44 0 0,2 0 0,8 0 0,2 0 0,9 0 0,1 0 0,5 0 0,2 0 0,2 0 0,2 0 0,-1 0 0,0 0 0,-4 0 0,0 0 0,-1 0 0,-1 0 0,-6 0 0,-4 0 0,-7 0 0,-2 0 0,-5 0 0,-2 0 0,37 0 0,-1 0 0,1 0 0,-1 0 0,9 0 0,-43 0 0,2 0 0,8 0 0,3 0 0,8 0 0,1 0 0,4 0 0,2 0 0,7 0 0,2 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,-2 0 0,-2 0 0,-6 0 0,-3 0 0,-4 0 0,-3 0 0,-3 0 0,-2 0 0,-4 0 0,-2 0 0,-2 0 0,-2 0 0,3 0 0,-1 0 0,0 0 0,-2 0 0,0 0 0,-2 0 0,-3 0 0,-1 0 0,40 0 0,-11 0 0,-1 0 0,-4 0 0,-6 0 0,-6 0 0,-8-3 0,0-2 0,15-3 0,-21 3 0,4 0 0,17-1 0,6 0 0,19-4 0,6 0-521,-21 2 1,4-1 0,3 1 520,-8 0 0,2-1 0,3 0 0,1 1-543,7-1 1,2-1-1,2 1 1,0 0 542,-14 1 0,0 0 0,1 0 0,1 0 0,-2 1 0,0-1 0,1 0 0,-1 0 0,-1 0 0,-1 1 0,12-1 0,-2 0 0,-1 1 0,-3 0-197,17-2 0,-3 1 1,-5 0 196,-15 2 0,-4 1 0,-4 1 0,17 0 0,-5 0 0,-14 1 0,-2 0 666,-4 3 1,0 0-667,1 0 0,-1 0 1133,2 0 0,0 0-1133,1 0 0,-1 0 361,5 0 0,0 0-361,5 0 0,0 0 0,3 0 0,1 0 0,0 0 0,0 0 0,-6 0 0,-1 0 0,-9 0 0,-2 0 0,-6 0 0,-2 0 0,34 0 0,-12 0 0,-9 0 0,-9 0 0,-1 0 0,-6 0 0,-11 4 0,-11 2 0,-16-1 0,-7 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-08-06T20:18:42.040"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.1" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 168 24575,'20'0'0,"8"0"0,11 0 0,17 0 0,21 0 0,-28 0 0,3 0 0,14 0 0,3 0 0,12 0 0,4 0 0,8 0 0,2 0 0,2 0 0,0 0 0,-4 0 0,-2 0 0,-8 0 0,-4 0 0,-6 0 0,-2 0 0,-5 0 0,-1 0 0,-3 0 0,0 0 0,3 0 0,1 0 0,4 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 0,-4 0 0,-1 0 0,-6-2 0,-1 0 0,0-1 0,-1-1 0,-2 0 0,0 0 0,2 0 0,-1 0 0,0 0 0,1 1 0,1 0 0,0 0 0,3-1 0,2 0 0,4 0 0,1 2 0,4-1 0,2 1 0,3 2 0,1-1 0,4-1 0,0 0 0,-2-1 0,-1 0 0,0 0 0,-1 0 0,-2 1 0,1 0 0,-3 2 0,0 0 0,4 0 0,0 0 0,4 0 0,-1 0 0,-1 0 0,-1 0 0,-1 0 0,-1 0 0,-3 0 0,-1 0 0,-6-2 0,0 0 0,2 0 0,1-1 0,3 1 0,2-1 0,4 1 0,2 0 0,8 3 0,2-2 0,3 0 0,1-2 0,3 0 0,2 0 0,-32 1 0,1 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,3 0 0,1 1 0,0-1-144,0 0 1,0 1-1,0-1 144,-1 0 0,1 0 0,0 0 0,-1 1 0,0 0 0,0 0 0,27 1 0,0 0 0,-2 0 0,0 0 0,-4 0 0,0 0 0,-7 0 0,-1 0 0,-4 0 0,0 0 0,-5 0 0,0 0 0,-1 0 0,0 0 0,2 0 0,1 0 0,-2 0 0,0 0 0,-4 0 0,-1 0 215,-4 0 1,-2 0-216,-7 0 0,-1 0 0,-4 0 0,-2 0 0,39 0 0,-9 0 0,1 0 0,5 4 0,-35-1 0,2 2 0,2-1 0,2 1 0,5 1 0,1 0 0,3 1 0,-1-1 0,0-1 0,-1 0 0,0 0 0,-1-1 0,-7-1 0,-3 0 0,41 1 0,-12 3 0,-6 0 0,0 1 0,0 2 0,10-2 0,8-2 0,-41-4 0,1 0 0,3-2 0,-1 0 0,1-1 0,0 2 0,3-1 0,1 0 0,-1 0 0,2 0 0,4 0 0,2 0 0,6 0 0,1 0 0,3 0 0,3 0 0,4-2 0,1-1 0,-3 0 0,-1-1 0,-3-2 0,-1 0 0,-7 0 0,-1-1 0,-4 0 0,0 1 0,-2-1 0,1 1 0,-4 0 0,1 0 0,-1 0 0,0 0 0,-5 2 0,-2 1 0,44-5 0,-6 2 0,-1 2 0,6 1 0,0 3 0,-3 0 0,-7 0 0,-8 0 0,6 0 0,3 0 0,6 0 0,-42 0 0,1 0 0,-2 0 0,-1 0 0,45 0 0,-18 0 0,-16 0 0,-10 0 0,-3 0 0,-8 0 0,-4 0 0,-8 0 0,-4 0 0,7 0 0,4 0 0,13 0 0,13-3 0,12-2 0,8-2 0,-2-1 0,-13 2 0,-16 0 0,-12 3 0,-12 2 0,-3 1 0,-3 0 0,-5 0 0,-6 0 0,-3 0 0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14207,10 +16362,10 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -14228,10 +16383,10 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="6" t="s">
         <v>4</v>
       </c>
@@ -14259,8 +16414,8 @@
       <c r="Q15" s="6"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>22</v>
@@ -14302,8 +16457,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>24</v>
@@ -14345,8 +16500,8 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>23</v>
@@ -14388,8 +16543,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>26</v>
@@ -14431,8 +16586,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
         <v>27</v>
@@ -14474,8 +16629,8 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
@@ -14519,8 +16674,8 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>24</v>
@@ -14562,8 +16717,8 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
         <v>23</v>
@@ -14605,8 +16760,8 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
         <v>25</v>
@@ -14648,8 +16803,8 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
         <v>26</v>
@@ -14691,8 +16846,8 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
         <v>27</v>
@@ -14734,8 +16889,8 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
         <v>27</v>
@@ -14777,8 +16932,8 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
         <v>28</v>
@@ -14820,8 +16975,8 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
         <v>28</v>
@@ -14863,8 +17018,8 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
         <v>22</v>
@@ -14933,12 +17088,12 @@
       <c r="Q32" s="1"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="7" t="s">
         <v>6</v>
       </c>
@@ -14960,10 +17115,10 @@
       <c r="Q33" s="6"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
         <v>52</v>
@@ -15001,10 +17156,10 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
         <v>31</v>
@@ -15592,12 +17747,12 @@
       <c r="Q52" s="1"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53" s="22" t="s">
+      <c r="A53" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
       <c r="E53" s="6" t="s">
         <v>6</v>
       </c>
@@ -15685,103 +17840,103 @@
       <c r="A58" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
       <c r="E58" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F58" s="22" t="s">
+      <c r="F58" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="G58" s="22"/>
+      <c r="G58" s="20"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
       <c r="E59" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F59" s="20" t="s">
+      <c r="F59" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="G59" s="20"/>
+      <c r="G59" s="21"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
       <c r="E60" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F60" s="20" t="s">
+      <c r="F60" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="G60" s="20"/>
+      <c r="G60" s="21"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
       <c r="E61" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F61" s="20" t="s">
+      <c r="F61" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="G61" s="20"/>
+      <c r="G61" s="21"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
       <c r="E62" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F62" s="20" t="s">
+      <c r="F62" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="20"/>
+      <c r="G62" s="21"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
       <c r="E63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F63" s="20" t="s">
+      <c r="F63" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="20"/>
+      <c r="G63" s="21"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -15816,11 +17971,11 @@
       <c r="A67" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B67" s="21" t="s">
+      <c r="B67" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
       <c r="E67" s="8" t="s">
         <v>101</v>
       </c>
@@ -15831,11 +17986,11 @@
       <c r="A68" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
       <c r="E68" s="1" t="s">
         <v>120</v>
       </c>
@@ -15846,11 +18001,11 @@
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
       <c r="E69" s="1" t="s">
         <v>121</v>
       </c>
@@ -15859,11 +18014,11 @@
       <c r="A70" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
       <c r="E70" s="1" t="s">
         <v>122</v>
       </c>
@@ -15872,11 +18027,11 @@
       <c r="A71" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
       <c r="E71" s="1" t="s">
         <v>123</v>
       </c>
@@ -15885,11 +18040,11 @@
       <c r="A72" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
       <c r="E72" s="1" t="s">
         <v>128</v>
       </c>
@@ -16566,13 +18721,24 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
@@ -16587,24 +18753,13 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -16616,7 +18771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F6BEDF-58A8-7846-8BA3-49A7BA2DADCE}">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="125" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -17259,8 +19414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F45CEA-DDAA-4F86-A633-29B993BC7DE7}">
   <dimension ref="S39"/>
   <sheetViews>
-    <sheetView zoomScale="56" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView topLeftCell="A4" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17277,6 +19432,255 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78A8CBD-BA59-4F45-BAA1-C7A4B1A0FDDA}">
+  <dimension ref="A2:C28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="65" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>245</v>
+      </c>
+      <c r="B12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B14" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>251</v>
+      </c>
+      <c r="B15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B18" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B19" t="s">
+        <v>261</v>
+      </c>
+      <c r="C19" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>264</v>
+      </c>
+      <c r="B21" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B22" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>268</v>
+      </c>
+      <c r="B23" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>274</v>
+      </c>
+      <c r="B26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>276</v>
+      </c>
+      <c r="B27" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>278</v>
+      </c>
+      <c r="B28" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA4E5D8-8AD0-4CFD-9333-C4E2BFF55E5C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -17291,7 +19695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC27F950-0B8E-6F4A-BC17-1410D0AF1938}">
   <dimension ref="A1:AF5"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added more bit orders, used for compressed instructions
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklas/riscv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5977816-7E5D-7843-8432-AF60547F39D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7F67A6-D335-3E4D-A5D0-21197050395F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25440" windowHeight="17500" activeTab="3" xr2:uid="{A4EAB723-F944-4B35-B3B4-3FEEB26525D6}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="282">
   <si>
     <t>R-Type</t>
   </si>
@@ -884,6 +884,9 @@
   </si>
   <si>
     <t>4r</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -1038,16 +1041,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -12364,8 +12367,8 @@
       <xdr:row>41</xdr:row>
       <xdr:rowOff>70158</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId44">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="13" name="Ink 12">
@@ -12384,7 +12387,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="13" name="Ink 12">
@@ -12429,8 +12432,8 @@
       <xdr:row>61</xdr:row>
       <xdr:rowOff>98481</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId46">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="16" name="Ink 15">
@@ -12449,7 +12452,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="16" name="Ink 15">
@@ -12494,8 +12497,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>149073</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId48">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="17" name="Ink 16">
@@ -12514,7 +12517,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="17" name="Ink 16">
@@ -15332,7 +15335,7 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 278 24575,'22'0'0,"12"0"0,16 0 0,25 0 0,20 0 0,-40 0 0,1 0 0,5 0 0,1 0 0,3 0 0,1 0 0,5 0 0,2 0 0,4 0 0,-1 0 0,1 0 0,1 0 0,3 0 0,0 0 0,-3 0 0,-2 0 0,-2 0 0,0 0 0,-1 0 0,-2 0 0,-5 1 0,-1 2 0,-1 1 0,-2 1 0,-3 1 0,0 0 0,-3 1 0,0-1 0,3-2 0,-1 0 0,1 0 0,1-1 0,1 1 0,2 0 0,3 0 0,0 0 0,1 0 0,1 0 0,5-2 0,1 0 0,-1-2 0,0 1 0,-1 1 0,-1 0 0,-3 2 0,-2 1 0,-5 1 0,0 1 0,-2 0 0,0 2 0,-2-1 0,0-1 0,3 0 0,1 0 0,0-1 0,2 0 0,3 0 0,0 0 0,3 0 0,1-1 0,4 0 0,0-1 0,4-2 0,2-1 0,3 1 0,2-2 0,5 0 0,3 0 0,-28 0 0,2 0 0,0 0-186,5 0 1,0 0 0,1 0 185,2 0 0,0 0 0,0 0 0,-1 0 0,2 0 0,-3 0 0,-3 0 0,-1 0 0,-1 0 0,25 0 0,-3 0 0,-7 0 0,-4 0 0,-6 0 0,-4 0 0,-8 0 0,-2 0 0,-4 0 0,0 0 0,-1 0 0,-2 0 0,0 0 0,2 0 278,4 0 0,1 0-278,-2 0 0,-1 0 0,-5 1 0,-1 1 0,31 1 0,-26 2 0,-12 1 0,-7-3 0,7 3 0,15-2 0,11 0 0,12-1 0,14-3 0,-39 0 0,4 0 0,10 0 0,3 0 0,8 0 0,1-1 0,7-4 0,2-2 0,2-3 0,0-3 0,0-2 0,2-3 0,-28 5 0,0-1 0,1-1-215,2 0 0,2 0 0,0-2 215,3 1 0,1-1 0,1-1 0,4 1 0,0-3 0,-1 1 0,-4 0 0,0 1 0,-2 0 0,-5 1 0,-2 1 0,-2 1 0,24-5 0,-4 0 0,-12 5 0,-2 1 0,-6 2 0,-1 1 0,-7 3 0,-1 2 0,-5 0 0,-2 0 0,43-1 645,-5 0-645,-2-1 0,-3 3 0,-6 2 0,-13 3 0,-12 0 0,-9 0 0,0 0 0,8 0 0,11 0 0,14 0 0,1 0 0,-2 0 0,1 0 0,7 0 0,12 0 0,-42 0 0,1 0 0,-1 0 0,0 0 0,47 0 0,-3 0 0,-2 0 0,-42 0 0,3 0 0,5 0 0,2 0 0,6 0 0,2 0 0,8 0 0,2 0 0,5 0 0,2 2 0,5 3 0,-1 2 0,1 1 0,0 1 0,-3 3 0,-3 0 0,-10 1 0,-4 0 0,-12-3 0,-4-1 0,27 8 0,-25-7 0,-4-4 0,19 4 0,25-2 0,-38-3 0,2-2 0,3 0 0,1-1 0,-2-2 0,-1 1 0,-6-1 0,-1 0 0,39 0 0,-12 0 0,-17 0 0,-11 0 0,-2 0 0,-3 0 0,5 0 0,5 0 0,-5 0 0,0 0 0,-7 0 0,-3 0 0,4 0 0,1-1 0,-2-1 0,-11-2 0,-11 1 0,-8-1 0,-2 1 0,0 1 0,-8 0 0,-2 2 0,-7-2 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 269 24575,'22'0'0,"12"0"0,16 0 0,25 0 0,20 0 0,-40 0 0,1 0 0,5 0 0,1 0 0,2 0 0,2 0 0,5 0 0,2 0 0,4 0 0,-1 0 0,1 0 0,1 0 0,3 0 0,0 0 0,-3 0 0,-2 0 0,-2 0 0,0 0 0,-1 0 0,-3 0 0,-4 1 0,-1 2 0,-1 1 0,-2 1 0,-3 1 0,0 0 0,-3 0 0,0 0 0,3-2 0,-1 0 0,1 0 0,1-1 0,1 1 0,2 0 0,3-1 0,0 1 0,1 0 0,1 0 0,4-2 0,2 0 0,-1-2 0,0 1 0,-1 1 0,-1 0 0,-3 2 0,-2 0 0,-5 2 0,0 1 0,-2 0 0,0 2 0,-2-2 0,0 0 0,3 0 0,1 0 0,0-1 0,1-1 0,4 1 0,0 0 0,3 0 0,1-1 0,4-1 0,0 0 0,4-2 0,2-1 0,3 1 0,2-2 0,5 0 0,3 0 0,-28 0 0,2 0 0,-1 0-186,6 0 1,0 0 0,1 0 185,2 0 0,0 0 0,0 0 0,-1 0 0,2 0 0,-3 0 0,-3 0 0,-1 0 0,-1 0 0,25 0 0,-3 0 0,-8 0 0,-3 0 0,-6 0 0,-4 0 0,-8 0 0,-2 0 0,-4 0 0,0 0 0,-1 0 0,-2 0 0,0 0 0,2 0 278,4 0 0,1 0-278,-2 0 0,-1 0 0,-5 1 0,-1 1 0,31 1 0,-27 2 0,-11 1 0,-7-3 0,7 2 0,15-1 0,11 0 0,12-1 0,14-3 0,-39 0 0,4 0 0,10 0 0,3 0 0,8 0 0,1-1 0,7-4 0,2-2 0,1-2 0,1-4 0,0-1 0,2-4 0,-28 6 0,0-2 0,1-1-215,2 1 0,2-1 0,0-1 215,3 0 0,1 0 0,1-2 0,4 2 0,0-3 0,-2 0 0,-3 1 0,0 0 0,-2 1 0,-5 0 0,-2 2 0,-2 0 0,24-4 0,-4 0 0,-12 4 0,-2 2 0,-6 1 0,-1 1 0,-7 4 0,-1 1 0,-5 0 0,-3 0 0,44-1 645,-5 1-645,-2-2 0,-3 3 0,-6 2 0,-13 3 0,-12 0 0,-9 0 0,0 0 0,8 0 0,11 0 0,14 0 0,1 0 0,-2 0 0,1 0 0,6 0 0,13 0 0,-42 0 0,1 0 0,-1 0 0,0 0 0,47 0 0,-3 0 0,-2 0 0,-42 0 0,3 0 0,5 0 0,2 0 0,6 0 0,2 0 0,8 0 0,2 0 0,4 0 0,3 2 0,5 3 0,-1 2 0,1 0 0,0 2 0,-3 3 0,-3-1 0,-10 2 0,-4-1 0,-12-2 0,-4-1 0,27 7 0,-25-6 0,-5-4 0,20 4 0,25-3 0,-38-2 0,2-2 0,3 0 0,1-1 0,-2-2 0,-1 1 0,-6-1 0,-1 0 0,39 0 0,-12 0 0,-17 0 0,-11 0 0,-2 0 0,-3 0 0,4 0 0,6 0 0,-5 0 0,0 0 0,-7 0 0,-3 0 0,4 0 0,1-1 0,-2-1 0,-11-2 0,-11 1 0,-8-1 0,-2 1 0,0 1 0,-8 1 0,-2 1 0,-7-2 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15359,7 +15362,7 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 178 24575,'60'0'0,"9"0"0,28 0 0,-41-1 0,2 2 0,10 1 0,2 2 0,8 2 0,3 2 0,4 2 0,2 2 0,6 1 0,3-2 0,1-1 0,0-1 0,-30-4 0,2 0 0,-2 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,2-1 0,-2 1 0,3-1 0,0 1 0,1 1-235,2-1 0,-1 0 0,1 0 235,1-1 0,0-1 0,0 0 0,0 1 0,-2-2 0,0 1 0,-4-1 0,-2-1 0,0 0 87,23-1 0,-3 0-87,-11 1 0,-3 0 0,-7 1 0,-2 0 0,-6 0 0,-1 0 0,1 2 0,1-1 0,6 0 0,0 0 265,5 1 1,0 0-266,6 0 0,3 0 0,2-1 0,0-1 0,-1 1 0,-1-2 0,1 0 0,-2-1 0,-5 1 0,0-2 0,-2 1 0,0 0 0,-1 0 0,0 0 0,3 0 0,1 0 0,6 0 0,4 0 0,6 0 0,1 0 0,4 0 0,0 0 0,0 0 0,-3 0 0,-8 0 0,-2 0 0,-13 0 0,-3 0 0,-8 0 0,-3 0 0,38 0 0,6 0 0,-42 0 0,1 0 0,7 0 0,1 0 0,5 0 0,0 0 0,0 0 0,-2 0 0,-2 1 0,0-2 0,-3 1 0,-1-1 0,-3-3 0,0-1 0,3-2 0,2-1 0,6-3 0,2-2 0,6 0 0,3-1 0,6 1 0,2 2 0,-2-2 0,0 1 0,1 0 0,2 0 0,-1 0 0,0-1 0,2-3 0,2 0 0,-2 1 0,0-1 0,-2 1 0,0-2 0,-2 2 0,-1 1 0,-3 3 0,-3-1 0,-3 1 0,-3 0 0,-4 1 0,-2 2 0,-7 1 0,-1 1 0,-5 0 0,-3 2 0,45-1 0,-15 4 0,-6 1 0,-1 0 0,0 0 0,10 0 0,-34 0 0,1 0 0,7 0 0,1 0 0,11 0 0,4 0 0,6 0 0,2 0 0,0 0 0,0 0 0,1 0 0,0 0 0,-5 0 0,-1 0 0,-2 0 0,1 0 0,3 0 0,2 0 0,-1 0 0,1-1 0,2-1 0,1 0 0,-3-1 0,-1 1 0,-5 0 0,0-1 0,-5 1 0,-3 1 0,-6 1 0,-1 0 0,-3 0 0,-1 0 0,-5 0 0,0 0 0,44 0 0,0 2 0,-46 1 0,0 3 0,7 1 0,1 1 0,8 1 0,2 3 0,8 2 0,2 0 0,8-1 0,0 0 0,0-1 0,-1 2 0,-4-1 0,-3 0 0,-8-2 0,-3 1 0,-10 0 0,-4 0 0,36 7 0,-19-4 0,-11-6 0,6-5 0,18-1 0,-31-3 0,2 0 0,7-1 0,2 2 0,2 0 0,0 1 0,2 0 0,-2 1 0,-4 0 0,-2 1 0,-5 1 0,-1-1 0,37 0 0,-27-1 0,-16-2 0,-14-1 0,1 0 0,3 0 0,5 0 0,8 0 0,10 0 0,10 0 0,6 0 0,3 0 0,-4 0 0,-4 0 0,-8 0 0,-10 0 0,-6 0 0,-6 0 0,-1 0 0,1 0 0,2 0 0,5 0 0,-2 0 0,0 0 0,-3 0 0,-4 0 0,4 0 0,3 0 0,4 0 0,-3 0 0,-4 0 0,-3 0 0,2 0 0,2 0 0,1 0 0,3 0 0,2 2 0,-3 2 0,-1-1 0,-11-1 0,-4-2 0,-5 0 0,-6 0 0,0 0 0,-4 0 0,-4-19 0,-5 14 0,-4-13 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 171 24575,'60'0'0,"9"0"0,28 0 0,-41-1 0,2 2 0,10 1 0,2 2 0,8 2 0,2 1 0,5 3 0,2 1 0,6 2 0,3-2 0,1-2 0,0 0 0,-30-4 0,2-1 0,-2 1 0,0 0 0,1 0 0,-1 0 0,0-1 0,2 0 0,-2 1 0,2-1 0,1 1 0,1 0-235,2 0 0,-1 0 0,1 0 235,1-1 0,0-1 0,0-1 0,0 2 0,-2-2 0,0 1 0,-4-1 0,-2-1 0,0 0 87,23-1 0,-3 0-87,-12 1 0,-2 0 0,-7 1 0,-2 0 0,-6 0 0,-1 0 0,1 1 0,1 0 0,6 0 0,0 0 265,5 1 1,0 0-266,6 0 0,3-1 0,2 0 0,0-1 0,-1 1 0,-1-2 0,0 0 0,-1-1 0,-5 1 0,0-2 0,-2 1 0,0 0 0,-1 0 0,0 0 0,3 0 0,1 0 0,6 0 0,4 0 0,6 0 0,1 0 0,4 0 0,0 0 0,-1 0 0,-2 0 0,-8 0 0,-2 0 0,-13 0 0,-3 0 0,-8 0 0,-3 0 0,38 0 0,6 0 0,-42 0 0,1 0 0,7 0 0,1 0 0,5 0 0,0 0 0,0 0 0,-3 0 0,-1 1 0,0-2 0,-3 1 0,-1-1 0,-3-3 0,0-1 0,3-1 0,2-2 0,6-3 0,2-1 0,6-1 0,3 0 0,6 1 0,2 1 0,-2-2 0,0 2 0,0-1 0,3 1 0,-1-1 0,0 0 0,2-4 0,2 1 0,-2 1 0,0-2 0,-2 2 0,0-2 0,-2 1 0,-1 2 0,-3 2 0,-3 0 0,-3 0 0,-4 0 0,-3 2 0,-2 1 0,-7 1 0,-1 2 0,-5-1 0,-3 2 0,45-1 0,-15 4 0,-6 1 0,-1 0 0,0 0 0,10 0 0,-34 0 0,1 0 0,7 0 0,1 0 0,11 0 0,3 0 0,7 0 0,2 0 0,0 0 0,0 0 0,1 0 0,0 0 0,-5 0 0,-1 0 0,-2 0 0,1 0 0,3 0 0,2 0 0,-1 0 0,1-1 0,1-1 0,2 0 0,-3 0 0,-1 0 0,-5 0 0,0-1 0,-5 1 0,-3 1 0,-6 1 0,-1 0 0,-3 0 0,-1 0 0,-5 0 0,0 0 0,44 0 0,0 2 0,-46 1 0,0 3 0,6 0 0,2 2 0,8 1 0,2 2 0,8 3 0,2-1 0,8 0 0,0-1 0,0 0 0,-1 1 0,-4 0 0,-3-1 0,-8-1 0,-3 0 0,-10 1 0,-4-1 0,36 7 0,-20-3 0,-10-6 0,6-6 0,18 0 0,-31-3 0,2 0 0,7-1 0,2 2 0,2 0 0,0 1 0,2 0 0,-2 1 0,-4 0 0,-2 1 0,-5 0 0,-1 0 0,37 0 0,-27-1 0,-16-2 0,-14-1 0,1 0 0,2 0 0,6 0 0,8 0 0,10 0 0,10 0 0,6 0 0,3 0 0,-4 0 0,-4 0 0,-8 0 0,-10 0 0,-6 0 0,-6 0 0,-1 0 0,1 0 0,2 0 0,5 0 0,-2 0 0,0 0 0,-3 0 0,-4 0 0,4 0 0,3 0 0,4 0 0,-4 0 0,-3 0 0,-3 0 0,2 0 0,2 0 0,1 0 0,3 0 0,2 2 0,-3 2 0,-1-1 0,-11-1 0,-4-2 0,-5 0 0,-6 0 0,0 0 0,-4 0 0,-4-19 0,-5 15 0,-4-14 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15413,7 +15416,7 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 275 24575,'38'-4'0,"14"0"0,29 4 0,-31 0 0,1 0 0,5 0 0,0 0 0,0 0 0,-2 0 0,0 0 0,-3 0 0,46 0 0,1 0 0,-47 0 0,1 0 0,2 1 0,1-1 0,7 2 0,4 1 0,9 1 0,5 0 0,15 1 0,5 1-325,-24-2 0,3 0 0,0-2 325,6 0 0,2 0 0,-1 0 0,-1 0 0,-2-1 0,-2 0-36,-6-1 1,-1 0-1,-4 0 36,22 0 0,-3 0 0,-8 0 0,1 0 0,13 0 0,3 0-284,-26 0 1,3 0 0,1 0 283,7 0 0,3 0 0,2 0 0,0 0 0,1 0 0,0 0 0,-6 0 0,0 0 0,-1 0 0,4 0 0,0 0 0,1 0 0,3 0 0,0 0 0,2 0-410,5 0 1,0 0 0,1 0 409,-23 0 0,1 0 0,0 0 0,-2 0 0,23 0 0,0 0 0,-4 0 134,-8 0 0,-2 0 0,-2 0-134,-9 0 0,-2 0 0,-3 0 49,22 0 0,-2 0-49,-3 0 0,0 0 0,1 0 0,4 0 0,7-2 0,4 0 35,-26-1 0,3-1 0,1 1-35,-2-2 0,1-1 0,-1 0 0,3-1 0,-2 0 0,1-1 0,-2-1 0,1 0 0,-1 0 0,-4-1 0,-1 1 0,0-1 0,0 2 0,1 2 0,-1-2 376,-2 1 0,-1-1 0,-1 2-376,25 0 0,-3 1 249,-10 0 0,-3 0-249,-8 0 0,-2-2 0,-7 1 0,0-1 0,3 1 0,1 0 388,6 0 1,4 0-389,1 0 0,1 1 76,4 0 0,2 0-76,-4-1 0,0 0 0,-4 0 0,0 1 0,1 1 0,-1-1 0,1 0 0,0 0 0,6 0 0,2 1 0,0-1 0,-1 1 0,0 1 0,-1 1 0,-8 0 0,-3 1 0,-8 1 0,-1 0 0,-2 0 0,1 0 0,3 0 0,1 0 0,6 0 0,2 0 0,2 0 0,1 0 0,-5 0 0,-4 0 0,-10 0 0,-3 0 0,32 0 0,-12 0 0,1 0 0,15 0 0,-37 1 0,0 1 0,8 1 0,0 2 0,5 1 0,0 1 0,2 0 0,2 2 0,1 0 0,0 1 0,0-1 0,-1 0 0,-4-1 0,0 1 0,-8-1 0,-1 0 0,38 8 0,-22-2 0,-10-1 0,-12-3 0,0-1 0,16 1 0,19 0 0,-34-2 0,2 2 0,1-1 0,-1 1 0,-2 0 0,-2-2 0,38 7 0,-11-5 0,-8 0 0,-8-3 0,-6 0 0,-4-2 0,-5-2 0,1 0 0,8 3 0,10-2 0,18 0 0,17-1 0,-44-2 0,2-2 0,1 1 0,0 0 0,-1 0 0,-1 0 0,-2 0 0,-1 0 0,46 0 0,-9 0 0,-8 0 0,-12 0 0,-4 0 0,-1 0 0,6 0 0,9 0 0,5 0 0,13 0 0,-42 0 0,2 0 0,5 1 0,2-2 0,0 0 0,0-1 0,-10-1 0,-4 0 0,24-5 0,-26 0 0,-11-1 0,0 0 0,10-2 0,3 1 0,0 2 0,3 0 0,-2 0 0,3 2 0,1 3 0,-8 3 0,-7-2 0,-11-1 0,-9 1 0,-6-1 0,-4 1 0,-3-1 0,1 0 0,-1 1 0,0-1 0,-2-1 0,-2-3 0,-1-6 0,-3-7 0,-10-10-1696,-10-9 0,6 17 0,-2 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 262 24575,'38'-4'0,"14"0"0,29 4 0,-31 0 0,1 0 0,5 0 0,0 0 0,0 0 0,-2 0 0,0 0 0,-4 0 0,47 0 0,1 0 0,-47 0 0,1 0 0,2 1 0,1-1 0,7 2 0,4 1 0,9 0 0,5 1 0,15 1 0,5 1-325,-24-2 0,3-1 0,0-1 325,5 0 0,3 0 0,-1 0 0,-1 0 0,-2-1 0,-2 0-36,-6-1 1,-1 0-1,-4 0 36,22 0 0,-3 0 0,-8 0 0,1 0 0,13 0 0,3 0-284,-27 0 1,4 0 0,1 0 283,7 0 0,3 0 0,2 0 0,0 0 0,1 0 0,0 0 0,-6 0 0,0 0 0,-1 0 0,4 0 0,0 0 0,0 0 0,4 0 0,0 0 0,2 0-410,5 0 1,0 0 0,1 0 409,-23 0 0,1 0 0,0 0 0,-2 0 0,23 0 0,0 0 0,-5 0 134,-7 0 0,-2 0 0,-2 0-134,-9 0 0,-2 0 0,-3 0 49,22 0 0,-2 0-49,-3 0 0,0 0 0,1 0 0,4 0 0,7-2 0,4 0 35,-27-1 0,4-1 0,1 1-35,-2-1 0,1-2 0,-1 0 0,3 0 0,-2-1 0,1-1 0,-2 0 0,1-1 0,-1 1 0,-4-2 0,-1 2 0,0-2 0,-1 2 0,2 3 0,-1-3 376,-2 2 0,-1-2 0,-1 2-376,25 0 0,-3 2 249,-10-1 0,-3 0-249,-8 0 0,-2-1 0,-7 0 0,0-1 0,3 2 0,1-1 388,6 0 1,3 1-389,2-1 0,1 1 76,4 0 0,2 1-76,-4-2 0,0 0 0,-4 1 0,0 0 0,1 1 0,-1-1 0,1 0 0,0 1 0,6-1 0,2 1 0,0-1 0,-2 2 0,1 0 0,-1 1 0,-8 0 0,-3 1 0,-8 1 0,-1 0 0,-2 0 0,1 0 0,3 0 0,1 0 0,6 0 0,2 0 0,2 0 0,1 0 0,-5 0 0,-4 0 0,-10 0 0,-4 0 0,33 0 0,-12 0 0,1 0 0,15 0 0,-37 1 0,0 1 0,8 1 0,0 1 0,5 2 0,0 1 0,2-1 0,2 3 0,1 0 0,0 0 0,0 0 0,-1-1 0,-4 0 0,-1 0 0,-7 0 0,-1 0 0,38 7 0,-22-2 0,-10-1 0,-12-2 0,0-1 0,16 0 0,19 1 0,-34-3 0,2 3 0,1-2 0,-1 2 0,-2-1 0,-2-1 0,38 6 0,-11-4 0,-8-1 0,-9-2 0,-5-1 0,-4-1 0,-5-2 0,1 0 0,8 3 0,10-3 0,18 1 0,17-1 0,-44-2 0,2-2 0,1 1 0,0 0 0,-1 0 0,-1 0 0,-2 0 0,-1 0 0,46 0 0,-9 0 0,-9 0 0,-11 0 0,-4 0 0,-1 0 0,6 0 0,9 0 0,5 0 0,13 0 0,-42 0 0,2 0 0,5 1 0,2-2 0,0 0 0,0-1 0,-10-1 0,-4 1 0,24-6 0,-26 0 0,-11 0 0,-1-1 0,11-1 0,3 0 0,0 3 0,3-1 0,-2 0 0,3 3 0,1 2 0,-8 3 0,-7-2 0,-11-1 0,-9 1 0,-6-1 0,-4 1 0,-3 0 0,1-1 0,-1 1 0,0-1 0,-2-1 0,-2-2 0,-1-7 0,-3-6 0,-10-9-1696,-10-9 0,6 16 0,-2 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15440,7 +15443,7 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 477 24575,'83'-4'0,"-20"2"0,9 1 0,23 0 0,8 2 0,-26-1 0,5 0 0,0 0 0,13 0 0,4 0 0,3 0-1141,-16 0 0,3 0 0,1 0 0,2 0 1141,-14 0 0,2 0 0,0 0 0,2 0 0,0 0 0,4 0 0,2 0 0,0 0 0,0 0 0,-2 0 0,15 0 0,-2 0 0,0 0 0,-4 0 95,-12 0 1,-2-1-1,-1 1 1,-5 1-96,10-1 0,-3 2 0,-5 0 478,13 3 1,-5 2-479,-5 2 0,0 2 0,9 4 0,2 0-347,-18-4 1,3 0 0,3-3 346,16 2 0,4-2 0,3-1-70,-16-2 1,1-1 0,3 0 0,2-1 69,-7-1 0,3 0 0,1-1 0,1-1 0,3 1-487,-5 0 0,1-1 0,2 1 0,1-1 0,2-1 1,1 0 486,-5-1 0,1 0 0,2 0 0,0-1 0,2-1 0,0 0 0,2-1-452,-6 0 0,2-1 0,1-1 0,1 0 0,0 1 0,1-3 0,0 1 0,0-2 452,-9 1 0,1-1 0,0-1 0,2 0 0,-1 0 0,-1-1 0,0 1 0,0-1 0,-1 0 0,5-1 0,1-1 0,-1-1 0,0 1 0,-2-1 0,0 1 0,0 0 0,-3 0-141,4-1 0,-2 0 0,1 0 0,-2 1 0,-2 0 0,-1 1 1,-1-1 140,15-1 0,-1-1 0,-3 2 0,-2 0 0,-2 2 100,6 0 0,-3 1 0,-1 1 0,-1 0-100,-5 0 0,0 1 0,-1 0 0,0 0 0,-2 1 0,-1 1 0,0 1 0,0-1 0,-3 1 0,0 1 0,-1-1 0,1 2 442,-1 0 1,0 0 0,0 1-1,-2 0-442,22 1 0,-3 0 0,-3 0 0,-6 2 0,-2 0 0,-2 0 1252,-3 0 0,-2 0 0,-1 0-1252,-9 0 0,-3 0 0,1 0 0,31 0 0,1 0 0,-2 0 0,0 0 0,-1 0 0,-1 0 0,-2 3 0,-3 2 1354,-9 1 1,-3 1-1355,-12 1 0,-3 1 867,-11-1 0,-2-1-867,42 3 627,-35-4 1,3 0-628,20 2 0,7-1 0,-18 0 0,5 0 0,0 0-49,4 0 1,2-1 0,-1-1 48,0 1 0,0 0 0,-4 0 0,23 1 0,-4 0 0,-17-2 0,-4 0 0,-12 0 0,-4-1 0,40-1 0,-47-3 0,1 0 0,3 0 0,0 0 0,2 0 0,-1 0 585,45 0-585,-20 3 0,-16 0 0,-12 2 0,0 3 0,9 0 0,-1 2 0,-7 0 0,-13-2 0,-12 0 0,-3-1 0,3 0 0,3 4 0,2 0 0,-1 2 0,-1-3 0,3 1 0,4 0 0,7-2 0,14 0 0,22 2 0,-31-7 0,2 0 0,5 1 0,1-1 0,-1-2 0,-1-1 0,39-1 0,-12 0 0,-20 0 0,-15 0 0,-13 0 0,-14 0 0,-10 0 0,-13-4-1696,-12-7 0,5 5 0,-3-4 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 465 24575,'83'-4'0,"-20"2"0,9 1 0,23 0 0,8 2 0,-26-1 0,5 0 0,-1 0 0,14 0 0,4 0 0,3 0-1141,-16 0 0,3 0 0,1 0 0,2 0 1141,-14 0 0,2 0 0,0 0 0,2 0 0,0 0 0,4 0 0,1 0 0,1 0 0,0 0 0,-2 0 0,15 0 0,-2 0 0,0 0 0,-4 0 95,-12 0 1,-2-1-1,-1 1 1,-5 1-96,10-1 0,-4 2 0,-4 0 478,13 3 1,-5 1-479,-5 3 0,0 2 0,9 3 0,2 1-347,-18-4 1,3 0 0,3-4 346,16 3 0,4-2 0,3-1-70,-17-2 1,2-2 0,3 1 0,2-1 69,-7-1 0,3 0 0,1-1 0,1-1 0,3 1-487,-5 0 0,1-1 0,2 1 0,1-1 0,2-1 1,0 0 486,-4-1 0,1 0 0,2 0 0,0-1 0,2-1 0,0 1 0,2-2-452,-6 0 0,2-1 0,1-1 0,1 0 0,0 1 0,0-2 0,1 0 0,0-2 452,-9 1 0,1 0 0,0-2 0,2 0 0,-1 1 0,-1-2 0,0 1 0,0-1 0,-1 1 0,5-2 0,0-1 0,0 0 0,0 0 0,-2 0 0,0 0 0,0 0 0,-3 1-141,4-2 0,-2 0 0,1 1 0,-2 0 0,-2 1 0,-1 0 1,-1-1 140,14 0 0,0-2 0,-3 2 0,-2 1 0,-2 1 100,6 0 0,-3 2 0,-1 0 0,-1 0-100,-5 1 0,0 0 0,-1 0 0,0 0 0,-3 1 0,0 2 0,0 0 0,0-1 0,-3 1 0,0 1 0,-1-1 0,1 2 442,-1 1 1,0-1 0,0 1-1,-2 0-442,22 1 0,-3 0 0,-4 0 0,-5 2 0,-2 0 0,-2 0 1252,-3 0 0,-2 0 0,-1 0-1252,-9 0 0,-3 0 0,1 0 0,31 0 0,1 0 0,-2 0 0,0 0 0,-1 0 0,-2 0 0,-1 3 0,-3 2 1354,-9 1 1,-3 0-1355,-12 2 0,-3 1 867,-11-1 0,-2-1-867,42 2 627,-35-3 1,3 0-628,20 2 0,7-1 0,-18-1 0,5 1 0,-1 0-49,5 0 1,2-1 0,-1-1 48,0 0 0,0 1 0,-4 0 0,23 1 0,-4 0 0,-17-2 0,-4 0 0,-12-1 0,-4 0 0,40-1 0,-47-3 0,1 0 0,3 0 0,-1 0 0,3 0 0,-1 0 585,45 0-585,-20 3 0,-16 0 0,-12 2 0,0 3 0,9 0 0,-1 1 0,-7 1 0,-13-2 0,-12 0 0,-3-2 0,3 1 0,3 4 0,2 0 0,-1 1 0,-1-2 0,3 1 0,4-1 0,7-1 0,14 0 0,22 2 0,-31-7 0,1 0 0,6 0 0,1 0 0,-1-2 0,-1-1 0,39-1 0,-12 0 0,-20 0 0,-15 0 0,-13 0 0,-14 0 0,-10 0 0,-13-4-1696,-12-6 0,5 4 0,-3-4 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15467,7 +15470,7 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 199 24575,'63'-4'0,"-17"2"0,7 1 0,29 0 0,8 2 0,-16-1 0,4 0 0,3 0 0,4 0 0,3 0 0,2 0-541,-14 0 1,1 0 0,2 0 0,-1 0 540,0 0 0,2 0 0,-1 0 0,1 0 0,4 0 0,1 0 0,0 0 0,1 0 0,4 0 0,2 0 0,-1 0 0,-2 0 0,-8 0 0,0 0 0,-3 0 0,1 0 0,-3-1 0,1 1 0,0 0 0,-3 1-98,18 0 0,-2 1 1,-1 0 97,-6 2 0,-2 0 0,0 0 0,-2 0 0,-1 1 0,-1 0-78,-8 0 1,-1 1 0,1 0 77,28-1 0,-1 1 0,-5-1 0,-1 0 0,0 1 0,0-2 0,0 0 0,-1-2 0,-3 1 0,-1-1 0,0 1 0,1-1 0,2 1 0,-1 0 0,-1 0 0,1 0 0,-4 1 0,1 1 0,-2-2 0,2-1 0,-2 1 0,0 0 0,6-1 0,3-1 0,3-1 0,1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,-1 0 0,-1 0 0,0 0 0,1 0 0,-24 0 0,2 0 0,0 0-256,8 0 1,1 0 0,2 0 255,1 0 0,1 0 0,0 0 0,5 0 0,-1 0 0,0 0 0,-3 0 0,1 0 0,-1 0 0,3 0 0,0 0 0,3 0 36,5 0 1,1 0 0,1 0-37,-20 0 0,-1 0 0,1 0 0,0 0 0,3 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-2 0 0,1 0 0,-1 0 0,-3 0 0,2 0 0,-2 0 0,-2 0 0,20-1 0,-1-1 0,-3-1-38,-3 0 0,-2-1 0,2-1 38,-1 0 0,-1-1 0,1-1 0,1 1 0,-1-1 0,1 1 0,2 1 0,1 1 0,0 0 0,2 0 0,0 0 0,1 1 0,-5-1 0,-1 0 0,0 0 0,-2-2 0,-2 1 0,-1-2 38,-9 2 1,-1-1 0,-3 0-39,19-1 0,-5 0 386,-10 0 0,-1 0-386,-8 2 0,1-1 718,3 0 0,1-2-718,11 0 0,2 2 0,3-3 0,1 0 0,3-2 0,-1 0 503,-7 3 0,-3-2-503,-12 1 0,-4 0 63,-11 2 0,-3 1-63,28-4 0,-7 4 0,7-1 0,7 0 0,3 2 0,-2 1 0,-11 4 0,-12 0 0,-4 0 0,-3 0 0,5 0 0,7 0 0,4 0 0,0 0 0,-8 0 0,-10 0 0,-5 0 0,3 0 0,16 0 0,18 0 0,10 0 0,-1 0 0,-10 0 0,-18 0 0,-11 0 0,-6 0 0,0 0 0,6 0 0,1 0 0,0 0 0,-6 0 0,-4 0 0,0 0 0,2 0 0,9 0 0,7 0 0,6 1 0,-5 1 0,-11 2 0,-13 2 0,-12 1 0,-6-1 0,-5-2 0,-4 0 0,-2-1 0,-3 0 0,-2-2 0,0 1 0,0 0 0,1-2 0,4 0 0,2 0 0,2 0 0,0 2 0,-1 0 0,-4-1 0,-9-10 0,-1 5 0,-5-6 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 189 24575,'63'-4'0,"-17"2"0,7 2 0,29-1 0,8 2 0,-16-1 0,4 0 0,3 0 0,3 0 0,4 0 0,2 0-541,-14 0 1,1 0 0,2 0 0,-1 0 540,0 0 0,2 0 0,-1 0 0,1 0 0,4 0 0,1 0 0,0 0 0,0 0 0,5 0 0,2 0 0,-1 0 0,-2 0 0,-8 0 0,0 0 0,-3 0 0,1 0 0,-3-1 0,1 1 0,0 0 0,-3 1-98,18-1 0,-3 2 1,0 0 97,-6 2 0,-2 0 0,0 0 0,-2-1 0,-1 2 0,-1 0-78,-8 0 1,-1 0 0,1 1 77,28-1 0,-1 1 0,-5-2 0,-1 1 0,-1 1 0,1-2 0,0-1 0,-1-1 0,-3 1 0,-1-1 0,0 1 0,1-1 0,2 1 0,-1-1 0,-1 1 0,1 0 0,-4 1 0,0 1 0,-1-2 0,2-2 0,-2 2 0,0 0 0,6-1 0,3-1 0,3-1 0,1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,-2 0 0,0 0 0,0 0 0,1 0 0,-24 0 0,2 0 0,0 0-256,8 0 1,1 0 0,2 0 255,1 0 0,1 0 0,0 0 0,5 0 0,-2 0 0,1 0 0,-3 0 0,1 0 0,-1 0 0,3 0 0,0 0 0,3 0 36,5 0 1,1 0 0,1 0-37,-20 0 0,-1 0 0,1 0 0,-1 0 0,4 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-2 0 0,1 0 0,-1 0 0,-3 0 0,2 0 0,-2 0 0,-2 0 0,20-1 0,-2-1 0,-2-1-38,-3 0 0,-2 0 0,2-2 38,-1 0 0,-1-1 0,1 0 0,1 0 0,-1-1 0,1 2 0,2 0 0,1 1 0,-1 0 0,3 1 0,0-1 0,1 1 0,-5-1 0,-1 0 0,0 1 0,-2-3 0,-2 1 0,-1-2 38,-9 3 1,-1-2 0,-3 0-39,19 0 0,-6-1 386,-9 0 0,-1 1-386,-8 1 0,1-1 718,3 1 0,1-3-718,11 0 0,2 3 0,3-4 0,1 1 0,3-3 0,-1 1 503,-7 2 0,-3-1-503,-12 0 0,-5 0 63,-10 3 0,-3 0-63,28-3 0,-7 3 0,7-1 0,7 1 0,3 1 0,-2 1 0,-11 4 0,-12 0 0,-4 0 0,-3 0 0,5 0 0,7 0 0,4 0 0,0 0 0,-9 0 0,-9 0 0,-5 0 0,3 0 0,16 0 0,18 0 0,10 0 0,-1 0 0,-10 0 0,-18 0 0,-11 0 0,-6 0 0,0 0 0,6 0 0,1 0 0,0 0 0,-6 0 0,-4 0 0,0 0 0,1 0 0,10 0 0,7 0 0,6 1 0,-5 1 0,-11 2 0,-13 1 0,-12 2 0,-6-1 0,-5-2 0,-4-1 0,-2 0 0,-3 0 0,-2-2 0,0 1 0,0 0 0,1-2 0,4 0 0,2 0 0,2 0 0,0 2 0,-1 0 0,-4-1 0,-9-10 0,-1 5 0,-5-5 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15494,7 +15497,7 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 284 24575,'46'-4'0,"33"1"0,-17 3 0,6 0 0,-1 0 0,5 0 0,3 0 0,6 0 0,3 0 0,0 0 0,5 0 0,1 0 0,3 0-708,-16 0 0,2 0 0,0 0 1,-2 0 707,19 0 0,-3 0 0,1 0 0,-19 0 0,2 0 0,-1 0 0,0 0 0,-1 0 0,0 0 0,1 0 0,-3 0 0,15 0 0,-2 0 0,0 0 147,-3 1 0,-1-1 0,-3 1-147,23 1 0,-6 1 285,-18 1 0,-5 1-285,-11 0 0,-2 1 0,3 0 0,0-2 0,8 0 0,4-2 0,13 0 0,5 0 0,-26-2 0,1 0 0,-1 0 0,34 0 0,-3 0 0,-5 0 0,-1 0 0,-6 0 0,-2 0 0,-3 0 0,1 0 0,8 0 0,3 0 0,-27 0 0,1 0 0,1 0 294,3 0 0,3 0 0,-1 0-294,4 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,-2-2 0,0 1 0,-1-1 0,-2 0 0,0 0 0,-2 0 0,31-1 0,-3 0 176,-5 0 0,-3 1-176,-7 2 0,-2 0 0,-6 0 0,0 0 0,-5 0 0,0 0 0,0 0 0,0 0 0,-2 0 0,-2 0 284,0 0 1,0 0-285,0 0 0,1 0 8,1 0 1,1 0-9,14 0 0,3 0 0,-21 0 0,4 0 0,0 0-289,8 0 1,3 0-1,1 0 289,6 0 0,-1 0 0,0 0 0,-3 0 0,-1 0 0,-2 0 0,-7 0 0,-1 0 0,-3-1 0,26-1 0,-5 1 0,-5-2 0,-1 1 0,-2-1 0,1 1 0,3 0 0,0 0 0,1 0 0,2-1 0,1 1 0,0-1 0,2 1 0,1 0 0,0 0 0,-1 1 0,-1 1 0,0 0 0,-2 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-3 0 0,-2 0 0,-6 0 0,-3 0 0,-4 0 0,0 0 0,-4 0 0,1 0 0,-3 0 0,0 0 433,-2 0 0,-2 0-433,-5 0 0,-1 0 0,36 0 0,-11 0 0,0 0 0,4 0 0,13 0 0,-44-1 0,1-2 0,1 1 0,-1-1 0,4 0 0,-1-2 0,4-1 0,-1 1 0,6-2 0,3 0 0,18 0 0,5 0 0,6-1 0,3 2-267,-25 2 0,4 1 0,-1 1 267,3-1 0,1 0 0,0-1 0,-4-1 0,-1 0 0,-1 0 0,-2 1 0,-1 0 0,-2 0 0,21-3 0,-4-1 0,-10 2 0,-2-2 0,-4 1 0,1-1 0,12-2 0,4-1 0,10 2 0,2 0-247,-25 2 1,1 2 0,1 0 246,4-1 0,-1 1 0,-1 1 0,-5 0 0,-1 1 0,0 2 383,28-2 0,-4 0-383,-13 0 0,-1-1 0,-3 1 0,-1 1 0,-1-1 0,3 1 0,5 0 0,1 0 0,3 2 0,-2 0 0,-3 0 0,-4 0 0,-10 0 0,-4 0 0,33 0 769,-35 0-769,-27 0 5,-14 0-5,-9 0 0,-3 0 0,-4 0 0,-4 0 0,-2 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 270 24575,'46'-4'0,"33"1"0,-17 3 0,6 0 0,-1 0 0,5 0 0,3 0 0,6 0 0,2 0 0,1 0 0,5 0 0,1 0 0,3 0-708,-16 0 0,2 0 0,0 0 1,-2 0 707,19 0 0,-3 0 0,1 0 0,-19 0 0,2 0 0,-1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-3 0 0,15 0 0,-2 0 0,0 0 147,-3 1 0,-1-1 0,-3 1-147,23 1 0,-6 1 285,-18 1 0,-5 1-285,-11-1 0,-3 2 0,4 0 0,0-2 0,8-1 0,4-1 0,13 0 0,5 0 0,-26-2 0,1 0 0,-1 0 0,34 0 0,-3 0 0,-5 0 0,-1 0 0,-6 0 0,-2 0 0,-4 0 0,2 0 0,8 0 0,3 0 0,-27 0 0,1 0 0,1 0 294,3 0 0,3 0 0,-1 0-294,4 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,0 0 0,-2 0 0,1 0 0,0 0 0,-2-2 0,0 1 0,-1-1 0,-2 0 0,0 0 0,-2 1 0,31-2 0,-3 0 176,-5 0 0,-3 1-176,-7 2 0,-2 0 0,-6 0 0,-1 0 0,-4 0 0,0 0 0,0 0 0,0 0 0,-2 0 0,-2 0 284,0 0 1,0 0-285,0 0 0,1 0 8,1 0 1,1 0-9,14 0 0,3 0 0,-21 0 0,4 0 0,0 0-289,7 0 1,4 0-1,1 0 289,6 0 0,-1 0 0,0 0 0,-3 0 0,-1 0 0,-2 0 0,-7 0 0,-1 0 0,-3-1 0,26-1 0,-5 1 0,-5-2 0,-2 2 0,-1-2 0,1 1 0,3 0 0,0 0 0,1 0 0,2-1 0,1 1 0,0 0 0,2 0 0,1 0 0,0 0 0,-1 1 0,-1 1 0,-1 0 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,-3 0 0,-2 0 0,-6 0 0,-3 0 0,-4 0 0,0 0 0,-4 0 0,1 0 0,-3 0 0,0 0 433,-3 0 0,-1 0-433,-5 0 0,-1 0 0,36 0 0,-11 0 0,0 0 0,4 0 0,13 0 0,-44-1 0,1-2 0,1 1 0,-1-1 0,4 0 0,-1-1 0,4-2 0,-1 1 0,6-1 0,3-1 0,17 0 0,6 1 0,6-2 0,3 2-267,-25 3 0,4 0 0,-1 1 267,3-1 0,1 0 0,0-1 0,-4 0 0,-1-1 0,-1 0 0,-2 1 0,-1 0 0,-2 1 0,20-4 0,-3-1 0,-10 3 0,-2-3 0,-4 1 0,1 0 0,12-3 0,4 0 0,10 1 0,2 1-247,-25 1 1,1 2 0,1 1 246,4-2 0,-1 1 0,-2 1 0,-4 0 0,-1 2 0,0 1 383,28-2 0,-4 0-383,-13 0 0,-1-1 0,-3 1 0,-1 2 0,-1-2 0,3 1 0,5 0 0,1 0 0,3 2 0,-3 0 0,-2 0 0,-4 0 0,-10 0 0,-4 0 0,33 0 769,-35 0-769,-27 0 5,-14 0-5,-9 0 0,-3 0 0,-4 0 0,-4 0 0,-2 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15521,7 +15524,7 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 497 24575,'14'-3'0,"13"0"0,41 3 0,25 0 0,-22 0 0,6 0 0,5 0 0,3 0 0,5 0 0,2 0 0,-24 0 0,2 0 0,1 0-342,5 0 1,1 0 0,0 0 341,4 0 0,1 0 0,3 0 0,7 0 0,1 0 0,1 0 0,-1-1 0,-1 1 0,0 1 0,-4 0 0,1 0 0,0 2 0,4 0 0,1 1 0,1 1-381,-2 2 1,-1 2-1,3 0 381,-19-2 0,0 2 0,1-1 0,1 0 0,4 0 0,2 0 0,-1 0 0,1 0 0,0 1 0,2-1 0,-1 0 0,-1 0 0,-1-1 0,0 0 0,0-1 0,-1 1 0,-2-1 0,-1 0 0,1 1 0,-2 0 0,20 3 0,-2 0 0,2 1 0,-23-2 0,1 0 0,-1 1 0,2-1 0,3 2 0,1 0 0,-1 1 0,2 0 0,2 1 0,1 0 0,0-1 0,0 1 0,3 0 0,2 0 0,-1 0 0,-1-1 0,-4 0 0,1-1 0,-3 0 0,-1 0 0,17 2 0,-2-1 0,-2 0-201,-8-2 0,-2 0 1,-2-2 200,-7 2 0,-2-1 0,-1 1 0,-3-1 0,0 0 0,2 1 0,1-2 0,0 1 0,1-1 0,-1-1 0,0 1 0,-1 0 0,28-1 0,-2-1 0,-10-1 0,-4-2 0,-13 0 0,-3-1 347,-5-2 1,-1 0-348,10 0 0,1 0 0,10 0 0,4 0 0,-21 0 0,4 0 0,-1 0 243,8 0 0,1 0 1,1 0-244,2 0 0,-1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-7 0 0,-1 0 0,1 0 0,3-1 0,1 0 0,1-2 0,9-1 0,1-2 0,3-1-278,6-2 0,2-2 0,2 0 278,-19 1 0,1-2 0,0 1 0,-1-1 0,-4 1 0,1 0 0,-1 0 0,-3 1 0,17-3 0,-1 1 0,-2 1-155,-6 1 1,-2 1-1,-2 0 155,-7 0 0,-4 2 0,1-1 0,29-5 0,1-1 0,-29 4 0,-1 0 0,1-1 0,3-2 0,1-1 0,1-1 0,2 0 0,0 0 0,-1-1 0,-2 0 0,0 1 0,-4-2 0,23-6 0,-5 2 0,-11 5 0,-6 1 0,-11 2 0,-3 1 312,-6 2 1,-1 0-313,0 1 0,3 1 749,2-2 0,2-1-749,11-1 0,4 0 0,10-2 0,5-1 0,6-1 0,0-1 0,3 0 0,0-2 0,-5 0 0,-2-1 0,-6 2 0,-2-1 259,-4 1 0,-2 1-259,-6 2 0,-1 2 0,0 2 0,-3 1 0,0 2 0,-1 1 0,-3 2 0,-1 2 0,-1 0 0,-1 2 0,-4-1 0,0 2 0,1 0 0,0 0 0,5 0 0,2 0 0,1 0 0,-1 0 0,-1 0 0,-1 0 0,38 0 0,-22 0 0,-21 0 0,-12 0 0,-2 0 0,6 5 0,3 7 0,1 4 0,0 4 0,-1-3 0,6 1 0,5 3 0,0 1 0,-10 1 0,-11-4 0,-13-4 0,-7-4 0,-2-2 0,0-1 0,0 1 0,6 2 0,8 4 0,4-1 0,-3-4 0,-16-6 0,-25-4 0,-38 0 0,-35 0 0,31 0 0,-2-1 0,0-1 0,1-1 0,-36-7 0,13-3 0,-12-3 0,31 6 0,-4 0 0,-14-2 0,-3 1 0,-9-1 0,1 1 0,6 1 0,4 1 0,12 4 0,3 0 0,-22-2 0,25 0 0,6-2 0,-7-1 0,-12 0 0,-6 2 0,-10 4 0,-7-3 0,36 3 0,-3-1 0,-15-3 0,-2 1 0,-3-3 0,-1 0 0,1 0 0,1 0 0,8 1 0,1 0 0,-3 2 0,-4 1 0,-15 1 0,-3 2-245,22 0 0,-2 1 1,-2-1 244,-3 0 0,0 1 0,1-1 0,9 0 0,0-1 0,4-1 0,-21-2 0,3-2 0,-1 0 0,-3-1 0,19 3 0,-2 0 0,-5 1-549,-19 0 1,-6 3-1,-1-2 549,19 1 0,-3 1 0,-1-1 0,2 1 0,1 0 0,1 0 0,-1 0 0,4-1-100,-14-1 0,3 0 0,5-2 100,-11-2 0,9-2 331,24 3 0,6 0-331,-23-4 0,18 0 0,-10 3 1679,-24 2-1679,38 5 0,-4 1 169,-7 0 1,-3 0-170,-6 1 0,-1 0 0,-3 0 0,-1 0 0,-1 0 0,0 0 0,2 0 0,-1 0 0,7 1 0,0 2 0,4 2 0,1 2 0,2 3 0,1 2 0,0 0 0,-1 3 0,2 0 0,1 0 0,7-2 0,3 0 0,-39 6 0,24-2 0,14-3 0,7-1 0,0-1 0,-4-1 0,-9 1 0,-7 0 0,-4 2 0,-12 2 0,37-8 0,-2 1 0,-5 2 0,-2 0 0,-5-1 0,-2 2 0,-4 0 0,0 0 0,0 1 0,0-1 0,0 0 0,3-1 0,4-3 0,3 0 0,5 0 0,2-1 0,-44 1 0,4-4 0,-3-1 0,45-3 0,-1 0 0,-11 0 0,-1 0 0,-1 0 0,-1 0 0,0 0 0,1 0 0,1 0 0,2 0 0,8 0 0,1 0 0,2 0 0,1 0 0,-39 0 0,12 0 0,11-2 0,9-1 0,2 0 0,-4-3 0,-7 1 0,-7-2 0,-1 0 0,3 3 0,-3 0 0,-7 4 0,-7 0 0,-3 0 0,0-3 0,9 0 0,3-1 0,0 1 0,-8 3 0,36 0 0,-3 0 0,-5 0 0,-1 0 0,-3 0 0,-1 0 0,-1 0 0,-2 0 0,-2 0 0,-2 1 0,-11 3 0,-5 3 0,15 1 0,-3 3 0,-3 3-52,6 1 0,-4 2 1,0 1-1,8-3 1,-20 6-1,6 0 1,0 2-1,-2 0 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 483 24575,'14'-3'0,"13"0"0,41 3 0,25 0 0,-22 0 0,6 0 0,5 0 0,3 0 0,5 0 0,1 0 0,-23 0 0,2 0 0,1 0-342,5 0 1,1 0 0,0 0 341,4 0 0,1 0 0,3 0 0,7 0 0,1 0 0,1 0 0,-1-1 0,-2 1 0,1 1 0,-4 0 0,1 0 0,0 2 0,4 0 0,1 1 0,1 1-381,-2 2 1,-1 1-1,3 1 381,-19-2 0,0 2 0,1-2 0,0 1 0,5 0 0,2 0 0,-1-1 0,1 1 0,0 1 0,2-1 0,-1 0 0,-1-1 0,-1 0 0,0 0 0,0-1 0,-1 1 0,-2-2 0,-1 1 0,0 1 0,-1 0 0,20 3 0,-2-1 0,2 2 0,-23-2 0,1-1 0,-1 2 0,2-1 0,3 2 0,1-1 0,-1 2 0,2 0 0,2 0 0,1 1 0,-1-1 0,1 0 0,3 1 0,2-1 0,-1 1 0,-1-1 0,-4-1 0,1 0 0,-3 0 0,-1 0 0,17 1 0,-2 0 0,-2-1-201,-8-1 0,-3 0 1,-1-2 200,-7 1 0,-2 0 0,-1 1 0,-3-1 0,0-1 0,2 2 0,1-2 0,0 1 0,1-2 0,-1 0 0,0 1 0,-1 0 0,28-1 0,-2-2 0,-11 0 0,-3-2 0,-13 0 0,-3-1 347,-5-2 1,-1 0-348,10 0 0,1 0 0,10 0 0,4 0 0,-21 0 0,4 0 0,-1 0 243,8 0 0,1 0 1,1 0-244,2 0 0,-2 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-7 0 0,-1 0 0,1 0 0,3-1 0,1 0 0,1-2 0,9-1 0,1-2 0,3 0-278,6-3 0,1-2 0,3 1 278,-19 0 0,1-2 0,0 1 0,-1 0 0,-4 0 0,1 0 0,-1 1 0,-3 0 0,17-3 0,-1 2 0,-2 0-155,-6 1 1,-2 2-1,-3-1 155,-6 0 0,-4 2 0,1-1 0,29-4 0,1-2 0,-29 4 0,-1 1 0,1-2 0,3-2 0,1 0 0,1-2 0,2 1 0,0-1 0,-1 0 0,-2-1 0,-1 1 0,-3-1 0,23-6 0,-5 1 0,-11 6 0,-6 0 0,-11 2 0,-3 2 312,-6 1 1,-1 0-313,0 2 0,3 0 749,2-2 0,2-1-749,11 0 0,4-1 0,10-2 0,5 0 0,5-2 0,1 0 0,3-1 0,0-1 0,-5-1 0,-2 0 0,-6 1 0,-2 0 259,-4 0 0,-2 2-259,-6 1 0,-1 3 0,0 1 0,-3 1 0,0 2 0,-1 2 0,-4 1 0,0 2 0,-1 0 0,-1 2 0,-4-1 0,0 2 0,1 0 0,0 0 0,5 0 0,2 0 0,1 0 0,-1 0 0,-1 0 0,-1 0 0,38 0 0,-22 0 0,-21 0 0,-12 0 0,-2 0 0,6 5 0,3 7 0,0 3 0,1 5 0,-1-4 0,6 2 0,5 2 0,0 1 0,-10 2 0,-11-5 0,-13-3 0,-7-5 0,-2-1 0,0-1 0,0 1 0,6 1 0,8 5 0,4-1 0,-3-5 0,-16-5 0,-25-4 0,-38 0 0,-35 0 0,31 0 0,-2-1 0,0-1 0,1-1 0,-36-6 0,13-4 0,-12-3 0,32 7 0,-5-1 0,-14-2 0,-3 2 0,-9-2 0,1 1 0,6 2 0,4 0 0,12 4 0,3 0 0,-22-2 0,25 1 0,6-3 0,-7-1 0,-12 0 0,-6 3 0,-10 3 0,-6-3 0,35 3 0,-3-1 0,-15-3 0,-2 2 0,-3-4 0,-1 0 0,1 0 0,1 1 0,8 0 0,1 0 0,-3 2 0,-4 2 0,-15 0 0,-3 2-245,22 0 0,-1 1 1,-3-1 244,-3 0 0,0 1 0,1-1 0,9 0 0,0-1 0,4 0 0,-21-3 0,3-2 0,-1 0 0,-3 0 0,19 2 0,-2 0 0,-5 1-549,-19 0 1,-5 3-1,-2-2 549,19 2 0,-3 0 0,-1-1 0,2 1 0,1 0 0,1 0 0,-1 0 0,4-1-100,-14-1 0,3 1 0,5-3 100,-10-2 0,8-2 331,24 4 0,6-1-331,-23-4 0,18 0 0,-10 4 1679,-24 1-1679,38 5 0,-4 1 169,-7 0 1,-3 0-170,-6 1 0,-1 0 0,-3 0 0,-1 0 0,-1 0 0,1 0 0,1 0 0,-1 0 0,7 1 0,0 2 0,4 2 0,1 2 0,2 2 0,1 3 0,0 0 0,-1 2 0,2 1 0,1-1 0,7-1 0,3 0 0,-39 5 0,25-1 0,13-4 0,7 0 0,0-1 0,-4-2 0,-9 2 0,-7 0 0,-4 1 0,-12 3 0,37-9 0,-2 2 0,-5 2 0,-2 0 0,-5-2 0,-2 3 0,-4 0 0,0-1 0,0 2 0,0-1 0,0-1 0,4 0 0,3-3 0,3 0 0,5-1 0,2 0 0,-44 1 0,4-4 0,-3-1 0,45-3 0,-1 0 0,-11 0 0,-1 0 0,-1 0 0,-1 0 0,0 0 0,1 0 0,1 0 0,2 0 0,9 0 0,0 0 0,2 0 0,1 0 0,-39 0 0,12 0 0,11-2 0,9-1 0,2 0 0,-4-3 0,-7 1 0,-7-2 0,-1 1 0,3 2 0,-3 0 0,-7 4 0,-7 0 0,-3 0 0,1-3 0,8 0 0,3-1 0,0 1 0,-8 3 0,36 0 0,-3 0 0,-5 0 0,-1 0 0,-3 0 0,-1 0 0,-1 0 0,-2 0 0,-2 0 0,-2 1 0,-11 3 0,-5 3 0,16 1 0,-4 2 0,-3 4-52,6 0 0,-4 3 1,0 1-1,8-4 1,-20 7-1,6-1 1,0 2-1,-2 1 1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15575,8 +15578,8 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 24575,'27'3'0,"18"2"0,29 8 0,-21-1 0,4 4 0,10 5 0,1 3 0,2 2 0,0 0 0,-1 1 0,-1-1 0,-6-2 0,-2-1 0,-5-3 0,0-1 0,2-1 0,0-2 0,0-1 0,0-2 0,5-2 0,0-1 0,0 0 0,-1-2 0,-6-2 0,-3 0 0,36 3 0,-14-3 0,2 0 0,17-2 0,-37-2 0,1-1 0,4-1 0,0 1 0,-2 0 0,-1 1 0,-3 0 0,-1-1 0,-3 1 0,0 0 0,0 0 0,0-1 0,2-1 0,0 0 0,-2 0 0,-1 0 0,41 0 0,-16 0 0,-14-2 0,-2-4 0,7-4 0,11-3 0,3-2 0,-2 1 0,-10 2 0,-8 3 0,-6 3 0,-1 2 0,5 0 0,4-1 0,7 0 0,4-1 0,2 1 0,0 2 0,-5 1 0,-2-1 0,-6 0 0,-4 1 0,-4-3 0,-1 2 0,5 0 0,9 0 0,9 0 0,11-1 0,9 1 0,-45 2 0,0 0 0,0 1 0,1 0 0,46 0 0,-11 0 0,-10 0 0,-7 0 0,-8-3 0,-1 1 0,0-4 0,6 1 0,4 2 0,-1 0 0,-4 2 0,-5-1 0,0-3 0,-1 0 0,-1-1 0,-5 2 0,-7 0 0,1 2 0,5-1 0,10 1 0,12-4 0,5 0 0,1 2 0,-3 1 0,0 3 0,-3 0 0,0 0 0,-4 0 0,-7 0 0,-2 0 0,-1 0 0,-2 0 0,2 0 0,1 0 0,5 0 0,5 0 0,3 0 0,-1 0 0,-3 0 0,-4 0 0,-2 0 0,5 0 0,5 0 0,5 0 0,5 0 0,-4 0 0,-7 0 0,-8 0 0,-3-2 0,3-2 0,2-3 0,2-1 0,-4 2 0,-5 0 0,-3 2 0,4 1 0,13-2 0,13 1 0,-38 1 0,2-1 0,0 0 0,1 1 0,43-1 0,-11 1 0,-12 3 0,-8 0 0,0 0 0,-2 0 0,-5 0 0,-4 0 0,-7 0 0,-2 0 0,1 0 0,4 0 0,18 3 0,18 3 0,-25-1 0,5 2 0,17 0 0,5 1-244,-18-2 0,3 0 0,1 0 244,4 0 0,2 0 0,0-1 0,1 0 0,0 0 0,-1-1 0,-4-1 0,-1 1 0,-2-2 0,21 0 0,-5 0 0,-11 0 0,-5 1 0,-18-2 0,-5 1 0,32 2 0,-6-1 0,0-1 732,6 1-732,3 0 0,-8 1 0,-9 0 0,-10 1 0,-7 2 0,-3 0 0,4 2 0,4 1 0,5 1 0,5 0 0,9-2 0,12 0 0,10 1 0,-42-5 0,1 0 0,0 1 0,-2 0 0,-2-1 0,-3-1 0,39 1 0,-16-2 0,-10-3 0,-4 0 0,-5 0 0,-2 0 0,7 0 0,9 0 0,12 0 0,12 0 0,3 0 0,4 0 0,-5 0 0,-5 0 0,-8 0 0,-3 0 0,-5 0 0,-9 0 0,-5-2 0,-8 0 0,-4 0 0,-5-2 0,-6 2 0,-6-2 0,-3 1 0,-2-1 0,2-1 0,3-1 0,3 0 0,2-3 0,-2 1 0,-1-2 0,1-2 0,3 2 0,7-2 0,3-1 0,2 0 0,-2 0 0,-1 0 0,-2 3 0,1 0 0,3 0 0,1 3 0,2-1 0,-3 3 0,-5 0 0,-3 0 0,-3 3 0,3-1 0,0 1 0,0 0 0,-4-1 0,-5-1 0,-3 2 0,0 0 0,1 0 0,1 0 0,4 0 0,-6 0 0,0 0 0,-6 0 0,-5 0 0,0 0 0,-3 0 0,1 0 0,-1 0 0,-1 0 0,-2 1 0,-3 1 0,-1 0 0,0 0 0,0 0 0,-2 0 0,-11-6 0,-1-4 0,-8-5 0,3 1 0,-79 1 0,18 9 0,-12 2 0,7 0 0,10-1 0,0 1 0,-1 1 0,0 0 0,-1 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2448">16017 255 24575,'46'0'0,"4"0"0,14 0 0,0 0 0,-5 0 0,3 0 0,9 0 0,12 4 0,15 6 0,-45-4 0,1 1 0,2 1 0,0 0 0,1-1 0,-1 0 0,-1 0 0,-2-1 0,45 7 0,-16-1 0,-18-4 0,-13-1 0,-12-4 0,-2-1 0,2-1 0,13 1 0,8 0 0,10 4 0,2 1 0,-5-1 0,-4 0 0,-7-2 0,-4-1 0,-8-1 0,-8-2 0,-9 0 0,-7 0 0,-2 0 0,1 0 0,3 0 0,1 0 0,1 0 0,0 0 0,-3 0 0,-3 0 0,-3 0 0,-1-2 0,2-1 0,1-1 0,1 1 0,-3 2 0,-3 0 0,-3 1 0,-3 0 0,-2 0 0,-1 0 0,0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 24575,'27'3'0,"18"2"0,30 8 0,-22-1 0,4 4 0,11 5 0,0 3 0,2 2 0,1 0 0,-2 1 0,0-1 0,-7-3 0,-2 0 0,-4-3 0,-1-1 0,2-1 0,0-2 0,1-1 0,-1-2 0,5-2 0,1-1 0,-1 0 0,-1-2 0,-5-2 0,-4 0 0,36 3 0,-13-3 0,1 0 0,18-2 0,-38-2 0,1-1 0,5-1 0,-1 1 0,-2 0 0,0 1 0,-4 0 0,-1-1 0,-2 1 0,-1 0 0,0 0 0,0-1 0,3-1 0,-1 0 0,-2 0 0,-1 0 0,42 0 0,-17 0 0,-13-2 0,-3-4 0,7-4 0,12-3 0,2-2 0,-1 1 0,-11 2 0,-8 3 0,-5 3 0,-2 2 0,5 0 0,5-1 0,6 0 0,4-1 0,3 1 0,-1 2 0,-5 1 0,-1-1 0,-7 0 0,-4 1 0,-3-3 0,-2 2 0,5 0 0,10 0 0,8 0 0,12-1 0,8 1 0,-45 2 0,1 0 0,-1 1 0,1 0 0,47 0 0,-12 0 0,-9 0 0,-8 0 0,-8-3 0,0 1 0,-1-4 0,6 1 0,5 2 0,-2 0 0,-4 2 0,-4-1 0,-1-3 0,-1 0 0,0-1 0,-6 2 0,-7 0 0,2 2 0,4-1 0,10 1 0,13-4 0,4 1 0,1 1 0,-2 1 0,-1 3 0,-2 0 0,-1 0 0,-3 0 0,-8 0 0,-2 0 0,0 0 0,-3 0 0,2 0 0,2 0 0,4 0 0,5 0 0,4 0 0,-2 0 0,-3 0 0,-3 0 0,-3 0 0,6 0 0,4 0 0,5 0 0,6 0 0,-5 0 0,-6 0 0,-9 0 0,-3-2 0,4-2 0,1-3 0,2-1 0,-3 2 0,-6 0 0,-3 2 0,5 1 0,12-2 0,14 1 0,-39 1 0,2-1 0,0 0 0,2 1 0,42-1 0,-10 1 0,-13 3 0,-8 0 0,1 0 0,-3 0 0,-5 0 0,-3 0 0,-8 0 0,-2 0 0,2 0 0,3 0 0,18 3 0,19 3 0,-26-1 0,5 2 0,18 0 0,4 1-244,-17-2 0,2 0 0,1 0 244,5 0 0,1 0 0,1-1 0,0 0 0,1-1 0,-2 0 0,-4-1 0,0 1 0,-3-2 0,22 0 0,-6 0 0,-10 0 0,-6 1 0,-18-2 0,-4 1 0,31 2 0,-6-1 0,1-1 732,5 1-732,4 0 0,-9 1 0,-9 0 0,-9 1 0,-8 2 0,-3 0 0,5 2 0,3 1 0,5 1 0,6 0 0,8-2 0,12 0 0,11 1 0,-43-5 0,2 0 0,-1 1 0,-2 0 0,-2-1 0,-2-1 0,38 1 0,-15-2 0,-11-3 0,-4 0 0,-4 0 0,-3 0 0,7 0 0,9 0 0,13 0 0,11 0 0,4 0 0,3 0 0,-4 0 0,-6 0 0,-7 0 0,-4 0 0,-4 0 0,-10 0 0,-5-2 0,-7 0 0,-5 0 0,-5-2 0,-6 2 0,-6-2 0,-2 1 0,-3-1 0,2-1 0,3-1 0,3 0 0,2-3 0,-2 1 0,0-2 0,0-2 0,3 2 0,7-2 0,3-1 0,3 0 0,-3 0 0,-1 0 0,-2 3 0,2 0 0,2 1 0,1 2 0,2-1 0,-2 3 0,-6 0 0,-3 0 0,-3 3 0,3-1 0,1 1 0,-1 0 0,-4-1 0,-5-1 0,-3 2 0,1 0 0,0 0 0,1 0 0,4 0 0,-6 0 0,0 0 0,-6 0 0,-5 0 0,1 0 0,-4 0 0,1 0 0,-1 0 0,-1 0 0,-2 1 0,-3 1 0,-1 0 0,0 0 0,0 0 0,-2 0 0,-11-6 0,-1-4 0,-8-5 0,3 1 0,-80 1 0,19 9 0,-13 2 0,8 0 0,10-1 0,-1 1 0,0 1 0,-1 0 0,0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2448">16103 254 24575,'46'0'0,"5"0"0,13 0 0,0 0 0,-4 0 0,2 0 0,9 0 0,13 4 0,14 6 0,-44-4 0,0 1 0,2 1 0,1 0 0,0-1 0,-1 0 0,0 0 0,-3-1 0,45 7 0,-15-1 0,-19-4 0,-13-1 0,-11-4 0,-3-1 0,2-1 0,13 1 0,9 0 0,9 4 0,2 1 0,-4-1 0,-5 0 0,-7-2 0,-3-1 0,-9-1 0,-8-2 0,-9 0 0,-7 0 0,-2 0 0,2 0 0,2 0 0,1 0 0,1 0 0,0 0 0,-3 0 0,-3 0 0,-3 0 0,-1-2 0,3-1 0,0-1 0,1 1 0,-3 2 0,-3 0 0,-3 1 0,-3 0 0,-2 0 0,-1 0 0,0 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15603,8 +15606,8 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 6 24575,'37'-3'0,"34"1"0,-20 1 0,3 2 0,9-1 0,0 0 0,0 0 0,-2 0 0,-8 0 0,-2 0 0,-1-1 0,1 2 0,2 0 0,1 0 0,3 1 0,0 0 0,2 0 0,-1 0 0,-6 1 0,-2 0 0,37 4 0,-7 3 0,-1 4 0,9 1 0,8 0 0,-46-8 0,1-1 0,2 1 0,3-1 0,4 0 0,2 1 0,3 0 0,1 0 0,3 2 0,-2 0 0,-3 0 0,-3 1 0,-8-2 0,-3 0 0,37 8 0,-12-4 0,3 0 0,9-1 0,-37-5 0,1 0 0,1 0 0,0 0 0,1 1 0,1-1 0,-1-1 0,0 0 0,44 1 0,-47-4 0,0-1 0,46-1 0,-5 0 0,-2 0 0,-3 0 0,4 0 0,4 0 0,-43 0 0,1 0 0,0 0 0,1 0 0,-2 0 0,-1 0 0,46 0 0,-14 0 0,-3 0 0,0 0 0,5 0 0,-34 0 0,1 0 0,5-1 0,2 1 0,6-1 0,2-2 0,2 0 0,0-1 0,-2 0 0,-1 0 0,-3 0 0,-2 1 0,-6 1 0,-1 0 0,-3 2 0,1 0 0,1 0 0,1 0 0,3 0 0,1 0 0,7 0 0,2 0 0,2 0 0,0 0 0,0 0 0,0 0 0,-2 0 0,0 0 0,-4 0 0,-1 0 0,1 0 0,0 0 0,-3 0 0,1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-2 0 0,0 0 0,2 0 0,1 0 0,-3 0 0,0 0 0,-1 0 0,-1 0 0,-3 0 0,-1 0 0,35 0 0,-21 0 0,-24 0 0,-25 0 0,-19 0 0,-14-1 0,-10-1 0,-4 0 0,0 0 0,2 1 0,1 1 0,4 0 0,5-3 0,6-1 0,6-2 0,3 2 0,6 13 0,0-3 0,1 9 0,-4-9 0,1 0 0,-1-2 0,0-2 0,-6-4 0,1-3 0,-3 2 0,5 0 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2018">7465 244 24575,'28'0'0,"31"0"0,40 0 0,-36 0 0,3 0 0,5-1 0,3 2 0,7-1 0,2 1 0,3 2 0,2 2 0,6 3 0,1 3 0,1 1 0,0 3 0,-6 1 0,-1 1 0,-3-1 0,-1 0 0,-1 0 0,-1 0 0,-1 0 0,0 0 0,1 1 0,1-1 0,1-2 0,-1 1 0,-3-1 0,-2-1 0,-3-2 0,-2 0 0,-8-1 0,-1-2 0,-5 0 0,0-1 0,-1-2 0,0 0 0,2-2 0,1 1 0,3-2 0,0-1 0,1 1 0,0-1 0,-2-1 0,0 0 0,1 0 0,2 0 0,1 0 0,2 0 0,5-2 0,2 0 0,7-1 0,1-1 0,5-2 0,1-1 0,1-2 0,2-1 0,-28 3 0,1-1 0,1 1-212,4-1 0,1 0 0,1 0 212,1 1 0,1-1 0,0 1 0,3 0 0,0 1 0,0 0 0,-2 1 0,1-1 0,-2 1 0,-2 1 0,0 0 0,0 1 0,3 0 0,0 1 0,0 0 0,3 0 0,-1 1 0,0 0 0,-2 1 0,-1 0 0,1 0 0,0 0 0,1 0 0,-2 0 0,-4 0 0,-1 0 0,0 0 0,-3 0 0,0 0 0,-2 0 0,28 0 0,-3 0 0,-11 0 0,-2 0 0,-6 0 0,-2 0 0,-6 0 0,-2 0 0,0 0 0,0 0 0,-3-1 0,-1 0 318,-2 0 0,0-1-318,-3 1 0,-1-1 0,45-4 0,-10-1 0,-10-2 0,-3-5 0,1-1 0,10-7 0,11-4 0,-47 12 0,-1 0 0,2-2 0,-1 1 0,40-14 0,-10 4 0,-10 2 0,-7 2 0,-1 0 0,0-2 0,1 0 0,-7 4 0,-6 4 0,-7 4 0,-1 4 0,-2 2 0,-7 1 0,-6 3 0,-8 0 0,-6 1 0,-3 0 0,-2 0 0,-1 0 0,1 0 0,2 0 0,4 0 0,11 0 0,19 5 0,11 5 0,4 3 0,-12-1 0,-19-3 0,-12-3 0,-10-3 0,-3-2 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 6 24575,'37'-3'0,"35"1"0,-21 1 0,3 2 0,10-1 0,-1 0 0,0 0 0,-1 0 0,-9 0 0,-2 0 0,-1-1 0,2 2 0,1 0 0,1 0 0,4 1 0,-1 0 0,2 0 0,0 0 0,-7 1 0,-2 0 0,38 4 0,-8 3 0,0 4 0,8 1 0,9 0 0,-47-8 0,1-1 0,3 1 0,2-1 0,4 0 0,3 1 0,2 0 0,1 0 0,4 2 0,-3-1 0,-3 1 0,-2 1 0,-9-2 0,-3 0 0,38 8 0,-13-4 0,4 0 0,8-1 0,-36-5 0,0 0 0,1 0 0,0 0 0,2 1 0,0-1 0,-1-1 0,1 0 0,43 1 0,-47-4 0,1-1 0,45-1 0,-4 0 0,-3 0 0,-2 0 0,3 0 0,5 0 0,-44 0 0,1 0 0,1 0 0,0 0 0,-2 0 0,0 0 0,45 0 0,-13 0 0,-4 0 0,0 0 0,6 0 0,-35 0 0,2 0 0,4-1 0,2 1 0,7-1 0,1-2 0,2 0 0,1-1 0,-3 0 0,-1 0 0,-2 0 0,-3 1 0,-6 1 0,0 0 0,-4 2 0,1 0 0,2 0 0,0 0 0,3 0 0,2 0 0,6 0 0,2 0 0,3 0 0,-1 0 0,0 0 0,1 0 0,-3 0 0,1 0 0,-5 0 0,-1 0 0,2 0 0,-1 0 0,-3 0 0,2 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-2 0 0,1 0 0,1 0 0,1 0 0,-2 0 0,-1 0 0,-1 0 0,0 0 0,-4 0 0,-1 0 0,36 0 0,-22 0 0,-24 0 0,-24 0 0,-20 0 0,-15-1 0,-9-1 0,-4 0 0,0 0 0,2 1 0,1 1 0,4 0 0,4-3 0,7-1 0,6-2 0,3 2 0,6 13 0,0-3 0,1 9 0,-4-9 0,1 0 0,-1-2 0,0-2 0,-6-4 0,1-3 0,-3 2 0,5 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2018">7507 243 24575,'28'0'0,"32"0"0,39 0 0,-35 0 0,2 0 0,5-1 0,4 2 0,6-1 0,3 1 0,2 2 0,3 2 0,5 3 0,2 3 0,0 1 0,1 3 0,-7 1 0,0 1 0,-4-1 0,0 0 0,-2 0 0,0 0 0,-2 0 0,1 0 0,0 1 0,2-2 0,0-1 0,0 1 0,-4-1 0,-1-1 0,-4-2 0,-2 0 0,-7-1 0,-2-2 0,-4 0 0,-1-1 0,-1-2 0,1 0 0,1-2 0,1 1 0,4-2 0,-1-1 0,1 1 0,1-1 0,-3-1 0,0 0 0,2 0 0,1 0 0,2 0 0,1 0 0,5-2 0,3 0 0,6-1 0,2-1 0,4-2 0,2-1 0,0-2 0,3-1 0,-29 3 0,2-1 0,0 1-212,4-1 0,2 0 0,0 0 212,2 1 0,0-1 0,1 1 0,2 0 0,0 1 0,1 0 0,-3 1 0,2-1 0,-3 1 0,-1 2 0,-1-1 0,0 1 0,4 0 0,-1 1 0,1 0 0,2 0 0,0 1 0,-1 0 0,-1 1 0,-2 0 0,1 0 0,1 0 0,0 0 0,-1 0 0,-5 0 0,0 0 0,-1 0 0,-3 0 0,1 0 0,-3 0 0,29 0 0,-4 0 0,-10 0 0,-3 0 0,-6 0 0,-1 0 0,-7 0 0,-1 0 0,-1 0 0,0 0 0,-2-1 0,-2 0 318,-2 0 0,1-1-318,-4 1 0,-1-1 0,46-4 0,-11-1 0,-9-2 0,-4-5 0,2-1 0,9-7 0,12-4 0,-48 12 0,-1 0 0,2-2 0,0 1 0,39-14 0,-9 4 0,-11 2 0,-7 2 0,0 1 0,-1-3 0,1 0 0,-6 4 0,-7 4 0,-7 4 0,-1 4 0,-1 2 0,-8 1 0,-6 3 0,-8 0 0,-6 1 0,-3 0 0,-2 0 0,-1 0 0,1 0 0,2 0 0,4 0 0,12 0 0,18 5 0,11 5 0,4 3 0,-11-1 0,-20-3 0,-12-3 0,-10-3 0,-3-2 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15631,7 +15634,7 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 334 24575,'23'0'0,"8"0"0,11 0 0,13 0 0,13 0 0,17 0 0,14 0 0,-48 1 0,-1 1 0,49 4 0,-9 5 0,-9 2 0,0 0 0,4 0 0,7 2 0,-41-8 0,0 0 0,1 0 0,1 1 0,0 0 0,-1 0 0,3-1 0,0 0 0,3 0 0,1 0 0,2-1 0,2-2 0,1-1 0,2-1 0,2 0 0,1 0 0,2 0 0,2 0 0,16 0 0,3 0 0,4 0 0,2 0-151,-29-1 1,1 0 0,0 0 150,0 0 0,1-2 0,-2 1 0,25 0 0,-2 0 0,0 0 0,-2 0 0,-8 0 0,-2 0 0,-3 0 0,-2 0 0,-2 0 0,-2 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,-2 0 0,0 0 225,-1 0 1,1 0-226,-1 0 0,1 0 0,2-2 0,2 0 0,5-2 0,1 0 0,3-1 0,-1 0 0,-1-1 0,-1 0 0,-4 1 0,0 0 0,-6 1 0,-1 0 0,-2 0 0,1 0 0,2 1 0,0-1 0,3 0 0,0 0 0,3-1 0,0-1 0,2 0 0,0 0 0,-2-2 0,-1 0 0,-4 1 0,-2-1 0,-2 0 0,-1 0 0,1 0 0,1 0 0,7-2 0,2-1 0,8-1 0,1-1 0,7-2 0,1 0 0,1-2 0,0 0 0,0 0 0,-1 0 0,-2 0 0,-2 0 0,-5 3 0,-3 0 0,-5 1 0,-1 2 0,-5 1 0,-1 1 0,-4 1 0,0 0 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 2 0,-1 0 0,-2 0 0,0 0 0,-2 1 0,-1 0 0,-5 0 0,-1 0 0,45-3 0,-3 4 0,-45 2 0,0 2 0,1-1 0,1 2 0,1-1 0,0 0 0,0 0 0,0 0 0,-2 0 0,2 0 0,5 0 0,2 0 0,5 0 0,2 0 0,3 0 0,0 0 0,3 0 0,-1 0 0,-5 0 0,0 0 0,-5 0 0,-2 0 0,-4 0 0,-2 0 0,46 0 0,-12 0 0,-13 2 0,-11 3 0,-9 3 0,-2 3 0,5-1 0,10 1 0,8 0 0,4 0 0,3 0 0,-2 1 0,4 0 0,3 3 0,6 0 0,-44-7 0,1 0 0,1 0 0,0 0 0,1-2 0,0-1 0,0 0 0,0-1 0,0 0 0,0-1 0,0-1 0,0 0 0,-1-1 0,0 0 0,47-1 0,-4 2 0,-4 1 0,7 1 0,-43-3 0,0 1 0,5-2 0,0 1 0,2 0 0,0 1 0,-2-1 0,-2 1 0,-2 1 0,-1 1 0,-2-1 0,0 0 0,3-1 0,1 1 0,5 0 0,2 0 0,7 0 0,3 0 0,4 0 0,1 1 0,-1 1 0,-2 0 0,-4-1 0,-3 0 0,-9-1 0,-3 0 0,-5-1 0,-1 0 0,44-2 0,-4 2 0,3 2 0,-42-2 0,1-1 0,2 1 0,0-1 0,4-1 0,0 0 0,1 2 0,0-1 0,-1 1 0,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,-2-1 0,-1 0 0,-4 0 0,-1 0 0,44 0 0,-5 0 0,0 0 0,0 0 0,4 0 0,-3 0 0,-5 0 0,-11 0 0,-15 0 0,-11 2 0,-7 0 0,-1 2 0,1 2 0,0 0 0,1 0 0,-1 0 0,-1-1 0,1-1 0,0 1 0,3-3 0,-2 2 0,2-2 0,-3 1 0,-7-1 0,-3 0 0,-3 0 0,0-1 0,2-1 0,-2 0 0,-3 0 0,-13 0 0,-5 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 333 24575,'23'0'0,"8"0"0,12 0 0,12 0 0,13 0 0,18 0 0,13 0 0,-47 1 0,-2 1 0,49 4 0,-8 5 0,-10 2 0,1 0 0,3-1 0,8 3 0,-42-8 0,0 0 0,2 0 0,0 1 0,0 0 0,0 0 0,2-1 0,0 0 0,4 0 0,0 0 0,2-1 0,3-2 0,0-1 0,2-1 0,3 0 0,0 0 0,2 0 0,3 0 0,15 0 0,4 0 0,3 0 0,3 0-151,-30-1 1,2 0 0,-1 0 150,1 0 0,0-2 0,-2 1 0,26 0 0,-3 0 0,1 0 0,-3 0 0,-7 0 0,-3 0 0,-2 0 0,-3 0 0,-1 0 0,-3 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-3 0 0,0 0 225,0 0 1,0 0-226,0 0 0,0 0 0,2-2 0,3 0 0,4-2 0,2 0 0,2-1 0,0 0 0,-2-1 0,0 0 0,-5 1 0,0 0 0,-5 1 0,-2 0 0,-1 0 0,0 0 0,2 1 0,1-1 0,2 0 0,0 0 0,4-1 0,-1-1 0,3 0 0,-1 0 0,-1-2 0,-2 0 0,-4 1 0,-1 0 0,-3-1 0,0 0 0,0 0 0,1 0 0,8-2 0,1-1 0,9-1 0,0-1 0,8-2 0,0 0 0,2-2 0,-1 0 0,1 0 0,-2 0 0,-1 0 0,-3 0 0,-4 3 0,-4 0 0,-4 1 0,-2 3 0,-5 0 0,0 1 0,-5 1 0,1 0 0,-1 1 0,-1-1 0,2 1 0,-2-1 0,1 2 0,0 0 0,-3 0 0,1 0 0,-3 1 0,-1 0 0,-5 0 0,0 0 0,44-3 0,-2 4 0,-46 2 0,0 2 0,2-1 0,0 2 0,1-1 0,1 0 0,-1 0 0,0 0 0,-1 0 0,1 0 0,5 0 0,2 0 0,6 0 0,1 0 0,4 0 0,-1 0 0,3 0 0,0 0 0,-6 0 0,1 0 0,-6 0 0,-2 0 0,-3 0 0,-3 0 0,46 0 0,-11 0 0,-14 2 0,-10 3 0,-10 3 0,-2 3 0,6-1 0,9 1 0,9 0 0,3 0 0,3 0 0,-1 1 0,3 0 0,4 3 0,5-1 0,-43-6 0,0 0 0,1 0 0,1 0 0,0-2 0,0-1 0,0 0 0,1-1 0,-1 0 0,0-1 0,1-1 0,-1 0 0,-1-1 0,1 0 0,46-1 0,-3 2 0,-5 1 0,8 1 0,-44-3 0,0 1 0,6-2 0,-1 1 0,2 0 0,1 1 0,-3-1 0,-2 1 0,-1 1 0,-2 1 0,-2-1 0,1 0 0,2-1 0,1 1 0,6 0 0,1 0 0,7 0 0,4 0 0,3 0 0,2 1 0,-2 1 0,-1 0 0,-5-1 0,-3 0 0,-8-1 0,-4 0 0,-5-1 0,0 0 0,43-2 0,-3 2 0,2 2 0,-42-2 0,2-1 0,1 1 0,0-1 0,5-1 0,-1 0 0,1 2 0,1-1 0,-2 1 0,0 0 0,1 0 0,0-1 0,-1 1 0,1-1 0,-3-1 0,-1 0 0,-3 0 0,-2 0 0,44 0 0,-4 0 0,-1 0 0,1 0 0,4 0 0,-4 0 0,-4 0 0,-12 0 0,-15 0 0,-10 2 0,-8 0 0,-1 2 0,1 2 0,1 0 0,0 0 0,-1 0 0,-1-1 0,1-1 0,1 1 0,2-3 0,-2 2 0,2-2 0,-2 1 0,-8-1 0,-3 0 0,-3 0 0,0-1 0,3-1 0,-3 0 0,-3 0 0,-13 0 0,-5 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -15825,7 +15828,7 @@
       <inkml:brushProperty name="height" value="0.1" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 168 24575,'20'0'0,"8"0"0,11 0 0,17 0 0,22 0 0,-29 0 0,3 0 0,14 0 0,3 0 0,13 0 0,3 0 0,8 0 0,2 0 0,3 0 0,-1 0 0,-4 0 0,-2 0 0,-7 0 0,-5 0 0,-6 0 0,-2 0 0,-4 0 0,-2 0 0,-3 0 0,0 0 0,3 0 0,1 0 0,5 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-5 0 0,-1 0 0,-6-2 0,-1 0 0,1-1 0,-2-1 0,-2 0 0,0 0 0,2 0 0,-1 0 0,1 0 0,0 1 0,1 0 0,0 0 0,3-1 0,2 0 0,5 0 0,0 2 0,4-1 0,2 1 0,3 2 0,2-1 0,3-1 0,0 0 0,-2-1 0,0 0 0,-1 0 0,-1 0 0,-2 1 0,1 0 0,-2 2 0,-1 0 0,4 0 0,0 0 0,5 0 0,-2 0 0,-1 0 0,-1 0 0,-1 0 0,0 0 0,-4 0 0,-1 0 0,-6-2 0,1 0 0,1 0 0,1-1 0,3 1 0,2-1 0,5 1 0,1 0 0,8 3 0,2-2 0,4 0 0,0-2 0,3 0 0,2 0 0,-31 1 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,2 0 0,1 1 0,0-1-144,0 0 1,1 1-1,-1-1 144,-1 0 0,1 0 0,0 0 0,0 1 0,-1 0 0,0 0 0,27 1 0,1 0 0,-3 0 0,0 0 0,-4 0 0,1 0 0,-8 0 0,-1 0 0,-4 0 0,1 0 0,-6 0 0,0 0 0,-1 0 0,1 0 0,1 0 0,1 0 0,-2 0 0,0 0 0,-3 0 0,-2 0 215,-4 0 1,-2 0-216,-7 0 0,-1 0 0,-3 0 0,-3 0 0,39 0 0,-9 0 0,2 0 0,4 4 0,-35-1 0,2 2 0,2-1 0,2 1 0,6 1 0,0 0 0,3 1 0,-1-1 0,0-1 0,-1 0 0,1 0 0,-2-1 0,-7-1 0,-3 0 0,41 1 0,-11 3 0,-7 0 0,0 1 0,0 2 0,11-2 0,7-2 0,-41-4 0,1 0 0,3-2 0,-1 0 0,2-1 0,-1 2 0,3-1 0,1 0 0,-1 0 0,2 0 0,5 0 0,1 0 0,6 0 0,1 0 0,4 0 0,2 0 0,4-2 0,1-1 0,-3 0 0,0-1 0,-4-2 0,-1 0 0,-7 0 0,0-1 0,-5 0 0,0 1 0,-2-1 0,1 1 0,-4 0 0,2 0 0,-2 0 0,0 0 0,-5 2 0,-2 1 0,45-5 0,-7 2 0,-1 2 0,6 1 0,1 3 0,-4 0 0,-7 0 0,-8 0 0,7 0 0,2 0 0,6 0 0,-42 0 0,2 0 0,-3 0 0,-1 0 0,45 0 0,-18 0 0,-16 0 0,-9 0 0,-4 0 0,-8 0 0,-4 0 0,-8 0 0,-4 0 0,7 0 0,4 0 0,13 0 0,14-3 0,11-2 0,8-2 0,-2-1 0,-13 2 0,-15 0 0,-13 3 0,-12 2 0,-3 1 0,-3 0 0,-5 0 0,-6 0 0,-3 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 168 24575,'20'0'0,"8"0"0,11 0 0,17 0 0,22 0 0,-29 0 0,3 0 0,14 0 0,3 0 0,13 0 0,2 0 0,9 0 0,2 0 0,3 0 0,-1 0 0,-4 0 0,-2 0 0,-7 0 0,-5 0 0,-6 0 0,-2 0 0,-4 0 0,-2 0 0,-3 0 0,-1 0 0,4 0 0,1 0 0,5 0 0,0 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,-5 0 0,-1 0 0,-6-2 0,-1 0 0,1-1 0,-2-1 0,-2 0 0,0 0 0,2 0 0,-2 0 0,2 0 0,0 1 0,1 0 0,0 0 0,3-1 0,2 0 0,5 0 0,0 2 0,4-1 0,2 1 0,3 2 0,2-1 0,3-1 0,0 0 0,-2-1 0,-1 0 0,0 0 0,-1 0 0,-2 1 0,1 0 0,-2 2 0,-1 0 0,4 0 0,0 0 0,5 0 0,-2 0 0,-1 0 0,-1 0 0,-1 0 0,0 0 0,-5 0 0,0 0 0,-6-2 0,1 0 0,1 0 0,1-1 0,3 1 0,2-1 0,5 1 0,1 0 0,8 3 0,2-2 0,4 0 0,0-2 0,2 0 0,3 0 0,-31 1 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,2 0 0,1 1 0,0-1-144,0 0 1,1 1-1,-1-1 144,-1 0 0,1 0 0,-1 0 0,1 1 0,-1 0 0,0 0 0,27 1 0,1 0 0,-3 0 0,0 0 0,-4 0 0,1 0 0,-8 0 0,-1 0 0,-4 0 0,0 0 0,-5 0 0,0 0 0,-1 0 0,1 0 0,1 0 0,1 0 0,-2 0 0,0 0 0,-3 0 0,-2 0 215,-4 0 1,-2 0-216,-7 0 0,-1 0 0,-3 0 0,-3 0 0,38 0 0,-8 0 0,2 0 0,4 4 0,-35-1 0,2 2 0,2-1 0,2 1 0,6 1 0,0 0 0,3 1 0,-1-1 0,0-1 0,-1 0 0,1 0 0,-2-1 0,-7-1 0,-3 0 0,40 1 0,-10 3 0,-7 0 0,0 1 0,0 2 0,11-2 0,7-2 0,-41-4 0,1 0 0,3-2 0,-1 0 0,2-1 0,-1 2 0,3-1 0,1 0 0,-1 0 0,2 0 0,4 0 0,2 0 0,6 0 0,1 0 0,4 0 0,2 0 0,4-2 0,1-1 0,-3 0 0,0-1 0,-4-2 0,-1 0 0,-7 0 0,0-1 0,-5 0 0,-1 1 0,-1-1 0,1 1 0,-4 0 0,2 0 0,-2 0 0,0 0 0,-5 2 0,-2 1 0,45-5 0,-7 2 0,-1 2 0,6 1 0,1 3 0,-4 0 0,-8 0 0,-7 0 0,7 0 0,2 0 0,6 0 0,-42 0 0,2 0 0,-3 0 0,-1 0 0,45 0 0,-18 0 0,-16 0 0,-9 0 0,-4 0 0,-8 0 0,-4 0 0,-8 0 0,-4 0 0,7 0 0,4 0 0,12 0 0,15-3 0,11-2 0,8-2 0,-2-1 0,-13 2 0,-15 0 0,-13 3 0,-12 2 0,-3 1 0,-3 0 0,-5 0 0,-6 0 0,-3 0 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -16148,7 +16151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC93BE0-3612-4B4B-91A6-E5F017AEE7A8}">
   <dimension ref="A1:Q132"/>
   <sheetViews>
-    <sheetView topLeftCell="J55" zoomScale="244" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="J59" zoomScale="244" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
@@ -16687,10 +16690,10 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="23"/>
+      <c r="B14" s="22"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -16708,10 +16711,10 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="6" t="s">
         <v>4</v>
       </c>
@@ -16739,8 +16742,8 @@
       <c r="Q15" s="6"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
         <v>22</v>
@@ -16782,8 +16785,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
         <v>24</v>
@@ -16825,8 +16828,8 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
         <v>23</v>
@@ -16868,8 +16871,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
         <v>26</v>
@@ -16911,8 +16914,8 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
         <v>27</v>
@@ -16954,8 +16957,8 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
@@ -16999,8 +17002,8 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
         <v>24</v>
@@ -17042,8 +17045,8 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
         <v>23</v>
@@ -17085,8 +17088,8 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
         <v>25</v>
@@ -17128,8 +17131,8 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
         <v>26</v>
@@ -17171,8 +17174,8 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
         <v>27</v>
@@ -17214,8 +17217,8 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
         <v>27</v>
@@ -17257,8 +17260,8 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
         <v>28</v>
@@ -17300,8 +17303,8 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="20"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
         <v>28</v>
@@ -17343,8 +17346,8 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
         <v>22</v>
@@ -17413,12 +17416,12 @@
       <c r="Q32" s="1"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="7" t="s">
         <v>6</v>
       </c>
@@ -17440,10 +17443,10 @@
       <c r="Q33" s="6"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
         <v>52</v>
@@ -17481,10 +17484,10 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
         <v>31</v>
@@ -18072,12 +18075,12 @@
       <c r="Q52" s="1"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53" s="22" t="s">
+      <c r="A53" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
       <c r="E53" s="6" t="s">
         <v>6</v>
       </c>
@@ -18165,103 +18168,103 @@
       <c r="A58" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C58" s="22"/>
-      <c r="D58" s="22"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
       <c r="E58" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F58" s="22" t="s">
+      <c r="F58" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="G58" s="22"/>
+      <c r="G58" s="20"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
       <c r="E59" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F59" s="20" t="s">
+      <c r="F59" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="G59" s="20"/>
+      <c r="G59" s="21"/>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
       <c r="E60" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F60" s="20" t="s">
+      <c r="F60" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="G60" s="20"/>
+      <c r="G60" s="21"/>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
       <c r="E61" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F61" s="20" t="s">
+      <c r="F61" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="G61" s="20"/>
+      <c r="G61" s="21"/>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
       <c r="E62" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F62" s="20" t="s">
+      <c r="F62" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="20"/>
+      <c r="G62" s="21"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
       <c r="E63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F63" s="20" t="s">
+      <c r="F63" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="20"/>
+      <c r="G63" s="21"/>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -18296,11 +18299,11 @@
       <c r="A67" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B67" s="21" t="s">
+      <c r="B67" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
       <c r="E67" s="8" t="s">
         <v>101</v>
       </c>
@@ -18311,11 +18314,11 @@
       <c r="A68" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
       <c r="E68" s="1" t="s">
         <v>120</v>
       </c>
@@ -18326,11 +18329,11 @@
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
       <c r="E69" s="1" t="s">
         <v>121</v>
       </c>
@@ -18339,11 +18342,11 @@
       <c r="A70" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
       <c r="E70" s="1" t="s">
         <v>122</v>
       </c>
@@ -18352,11 +18355,11 @@
       <c r="A71" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
       <c r="E71" s="1" t="s">
         <v>123</v>
       </c>
@@ -18365,11 +18368,11 @@
       <c r="A72" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
       <c r="E72" s="1" t="s">
         <v>128</v>
       </c>
@@ -19046,13 +19049,24 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:D61"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A34:D34"/>
@@ -19067,24 +19081,13 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -19096,7 +19099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F6BEDF-58A8-7846-8BA3-49A7BA2DADCE}">
   <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="125" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -19760,7 +19763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78A8CBD-BA59-4F45-BAA1-C7A4B1A0FDDA}">
   <dimension ref="A2:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T34" zoomScale="188" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B93" zoomScale="132" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -19770,7 +19773,7 @@
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>223</v>
       </c>
@@ -19781,7 +19784,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>225</v>
       </c>
@@ -19789,7 +19792,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>226</v>
       </c>
@@ -19797,7 +19800,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>229</v>
       </c>
@@ -19805,7 +19808,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>231</v>
       </c>
@@ -19813,7 +19816,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>233</v>
       </c>
@@ -19821,7 +19824,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>235</v>
       </c>
@@ -19829,7 +19832,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>237</v>
       </c>
@@ -19837,7 +19840,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>239</v>
       </c>
@@ -19848,7 +19851,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>243</v>
       </c>
@@ -19856,7 +19859,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>245</v>
       </c>
@@ -19864,7 +19867,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>247</v>
       </c>
@@ -19872,15 +19875,18 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>249</v>
       </c>
       <c r="B14" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>251</v>
       </c>
@@ -19888,7 +19894,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>253</v>
       </c>
@@ -20027,10 +20033,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC27F950-0B8E-6F4A-BC17-1410D0AF1938}">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AF8"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView topLeftCell="M1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11:AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20238,6 +20244,9 @@
       <c r="U3">
         <v>0</v>
       </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
       <c r="W3">
         <v>2</v>
       </c>
@@ -20373,6 +20382,120 @@
       </c>
       <c r="AF5">
         <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>2</v>
+      </c>
+      <c r="AB6">
+        <v>3</v>
+      </c>
+      <c r="AC6">
+        <v>4</v>
+      </c>
+      <c r="AD6">
+        <v>5</v>
+      </c>
+      <c r="AE6">
+        <v>6</v>
+      </c>
+      <c r="AF6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>4</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>6</v>
+      </c>
+      <c r="V7">
+        <v>7</v>
+      </c>
+      <c r="W7">
+        <v>8</v>
+      </c>
+      <c r="X7">
+        <v>9</v>
+      </c>
+      <c r="Y7">
+        <v>10</v>
+      </c>
+      <c r="Z7">
+        <v>11</v>
+      </c>
+      <c r="AA7">
+        <v>12</v>
+      </c>
+      <c r="AB7">
+        <v>13</v>
+      </c>
+      <c r="AC7">
+        <v>14</v>
+      </c>
+      <c r="AD7">
+        <v>15</v>
+      </c>
+      <c r="AE7">
+        <v>16</v>
+      </c>
+      <c r="AF7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>2</v>
+      </c>
+      <c r="Z8">
+        <v>3</v>
+      </c>
+      <c r="AA8">
+        <v>4</v>
+      </c>
+      <c r="AB8">
+        <v>5</v>
+      </c>
+      <c r="AC8">
+        <v>6</v>
+      </c>
+      <c r="AD8">
+        <v>7</v>
+      </c>
+      <c r="AE8">
+        <v>8</v>
+      </c>
+      <c r="AF8">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>